<commit_message>
TileControl() Work on distributing human and/or computer tiles, for continuing game logic.
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{122E6D40-3E98-0649-8E79-5508E1D45B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208F8467-40E7-4647-BC52-083A1D37C039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27360" yWindow="-2180" windowWidth="26040" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -415,7 +415,7 @@
     <xf numFmtId="20" fontId="12" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
@@ -423,6 +423,18 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -441,18 +453,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -2923,26 +2923,26 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" ht="38" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="16" t="str">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="10" t="str">
         <f ca="1">'Target '!A2-'Target '!A1&amp;" days remaining"</f>
         <v>-16 days remaining</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="12"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" s="2" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
@@ -3029,24 +3029,24 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="31" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="23" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="23" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A1" s="17">
+      <c r="A1" s="11">
         <v>45373</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2" s="19">
+      <c r="A2" s="13">
         <f ca="1">TODAY()</f>
         <v>45357</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B3" s="17"/>
+      <c r="B3" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3074,15 +3074,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3382,6 +3373,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
   <ds:schemaRefs>
@@ -3395,14 +3395,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1101C2D-3F57-4FE3-804B-005C212162D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3423,6 +3415,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
printNumberInTileBag() Improve this print helper method, to show how many tiles remaining in back if/when human, computer tiles taken out. Still work in progress.
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208F8467-40E7-4647-BC52-083A1D37C039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923F5279-46F8-AF41-B720-D5BC1AC53139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27360" yWindow="-2180" windowWidth="26040" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27340" yWindow="-2180" windowWidth="26040" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dev Log" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>DATE</t>
   </si>
@@ -68,6 +68,16 @@
   </si>
   <si>
     <t xml:space="preserve">     SkraBBKle Coursework Project</t>
+  </si>
+  <si>
+    <t>Game now displays human, and or computer tiles (if open game).</t>
+  </si>
+  <si>
+    <t>Focus on getting methods working in a  'rough and ready' status.</t>
+  </si>
+  <si>
+    <t>With 14 days remaining, I'm becoming increasing aware of how quickly time is running out. Focus now on brute-forcibly trying to make the game work, with refinement and unit-testing pushed to the lesser background for now.  Becoming more au fait with ArrayList and Map data structures and how best to implement them.
+Developing an agile/scrum mental mindset, proritizing a 'product log' of fixes, encompassing the 'bigger picture', with lots of short, tactical scrum-style sprint-log periods.</t>
   </si>
 </sst>
 </file>
@@ -307,55 +317,49 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </left>
-      <right style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -406,24 +410,6 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="15" fontId="13" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="13" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="12" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -436,15 +422,6 @@
     <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -452,6 +429,33 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="13" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="12" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -469,7 +473,14 @@
     <cellStyle name="Phone" xfId="8" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Title" xfId="7" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -549,10 +560,10 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Library Book Checkout Sheet" defaultPivotStyle="PivotStyleMedium9">
     <tableStyle name="Library Book Checkout Sheet" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="4"/>
-      <tableStyleElement type="headerRow" dxfId="3"/>
-      <tableStyleElement type="firstColumn" dxfId="2"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="1"/>
+      <tableStyleElement type="wholeTable" dxfId="5"/>
+      <tableStyleElement type="headerRow" dxfId="4"/>
+      <tableStyleElement type="firstColumn" dxfId="3"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="2"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2906,7 +2917,7 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -2923,70 +2934,80 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" ht="38" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="10" t="str">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="4" t="str">
         <f ca="1">'Target '!A2-'Target '!A1&amp;" days remaining"</f>
-        <v>-16 days remaining</v>
+        <v>-14 days remaining</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="16"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="2" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" ht="199" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" s="2" customFormat="1" ht="199" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
-      <c r="B4" s="4">
-        <v>45357</v>
+      <c r="B4" s="16">
+        <v>45359</v>
       </c>
-      <c r="C4" s="5">
-        <v>0.55972222222222223</v>
+      <c r="C4" s="17">
+        <v>20.32</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>2</v>
+      <c r="D4" s="18" t="s">
+        <v>10</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>4</v>
+      <c r="E4" s="18" t="s">
+        <v>11</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>5</v>
+      <c r="F4" s="19" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" ht="199" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="B5" s="16">
+        <v>45357</v>
+      </c>
+      <c r="C5" s="17">
+        <v>13.26</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:6" s="2" customFormat="1" ht="199" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
@@ -3002,20 +3023,22 @@
     <mergeCell ref="B1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" display="maria@example.com" xr:uid="{88B321A4-DD7B-F84F-B438-77F9C9A234B6}"/>
-  </hyperlinks>
+  <conditionalFormatting sqref="B5:F5">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$A5=1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
-  <pageSetup scale="75" fitToHeight="0" orientation="landscape" r:id="rId2"/>
+  <pageSetup scale="75" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3029,24 +3052,24 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="31" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="23" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A1" s="11">
+      <c r="A1" s="5">
         <v>45373</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2" s="13">
+      <c r="A2" s="7">
         <f ca="1">TODAY()</f>
-        <v>45357</v>
+        <v>45359</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B3" s="11"/>
+      <c r="B3" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3054,23 +3077,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3374,22 +3386,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3416,9 +3435,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
printTileMap() Implement TreeMap data structure. This helper method now prints remaining tiles in alphabetical order. changed newGame instance, to currentGame
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F7825B-3CE0-7849-BD75-B17BD25860D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A2C724-D77C-5E43-A8BD-87783C3D9B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27340" yWindow="-2180" windowWidth="26040" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dev Log" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>DATE</t>
   </si>
@@ -80,16 +80,35 @@
 Developing an agile/scrum mental mindset, proritizing a 'product log' of fixes, encompassing the 'bigger picture', with lots of short, tactical scrum-style sprint-log periods.</t>
   </si>
   <si>
-    <t xml:space="preserve">  New dedicated 
-• Tile class
-• TileBag class</t>
-  </si>
-  <si>
     <t>Focus on requirements and the most appropriate data structures</t>
   </si>
   <si>
     <t>Major refactoring, as the HashMap had limitations (you can't put more than one of the same set element (2 x [E1] for example). Now single tile class dedicated to constructing a tile with letter and value.
 This is in conjunction with a new TileBag class. which is responsible for managing a collection of tiles, initializing them with their respective letters and values, and will hsve methods that eventually allow players to draw tiles randomlly, decrement the tileBag and a 'helper method' for printing the current contents of the tile bag.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  New dedicated 
+• Tile class
+• TileBag class
+• tileSetArray()</t>
+  </si>
+  <si>
+    <t>A tool to help as I move onto the turn-based game-play phase</t>
+  </si>
+  <si>
+    <t>printTileBag() helper method</t>
+  </si>
+  <si>
+    <t>Succressfully implented the printTileBag() method. While not in the brief, this helper file is a good tool for me to check if bag is decrementing as computer and human play goes on. 
+Initially, had problems as it would prtint the tiles in random order. such as:
+2 x [V4]
+1 x [K6]
+1 x [Z11] etc...
+Then worked the method to a TreeMap structure which preserves the order in which they were entered (tileBag), so they now print out:
+8 x [A1]
+2 x [B3]
+2 x [C3] etc...
+a good learning curve. Perhaps i'll implement this for humanRackTile()  and computerRackTile()</t>
   </si>
 </sst>
 </file>
@@ -452,6 +471,9 @@
     <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="13" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -468,9 +490,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="13" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2656,10 +2675,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Library Orig">
   <a:themeElements>
@@ -2927,7 +2942,7 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
@@ -2946,12 +2961,12 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" ht="38" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="20"/>
       <c r="F1" s="4" t="str">
         <f ca="1">'Target '!A2-'Target '!A1&amp;" days remaining"</f>
         <v>-13 days remaining</v>
@@ -2959,13 +2974,13 @@
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="17"/>
     </row>
     <row r="3" spans="1:6" s="2" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
@@ -2985,57 +3000,74 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" ht="199" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" s="2" customFormat="1" ht="320" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="10">
         <v>45360</v>
       </c>
-      <c r="C4" s="20">
-        <v>0.21458333333333332</v>
+      <c r="C4" s="14">
+        <v>0.27291666666666664</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" ht="199" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="10">
-        <v>45359</v>
+        <v>45360</v>
       </c>
-      <c r="C5" s="11">
-        <v>20.32</v>
+      <c r="C5" s="14">
+        <v>0.21458333333333332</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="2" customFormat="1" ht="199" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="10">
+        <v>45359</v>
+      </c>
+      <c r="C6" s="11">
+        <v>20.32</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="192" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="10">
         <v>45357</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C7" s="11">
         <v>13.26</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F7" s="13" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3044,7 +3076,7 @@
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B1:E1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:F6">
+  <conditionalFormatting sqref="B4:F7">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$A4=1</formula>
     </cfRule>
@@ -3094,23 +3126,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3414,22 +3435,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3456,9 +3484,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Player() - Create two subclasses HumanPlayer() and ComputerPlayer() that extend methods from Player, and consequently, instances of these can have their own tileRack, dynamic score, etc.
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A2C724-D77C-5E43-A8BD-87783C3D9B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1ABF12F-F21D-754F-ADE5-30A95C2865B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>DATE</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>PERCEPTION</t>
-  </si>
-  <si>
-    <t>REFLECTIONS</t>
   </si>
   <si>
     <t xml:space="preserve">     SkraBBKle Coursework Project</t>
@@ -109,6 +106,19 @@
 2 x [B3]
 2 x [C3] etc...
 a good learning curve. Perhaps i'll implement this for humanRackTile()  and computerRackTile()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The theory </t>
+  </si>
+  <si>
+    <t>It's Mother's Day, and I've created a 'Mother' class called Player(), along with two sibling child subclasses - HumanPlayer and ComputerPlayer. 
+These subclasses extend Player, which in turn utilize elements of TilBag, so the Human and Computer player instances can have their own tile racks, own scores, and both draw from the same TileBag.</t>
+  </si>
+  <si>
+    <t>Create superclasss Player, and two subclasses for inheritence</t>
+  </si>
+  <si>
+    <t>Thinking about efficiecny of code inheritence, and how instances can dynamically have their own methods, but share from the same superclass.</t>
   </si>
 </sst>
 </file>
@@ -2942,10 +2952,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2969,13 +2979,13 @@
       <c r="E1" s="20"/>
       <c r="F1" s="4" t="str">
         <f ca="1">'Target '!A2-'Target '!A1&amp;" days remaining"</f>
-        <v>-13 days remaining</v>
+        <v>-12 days remaining</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
@@ -2997,77 +3007,94 @@
         <v>7</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" ht="320" x14ac:dyDescent="0.15">
-      <c r="A4" s="1"/>
-      <c r="B4" s="10">
-        <v>45360</v>
-      </c>
-      <c r="C4" s="14">
-        <v>0.27291666666666664</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" ht="199" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" s="2" customFormat="1" ht="288" x14ac:dyDescent="0.15">
+      <c r="A4" s="1"/>
+      <c r="B4" s="10">
+        <v>45361</v>
+      </c>
+      <c r="C4" s="14">
+        <v>9.7222222222222224E-3</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="2" customFormat="1" ht="224" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="10">
         <v>45360</v>
       </c>
       <c r="C5" s="14">
-        <v>0.21458333333333332</v>
+        <v>0.27291666666666664</v>
       </c>
       <c r="D5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>13</v>
-      </c>
       <c r="F5" s="13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="2" customFormat="1" ht="199" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="10">
-        <v>45359</v>
+        <v>45360</v>
       </c>
-      <c r="C6" s="11">
-        <v>20.32</v>
+      <c r="C6" s="14">
+        <v>0.21458333333333332</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="192" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10">
+        <v>45359</v>
+      </c>
+      <c r="C7" s="11">
+        <v>20.32</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="125" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="10">
         <v>45357</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C8" s="11">
         <v>13.26</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F8" s="13" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3076,7 +3103,7 @@
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B1:E1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:F7">
+  <conditionalFormatting sqref="B4:F8">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$A4=1</formula>
     </cfRule>
@@ -3114,7 +3141,7 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="7">
         <f ca="1">TODAY()</f>
-        <v>45360</v>
+        <v>45361</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
@@ -3126,12 +3153,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3435,29 +3473,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3484,13 +3515,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
GamePlay() Implement/Try various methods to utilize a humand and computer instance. Work in progress.
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1ABF12F-F21D-754F-ADE5-30A95C2865B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E5EBADF-7AAC-7D4F-8EEC-DE59EF38FD2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>DATE</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>PERCEPTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     SkraBBKle Coursework Project</t>
   </si>
   <si>
     <t>Game now displays human, and or computer tiles (if open game).</t>
@@ -108,9 +105,6 @@
 a good learning curve. Perhaps i'll implement this for humanRackTile()  and computerRackTile()</t>
   </si>
   <si>
-    <t xml:space="preserve">The theory </t>
-  </si>
-  <si>
     <t>It's Mother's Day, and I've created a 'Mother' class called Player(), along with two sibling child subclasses - HumanPlayer and ComputerPlayer. 
 These subclasses extend Player, which in turn utilize elements of TilBag, so the Human and Computer player instances can have their own tile racks, own scores, and both draw from the same TileBag.</t>
   </si>
@@ -119,6 +113,46 @@
   </si>
   <si>
     <t>Thinking about efficiecny of code inheritence, and how instances can dynamically have their own methods, but share from the same superclass.</t>
+  </si>
+  <si>
+    <t>Composition</t>
+  </si>
+  <si>
+    <t>Overall programme logic and modularism.</t>
+  </si>
+  <si>
+    <r>
+      <t>Starting to thing abstractly about the object relationships, and how things fit together like a jigsaw puzzle. Creating the Player superclass, with Human and Computer players extending Player class propertiesseems definitely the best way to go and highly logical. 
+Now starting to understand the nuances of '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="3" tint="-0.24994659260841701"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Composition</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="3" tint="-0.24994659260841701"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>' - the 'has a' relationship. Both Human and Computer playere have a tileRack. Therefore, by having the TileBag class one can reuse the same tileRack object across the various instances of Humand and Computer player.</t>
+    </r>
+  </si>
+  <si>
+    <t>REFLECTIONS</t>
+  </si>
+  <si>
+    <t>PROGRESS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      SkraBBKle Coursework Project</t>
   </si>
 </sst>
 </file>
@@ -129,7 +163,7 @@
     <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
     <numFmt numFmtId="165" formatCode="&quot;Overdue&quot;;&quot;&quot;;&quot;&quot;"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.24994659260841701"/>
@@ -247,6 +281,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3" tint="-0.24994659260841701"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -273,7 +314,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -303,58 +344,6 @@
         <color theme="3" tint="-0.24994659260841701"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -393,18 +382,44 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right style="medium">
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -437,8 +452,9 @@
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -451,9 +467,6 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -463,35 +476,32 @@
     <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="13" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="12" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="12" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="13" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="13" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="20" fontId="12" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="3" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -499,11 +509,29 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="12" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="13">
     <cellStyle name="Comma" xfId="6" builtinId="3" customBuiltin="1"/>
     <cellStyle name="Comma [0]" xfId="10" builtinId="6" customBuiltin="1"/>
     <cellStyle name="Date" xfId="9" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -514,10 +542,88 @@
     <cellStyle name="Icon Set" xfId="11" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Input" xfId="3" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Per cent" xfId="12" builtinId="5"/>
     <cellStyle name="Phone" xfId="8" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Title" xfId="7" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -597,10 +703,10 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Library Book Checkout Sheet" defaultPivotStyle="PivotStyleMedium9">
     <tableStyle name="Library Book Checkout Sheet" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="4"/>
-      <tableStyleElement type="headerRow" dxfId="3"/>
-      <tableStyleElement type="firstColumn" dxfId="2"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="1"/>
+      <tableStyleElement type="wholeTable" dxfId="15"/>
+      <tableStyleElement type="headerRow" dxfId="14"/>
+      <tableStyleElement type="firstColumn" dxfId="13"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="12"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -642,7 +748,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="311150" y="701675"/>
+          <a:off x="311150" y="688975"/>
           <a:ext cx="419100" cy="419100"/>
           <a:chOff x="2457447" y="228602"/>
           <a:chExt cx="419100" cy="419100"/>
@@ -2952,10 +3058,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2963,149 +3069,216 @@
     <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="93.85546875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7109375" style="1"/>
+    <col min="7" max="7" width="24.140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="38" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="37" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="4" t="str">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="21" t="str">
         <f ca="1">'Target '!A2-'Target '!A1&amp;" days remaining"</f>
         <v>-12 days remaining</v>
       </c>
+      <c r="G1" s="22"/>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="20"/>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="1"/>
+      <c r="B3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="2" customFormat="1" ht="170" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1"/>
+      <c r="B4" s="9">
+        <v>45361</v>
+      </c>
+      <c r="C4" s="13">
+        <v>0.15625</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="15">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="1"/>
+      <c r="B5" s="9">
+        <v>45361</v>
+      </c>
+      <c r="C5" s="13">
+        <v>9.7222222222222224E-3</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="15">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1"/>
+      <c r="B6" s="9">
+        <v>45360</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="15">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="9">
+        <v>45360</v>
+      </c>
+      <c r="C7" s="13">
+        <v>0.21458333333333332</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="15">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="9">
+        <v>45359</v>
+      </c>
+      <c r="C8" s="10">
+        <v>20.32</v>
+      </c>
+      <c r="D8" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17"/>
+      <c r="E8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="15">
+        <v>0.32</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="1"/>
-      <c r="B3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>18</v>
+    <row r="9" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="9">
+        <v>45357</v>
+      </c>
+      <c r="C9" s="10">
+        <v>13.26</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="15">
+        <v>0.22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" ht="288" x14ac:dyDescent="0.15">
-      <c r="A4" s="1"/>
-      <c r="B4" s="10">
-        <v>45361</v>
-      </c>
-      <c r="C4" s="14">
-        <v>9.7222222222222224E-3</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" ht="224" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="1"/>
-      <c r="B5" s="10">
-        <v>45360</v>
-      </c>
-      <c r="C5" s="14">
-        <v>0.27291666666666664</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" ht="199" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="1"/>
-      <c r="B6" s="10">
-        <v>45360</v>
-      </c>
-      <c r="C6" s="14">
-        <v>0.21458333333333332</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="192" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="10">
-        <v>45359</v>
-      </c>
-      <c r="C7" s="11">
-        <v>20.32</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="125" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="10">
-        <v>45357</v>
-      </c>
-      <c r="C8" s="11">
-        <v>13.26</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
+    <row r="10" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="17" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="18" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="19" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="20" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:F2"/>
+  <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:F8">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="B4:F9">
+    <cfRule type="expression" dxfId="0" priority="12">
       <formula>$A4=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4:G9">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FF00B050"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{272DF8F1-2D7A-C948-BB97-5E4DFA143735}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
@@ -3115,6 +3288,27 @@
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{272DF8F1-2D7A-C948-BB97-5E4DFA143735}">
+            <x14:dataBar minLength="0" maxLength="100">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G4:G9</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3128,24 +3322,24 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="31" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="23" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="23" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A1" s="5">
+      <c r="A1" s="4">
         <v>45373</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2" s="7">
+      <c r="A2" s="6">
         <f ca="1">TODAY()</f>
         <v>45361</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B3" s="5"/>
+      <c r="B3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3153,23 +3347,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3473,22 +3656,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3515,9 +3705,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Player() Refine class to explicitly administer Human / Computer playes and tiles. Reformat TileBag to HashMap data structure..
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E5EBADF-7AAC-7D4F-8EEC-DE59EF38FD2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91D7AA6-7467-4D4D-B910-CC6A00A61FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>DATE</t>
   </si>
@@ -153,6 +153,39 @@
   </si>
   <si>
     <t xml:space="preserve">      SkraBBKle Coursework Project</t>
+  </si>
+  <si>
+    <t>12 days to go. Panic stations</t>
+  </si>
+  <si>
+    <t>public void eatSleepCodeRepeat() {
+    boolean notFinished = true;
+    while (notFinished) {
+        if (SkraBBKleGame() == notfinished) {
+            panic();
+            eat();
+            sleep();
+            code();
+        } else {
+            notFinished = false;
+        }
+    }
+    haveBeer();
+    chill();
+}</t>
+  </si>
+  <si>
+    <t>Work on human and computer tiles</t>
+  </si>
+  <si>
+    <t>More work on human and computer tiles</t>
+  </si>
+  <si>
+    <t>Logic of tile distribution</t>
+  </si>
+  <si>
+    <t>Spent a lt of time finessing the Player() superclass, and the individual tiles to print the Human and Computer tileRack.
+Working to realise the GamePlay class should be abstracted from this, and only be concerned with calling fucntions to read wordlist, put valid words on the board, tot up score, and remove tiles from the board. This will be the focus of my next work in the coming days.</t>
   </si>
 </sst>
 </file>
@@ -500,8 +533,14 @@
     <xf numFmtId="20" fontId="12" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="3" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="3" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="12" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -524,12 +563,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="12" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="6" builtinId="3" customBuiltin="1"/>
@@ -546,84 +579,7 @@
     <cellStyle name="Phone" xfId="8" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Title" xfId="7" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <b/>
@@ -703,10 +659,10 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Library Book Checkout Sheet" defaultPivotStyle="PivotStyleMedium9">
     <tableStyle name="Library Book Checkout Sheet" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="15"/>
-      <tableStyleElement type="headerRow" dxfId="14"/>
-      <tableStyleElement type="firstColumn" dxfId="13"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="12"/>
+      <tableStyleElement type="wholeTable" dxfId="4"/>
+      <tableStyleElement type="headerRow" dxfId="3"/>
+      <tableStyleElement type="firstColumn" dxfId="2"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="1"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -3060,8 +3016,8 @@
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3078,28 +3034,28 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="37" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="21" t="str">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="23" t="str">
         <f ca="1">'Target '!A2-'Target '!A1&amp;" days remaining"</f>
         <v>-12 days remaining</v>
       </c>
-      <c r="G1" s="22"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="3" spans="1:7" s="2" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
@@ -3122,25 +3078,25 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="170" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
         <v>45361</v>
       </c>
       <c r="C4" s="13">
-        <v>0.15625</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>21</v>
+        <v>0.84236111111111112</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="G4" s="15">
-        <v>0.46</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3149,104 +3105,142 @@
         <v>45361</v>
       </c>
       <c r="C5" s="13">
-        <v>9.7222222222222224E-3</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>17</v>
+        <v>0.58819444444444446</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="G5" s="15">
-        <v>0.42</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
-        <v>45360</v>
+        <v>45361</v>
       </c>
       <c r="C6" s="13">
-        <v>0.27291666666666664</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>14</v>
+        <v>0.15625</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>20</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G6" s="15">
-        <v>0.37</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="9">
-        <v>45360</v>
+        <v>45361</v>
       </c>
       <c r="C7" s="13">
-        <v>0.21458333333333332</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>13</v>
+        <v>9.7222222222222224E-3</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>18</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>12</v>
+        <v>19</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="G7" s="15">
-        <v>0.34</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="9">
-        <v>45359</v>
-      </c>
-      <c r="C8" s="10">
-        <v>20.32</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>8</v>
+        <v>45360</v>
+      </c>
+      <c r="C8" s="13">
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>15</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G8" s="15">
-        <v>0.32</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="9">
+        <v>45360</v>
+      </c>
+      <c r="C9" s="13">
+        <v>0.21458333333333332</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="15">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="9">
+        <v>45359</v>
+      </c>
+      <c r="C10" s="10">
+        <v>20.32</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="15">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="9">
         <v>45357</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C11" s="10">
         <v>13.26</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E11" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F11" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G11" s="15">
         <v>0.22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="11" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="12" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="13" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="14" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3262,12 +3256,12 @@
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:F9">
+  <conditionalFormatting sqref="B4:F11">
     <cfRule type="expression" dxfId="0" priority="12">
       <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G9">
+  <conditionalFormatting sqref="G4:G11">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -3304,7 +3298,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G9</xm:sqref>
+          <xm:sqref>G4:G11</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
GamePlay() Work on logic for human to enter tiles  with new enterTile() method.
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD865443-ABE4-2E43-BF00-F650BCEB7EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F239669-1FBA-4C89-894B-6C89BA9D7107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dev Log" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>DATE</t>
   </si>
@@ -196,6 +196,15 @@
   </si>
   <si>
     <t>Key-value pairs transposed. Step Back Away from the computer !</t>
+  </si>
+  <si>
+    <t>Begin logic for user to enter tiles</t>
+  </si>
+  <si>
+    <t>Work on logic for user to enter tiles</t>
+  </si>
+  <si>
+    <t>Onwards and upwards</t>
   </si>
 </sst>
 </file>
@@ -585,7 +594,7 @@
     <cellStyle name="Icon Set" xfId="11" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Input" xfId="3" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Per cent" xfId="12" builtinId="5"/>
+    <cellStyle name="Percent" xfId="12" builtinId="5"/>
     <cellStyle name="Phone" xfId="8" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Title" xfId="7" builtinId="15" customBuiltin="1"/>
   </cellStyles>
@@ -714,7 +723,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="311150" y="688975"/>
+          <a:off x="304800" y="695325"/>
           <a:ext cx="419100" cy="419100"/>
           <a:chOff x="2457447" y="228602"/>
           <a:chExt cx="419100" cy="419100"/>
@@ -3026,23 +3035,23 @@
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="93.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.140625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.7109375" style="1"/>
+    <col min="5" max="5" width="19.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="93.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.109375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="37" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="37.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="18" t="s">
         <v>3</v>
@@ -3052,11 +3061,11 @@
       <c r="E1" s="19"/>
       <c r="F1" s="23" t="str">
         <f ca="1">'Target '!A2-'Target '!A1&amp;" days remaining"</f>
-        <v>-12 days remaining</v>
+        <v>-10 days remaining</v>
       </c>
       <c r="G1" s="24"/>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="20" t="s">
         <v>25</v>
@@ -3067,7 +3076,7 @@
       <c r="F2" s="21"/>
       <c r="G2" s="22"/>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="59.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="7" t="s">
         <v>0</v>
@@ -3088,209 +3097,228 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" s="2" customFormat="1" ht="297.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="C4" s="13">
-        <v>0.95208333333333328</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G4" s="15">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="285.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="9">
         <v>45361</v>
       </c>
       <c r="C5" s="13">
-        <v>0.84236111111111112</v>
+        <v>0.95208333333333328</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G5" s="15">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="285.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
         <v>45361</v>
       </c>
       <c r="C6" s="13">
-        <v>0.58819444444444446</v>
+        <v>0.84236111111111112</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G6" s="15">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="285.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="9">
         <v>45361</v>
       </c>
       <c r="C7" s="13">
-        <v>0.15625</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="G7" s="15">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="285.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="9">
         <v>45361</v>
       </c>
       <c r="C8" s="13">
+        <v>0.15625</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="15">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="285.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="9">
+        <v>45361</v>
+      </c>
+      <c r="C9" s="13">
         <v>9.7222222222222224E-3</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D9" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F9" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G9" s="15">
         <v>0.42</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="9">
-        <v>45360</v>
-      </c>
-      <c r="C9" s="13">
-        <v>0.27291666666666664</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="15">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="285.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="9">
         <v>45360</v>
       </c>
       <c r="C10" s="13">
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="15">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="285.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="9">
+        <v>45360</v>
+      </c>
+      <c r="C11" s="13">
         <v>0.21458333333333332</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D11" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G11" s="15">
         <v>0.34</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="9">
+    <row r="12" spans="1:7" ht="285.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="9">
         <v>45359</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C12" s="10">
         <v>20.32</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D12" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G12" s="15">
         <v>0.32</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="9">
+    <row r="13" spans="1:7" ht="285.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="9">
         <v>45357</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C13" s="10">
         <v>13.26</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D13" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E13" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F13" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G13" s="15">
         <v>0.22</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="17" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="18" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="19" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="20" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:7" ht="285.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:7" ht="285.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:7" ht="285.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="285.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="285.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="285.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="285.95" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:F12">
+  <conditionalFormatting sqref="B4:F13">
     <cfRule type="expression" dxfId="0" priority="12">
       <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G12">
+  <conditionalFormatting sqref="G4:G13">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -3327,7 +3355,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G12</xm:sqref>
+          <xm:sqref>G4:G13</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3343,25 +3371,25 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="31" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="30.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4">
         <v>45373</v>
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45361</v>
+        <v>45363</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="4"/>
     </row>
   </sheetData>
@@ -3390,6 +3418,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3689,15 +3726,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
   <ds:schemaRefs>
@@ -3711,6 +3739,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1101C2D-3F57-4FE3-804B-005C212162D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3731,14 +3767,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
Fix  logic using while loop to continuously prompt user, if they do not enter the correct format. - i.e.,  word followed by comma, and  letter (or _) and up to two numbers.
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F239669-1FBA-4C89-894B-6C89BA9D7107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF5A2D2-DFDE-4547-8FB0-0C23BC84437B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dev Log" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>DATE</t>
   </si>
@@ -205,6 +205,15 @@
   </si>
   <si>
     <t>Onwards and upwards</t>
+  </si>
+  <si>
+    <t>enterWordAndTile()</t>
+  </si>
+  <si>
+    <t>Fixing logic using while loop to continuously prompt user, if they do not enter the correct format. - ine.m word, letter (or _) and up to two numbers.</t>
+  </si>
+  <si>
+    <t>trying out different loops and string formatting techniques</t>
   </si>
 </sst>
 </file>
@@ -594,7 +603,7 @@
     <cellStyle name="Icon Set" xfId="11" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Input" xfId="3" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Percent" xfId="12" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="12" builtinId="5"/>
     <cellStyle name="Phone" xfId="8" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Title" xfId="7" builtinId="15" customBuiltin="1"/>
   </cellStyles>
@@ -723,7 +732,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="304800" y="695325"/>
+          <a:off x="311150" y="688975"/>
           <a:ext cx="419100" cy="419100"/>
           <a:chOff x="2457447" y="228602"/>
           <a:chExt cx="419100" cy="419100"/>
@@ -3035,23 +3044,23 @@
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="93.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.109375" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.6640625" style="1"/>
+    <col min="5" max="5" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="93.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="37.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="37" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="18" t="s">
         <v>3</v>
@@ -3061,11 +3070,11 @@
       <c r="E1" s="19"/>
       <c r="F1" s="23" t="str">
         <f ca="1">'Target '!A2-'Target '!A1&amp;" days remaining"</f>
-        <v>-10 days remaining</v>
+        <v>-9 days remaining</v>
       </c>
       <c r="G1" s="24"/>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="20" t="s">
         <v>25</v>
@@ -3076,7 +3085,7 @@
       <c r="F2" s="21"/>
       <c r="G2" s="22"/>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="59.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="7" t="s">
         <v>0</v>
@@ -3097,228 +3106,247 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="297.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
-        <v>45363</v>
+        <v>45364</v>
       </c>
       <c r="C4" s="13">
-        <v>0.56666666666666665</v>
+        <v>0.22708333333333333</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G4" s="15">
-        <v>0.54</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="285.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="9">
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="C5" s="13">
-        <v>0.95208333333333328</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G5" s="15">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" ht="285.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
         <v>45361</v>
       </c>
       <c r="C6" s="13">
-        <v>0.84236111111111112</v>
+        <v>0.95208333333333328</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G6" s="15">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="285.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="9">
         <v>45361</v>
       </c>
       <c r="C7" s="13">
-        <v>0.58819444444444446</v>
+        <v>0.84236111111111112</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G7" s="15">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="285.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="9">
         <v>45361</v>
       </c>
       <c r="C8" s="13">
-        <v>0.15625</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="G8" s="15">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="285.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="9">
         <v>45361</v>
       </c>
       <c r="C9" s="13">
+        <v>0.15625</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="15">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="9">
+        <v>45361</v>
+      </c>
+      <c r="C10" s="13">
         <v>9.7222222222222224E-3</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D10" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F10" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G10" s="15">
         <v>0.42</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="285.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="9">
-        <v>45360</v>
-      </c>
-      <c r="C10" s="13">
-        <v>0.27291666666666664</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="15">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="285.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9">
         <v>45360</v>
       </c>
       <c r="C11" s="13">
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="15">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="9">
+        <v>45360</v>
+      </c>
+      <c r="C12" s="13">
         <v>0.21458333333333332</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D12" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F12" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G12" s="15">
         <v>0.34</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="285.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="9">
+    <row r="13" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="9">
         <v>45359</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C13" s="10">
         <v>20.32</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D13" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E13" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G13" s="15">
         <v>0.32</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="285.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="9">
+    <row r="14" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="9">
         <v>45357</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C14" s="10">
         <v>13.26</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D14" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E14" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F14" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G14" s="15">
         <v>0.22</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="285.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:7" ht="285.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:7" ht="285.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="285.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="285.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="285.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="285.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="17" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="18" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="19" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="20" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:F13">
+  <conditionalFormatting sqref="B4:F14">
     <cfRule type="expression" dxfId="0" priority="12">
       <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G13">
+  <conditionalFormatting sqref="G4:G14">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -3355,7 +3383,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G13</xm:sqref>
+          <xm:sqref>G4:G14</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3371,25 +3399,25 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="30.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="31" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="23" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="4">
         <v>45373</v>
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45363</v>
+        <v>45364</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B3" s="4"/>
     </row>
   </sheetData>
@@ -3398,35 +3426,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3726,27 +3725,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1101C2D-3F57-4FE3-804B-005C212162D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3767,6 +3775,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
enterwordAndile() Update method to call an isValidWord() method that verifies if  first part of user string (the word), is in the directory.
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF5A2D2-DFDE-4547-8FB0-0C23BC84437B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7612BC4F-EE7E-4C41-BEA9-F2E34967780E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>DATE</t>
   </si>
@@ -214,6 +214,12 @@
   </si>
   <si>
     <t>trying out different loops and string formatting techniques</t>
+  </si>
+  <si>
+    <t>Testing validation against wordlist.txt</t>
+  </si>
+  <si>
+    <t>enterwordAndile() method Now verifes if first part of user string (the word), is in the directory. Although a lot of unit testing is needed.</t>
   </si>
 </sst>
 </file>
@@ -3044,8 +3050,8 @@
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3112,61 +3118,61 @@
         <v>45364</v>
       </c>
       <c r="C4" s="13">
-        <v>0.22708333333333333</v>
+        <v>0.35138888888888886</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>38</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G4" s="15">
-        <v>0.56000000000000005</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="9">
-        <v>45363</v>
+        <v>45364</v>
       </c>
       <c r="C5" s="13">
-        <v>0.56666666666666665</v>
+        <v>0.22708333333333333</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G5" s="15">
-        <v>0.54</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="C6" s="13">
-        <v>0.95208333333333328</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G6" s="15">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3174,19 +3180,19 @@
         <v>45361</v>
       </c>
       <c r="C7" s="13">
-        <v>0.84236111111111112</v>
+        <v>0.95208333333333328</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G7" s="15">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3194,19 +3200,19 @@
         <v>45361</v>
       </c>
       <c r="C8" s="13">
-        <v>0.58819444444444446</v>
+        <v>0.84236111111111112</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G8" s="15">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3214,19 +3220,19 @@
         <v>45361</v>
       </c>
       <c r="C9" s="13">
-        <v>0.15625</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="G9" s="15">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3234,39 +3240,39 @@
         <v>45361</v>
       </c>
       <c r="C10" s="13">
-        <v>9.7222222222222224E-3</v>
+        <v>0.15625</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="G10" s="15">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9">
-        <v>45360</v>
+        <v>45361</v>
       </c>
       <c r="C11" s="13">
-        <v>0.27291666666666664</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="G11" s="15">
-        <v>0.37</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3274,62 +3280,81 @@
         <v>45360</v>
       </c>
       <c r="C12" s="13">
-        <v>0.21458333333333332</v>
+        <v>0.27291666666666664</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G12" s="15">
-        <v>0.34</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="9">
-        <v>45359</v>
-      </c>
-      <c r="C13" s="10">
-        <v>20.32</v>
+        <v>45360</v>
+      </c>
+      <c r="C13" s="13">
+        <v>0.21458333333333332</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G13" s="15">
-        <v>0.32</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="9">
+        <v>45359</v>
+      </c>
+      <c r="C14" s="10">
+        <v>20.32</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="15">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="9">
         <v>45357</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C15" s="10">
         <v>13.26</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D15" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E15" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F15" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G15" s="15">
         <v>0.22</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="16" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="17" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="18" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3341,12 +3366,12 @@
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:F14">
+  <conditionalFormatting sqref="B4:F15">
     <cfRule type="expression" dxfId="0" priority="12">
       <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G14">
+  <conditionalFormatting sqref="G4:G15">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -3383,7 +3408,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G14</xm:sqref>
+          <xm:sqref>G4:G15</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3426,6 +3451,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3725,36 +3779,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1101C2D-3F57-4FE3-804B-005C212162D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3775,26 +3820,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
BoardInit() CHanges to board load, and GamePlay logic.
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7612BC4F-EE7E-4C41-BEA9-F2E34967780E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BA710B-322D-6E4F-B533-A830626A6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>DATE</t>
   </si>
@@ -220,6 +220,16 @@
   </si>
   <si>
     <t>enterwordAndile() method Now verifes if first part of user string (the word), is in the directory. Although a lot of unit testing is needed.</t>
+  </si>
+  <si>
+    <t>GamePlay() and BoardUnit(0 - working to set element to board</t>
+  </si>
+  <si>
+    <t>Pedal to the metal.</t>
+  </si>
+  <si>
+    <t>With 8 days remaining, the effort to really push out a working version (at the cost of rigourous testing) is becoming apparent. A deep learning curve does not tie in the the luxury of having enough time. Hence, the 'brute force' approach to trying everything and seeing - throwing mud at the wall and see if it sticks, then commit/push, or roll back.
+I now see the benefit of systemic test-driven development. But at this stage, it's a case of getting it to work, just to show I do understand how to implement this - even if in a very rudimental way, THEN looking at testing or optimizing code.</t>
   </si>
 </sst>
 </file>
@@ -3050,8 +3060,8 @@
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3076,7 +3086,7 @@
       <c r="E1" s="19"/>
       <c r="F1" s="23" t="str">
         <f ca="1">'Target '!A2-'Target '!A1&amp;" days remaining"</f>
-        <v>-9 days remaining</v>
+        <v>-8 days remaining</v>
       </c>
       <c r="G1" s="24"/>
     </row>
@@ -3115,22 +3125,22 @@
     <row r="4" spans="1:7" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="C4" s="13">
-        <v>0.35138888888888886</v>
+        <v>2.1527777777777778E-2</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G4" s="15">
-        <v>0.57999999999999996</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3139,60 +3149,60 @@
         <v>45364</v>
       </c>
       <c r="C5" s="13">
-        <v>0.22708333333333333</v>
+        <v>0.35138888888888886</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>38</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G5" s="15">
-        <v>0.56000000000000005</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
-        <v>45363</v>
+        <v>45364</v>
       </c>
       <c r="C6" s="13">
-        <v>0.56666666666666665</v>
+        <v>0.22708333333333333</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G6" s="15">
-        <v>0.54</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="9">
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="C7" s="13">
-        <v>0.95208333333333328</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G7" s="15">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3200,19 +3210,19 @@
         <v>45361</v>
       </c>
       <c r="C8" s="13">
-        <v>0.84236111111111112</v>
+        <v>0.95208333333333328</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G8" s="15">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3220,19 +3230,19 @@
         <v>45361</v>
       </c>
       <c r="C9" s="13">
-        <v>0.58819444444444446</v>
+        <v>0.84236111111111112</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G9" s="15">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3240,19 +3250,19 @@
         <v>45361</v>
       </c>
       <c r="C10" s="13">
-        <v>0.15625</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="G10" s="15">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3260,39 +3270,39 @@
         <v>45361</v>
       </c>
       <c r="C11" s="13">
-        <v>9.7222222222222224E-3</v>
+        <v>0.15625</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="G11" s="15">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="9">
-        <v>45360</v>
+        <v>45361</v>
       </c>
       <c r="C12" s="13">
-        <v>0.27291666666666664</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="G12" s="15">
-        <v>0.37</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3300,62 +3310,81 @@
         <v>45360</v>
       </c>
       <c r="C13" s="13">
-        <v>0.21458333333333332</v>
+        <v>0.27291666666666664</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G13" s="15">
-        <v>0.34</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="9">
-        <v>45359</v>
-      </c>
-      <c r="C14" s="10">
-        <v>20.32</v>
+        <v>45360</v>
+      </c>
+      <c r="C14" s="13">
+        <v>0.21458333333333332</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G14" s="15">
-        <v>0.32</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="9">
+        <v>45359</v>
+      </c>
+      <c r="C15" s="10">
+        <v>20.32</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="15">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="9">
         <v>45357</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C16" s="10">
         <v>13.26</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E16" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F16" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G16" s="15">
         <v>0.22</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="17" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="18" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="19" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3366,12 +3395,12 @@
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:F15">
+  <conditionalFormatting sqref="B4:F16">
     <cfRule type="expression" dxfId="0" priority="12">
       <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G15">
+  <conditionalFormatting sqref="G4:G16">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -3408,7 +3437,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G15</xm:sqref>
+          <xm:sqref>G4:G16</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3439,7 +3468,7 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45364</v>
+        <v>45365</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
@@ -3451,35 +3480,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3779,27 +3779,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1101C2D-3F57-4FE3-804B-005C212162D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3820,6 +3829,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
GamePlay gameInPlay(): Work on GamePlay class and a GameInPlay method that handles game logic (human player move, validate, score, computer move, validate, score, etc).
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BA710B-322D-6E4F-B533-A830626A6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68A69ED-CA10-7A4D-8D31-757AB7162ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32000" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dev Log" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>DATE</t>
   </si>
@@ -158,11 +158,88 @@
     <t>12 days to go. Panic stations</t>
   </si>
   <si>
+    <t>Work on human and computer tiles</t>
+  </si>
+  <si>
+    <t>More work on human and computer tiles</t>
+  </si>
+  <si>
+    <t>Logic of tile distribution</t>
+  </si>
+  <si>
+    <t>Spent a lt of time finessing the Player() superclass, and the individual tiles to print the Human and Computer tileRack.
+Working to realise the GamePlay class should be abstracted from this, and only be concerned with calling fucntions to read wordlist, put valid words on the board, tot up score, and remove tiles from the board. This will be the focus of my next work in the coming days.</t>
+  </si>
+  <si>
+    <t>After stepping away from computer for a bit, I came back to realise i had just created the biggest bug in the entire game. For some reason, i had transposed the keyxalue pairs from the data on the breif. so in stead of 8 x [A1], it was showing 1 x [A8] - 1 tile of A8 worth 8 points ! his was the reason why everything was printing wrong, and i was going down such a rabbit whole not realising this.
+Could not believe this how a critical error, so crucial to the game could be missed. I realise this is where the benefit of working in teams or in pairs helps. Sometimes one's eyes just do not spot the most glaringly obvious of bugs.</t>
+  </si>
+  <si>
+    <t>Critical bug fix</t>
+  </si>
+  <si>
+    <t>Key-value pairs transposed. Step Back Away from the computer !</t>
+  </si>
+  <si>
+    <t>Begin logic for user to enter tiles</t>
+  </si>
+  <si>
+    <t>Work on logic for user to enter tiles</t>
+  </si>
+  <si>
+    <t>Onwards and upwards</t>
+  </si>
+  <si>
+    <t>enterWordAndTile()</t>
+  </si>
+  <si>
+    <t>Fixing logic using while loop to continuously prompt user, if they do not enter the correct format. - ine.m word, letter (or _) and up to two numbers.</t>
+  </si>
+  <si>
+    <t>trying out different loops and string formatting techniques</t>
+  </si>
+  <si>
+    <t>Testing validation against wordlist.txt</t>
+  </si>
+  <si>
+    <t>enterwordAndile() method Now verifes if first part of user string (the word), is in the directory. Although a lot of unit testing is needed.</t>
+  </si>
+  <si>
+    <t>GamePlay() and BoardUnit(0 - working to set element to board</t>
+  </si>
+  <si>
+    <t>Pedal to the metal.</t>
+  </si>
+  <si>
+    <t>With 8 days remaining, the effort to really push out a working version (at the cost of rigourous testing) is becoming apparent. A deep learning curve does not tie in the the luxury of having enough time. Hence, the 'brute force' approach to trying everything and seeing - throwing mud at the wall and see if it sticks, then commit/push, or roll back.
+I now see the benefit of systemic test-driven development. But at this stage, it's a case of getting it to work, just to show I do understand how to implement this - even if in a very rudimental way, THEN looking at testing or optimizing code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spent today working on the GamePlay 
+class and a created a new gameInPlay()
+method that handles all in-game logic 
+(human player move, validate, score, 
+computer move, validate, score, etc). 
+Code looking very ‘spaghetti-like’’ at 
+the moment, but is something I 
+understand and can clean up later.
+Lots of // TODO comments as I’m just 
+fleshing out logic Within the GameInPlay class.
+Also lots of roll backs ‘reset current branch to main’, as tried and things tested are thrown away. All in all, getting better at using git. If I get this working, will be a major jump in progress.
+  </t>
+  </si>
+  <si>
+    <t>GamePlay() gameInPlay() - Overall game logic</t>
+  </si>
+  <si>
+    <t>Working on the 'Meat and Veg' - Fleshing out the game.</t>
+  </si>
+  <si>
     <t>public void eatSleepCodeRepeat() {
     boolean notFinished = true;
     while (notFinished) {
         if (SkraBBKleGame() == notfinished) {
-            panic();
+            panic();  // Check if currentDay &lt;= CW_DEADLINE_22_MARCH
             eat();
             sleep();
             code();
@@ -174,63 +251,6 @@
     chill();
 }</t>
   </si>
-  <si>
-    <t>Work on human and computer tiles</t>
-  </si>
-  <si>
-    <t>More work on human and computer tiles</t>
-  </si>
-  <si>
-    <t>Logic of tile distribution</t>
-  </si>
-  <si>
-    <t>Spent a lt of time finessing the Player() superclass, and the individual tiles to print the Human and Computer tileRack.
-Working to realise the GamePlay class should be abstracted from this, and only be concerned with calling fucntions to read wordlist, put valid words on the board, tot up score, and remove tiles from the board. This will be the focus of my next work in the coming days.</t>
-  </si>
-  <si>
-    <t>After stepping away from computer for a bit, I came back to realise i had just created the biggest bug in the entire game. For some reason, i had transposed the keyxalue pairs from the data on the breif. so in stead of 8 x [A1], it was showing 1 x [A8] - 1 tile of A8 worth 8 points ! his was the reason why everything was printing wrong, and i was going down such a rabbit whole not realising this.
-Could not believe this how a critical error, so crucial to the game could be missed. I realise this is where the benefit of working in teams or in pairs helps. Sometimes one's eyes just do not spot the most glaringly obvious of bugs.</t>
-  </si>
-  <si>
-    <t>Critical bug fix</t>
-  </si>
-  <si>
-    <t>Key-value pairs transposed. Step Back Away from the computer !</t>
-  </si>
-  <si>
-    <t>Begin logic for user to enter tiles</t>
-  </si>
-  <si>
-    <t>Work on logic for user to enter tiles</t>
-  </si>
-  <si>
-    <t>Onwards and upwards</t>
-  </si>
-  <si>
-    <t>enterWordAndTile()</t>
-  </si>
-  <si>
-    <t>Fixing logic using while loop to continuously prompt user, if they do not enter the correct format. - ine.m word, letter (or _) and up to two numbers.</t>
-  </si>
-  <si>
-    <t>trying out different loops and string formatting techniques</t>
-  </si>
-  <si>
-    <t>Testing validation against wordlist.txt</t>
-  </si>
-  <si>
-    <t>enterwordAndile() method Now verifes if first part of user string (the word), is in the directory. Although a lot of unit testing is needed.</t>
-  </si>
-  <si>
-    <t>GamePlay() and BoardUnit(0 - working to set element to board</t>
-  </si>
-  <si>
-    <t>Pedal to the metal.</t>
-  </si>
-  <si>
-    <t>With 8 days remaining, the effort to really push out a working version (at the cost of rigourous testing) is becoming apparent. A deep learning curve does not tie in the the luxury of having enough time. Hence, the 'brute force' approach to trying everything and seeing - throwing mud at the wall and see if it sticks, then commit/push, or roll back.
-I now see the benefit of systemic test-driven development. But at this stage, it's a case of getting it to work, just to show I do understand how to implement this - even if in a very rudimental way, THEN looking at testing or optimizing code.</t>
-  </si>
 </sst>
 </file>
 
@@ -240,7 +260,7 @@
     <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
     <numFmt numFmtId="165" formatCode="&quot;Overdue&quot;;&quot;&quot;;&quot;&quot;"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.24994659260841701"/>
@@ -363,6 +383,12 @@
       <sz val="15"/>
       <color theme="3" tint="-0.24994659260841701"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="3" tint="-0.24994659260841701"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -531,7 +557,7 @@
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -606,6 +632,12 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -2788,6 +2820,67 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3521028</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>8293099</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2705100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F950584-6B19-EFDA-04AF-30341341CE70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9070928" y="2095500"/>
+          <a:ext cx="4772071" cy="2667000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3058,10 +3151,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3076,7 +3169,7 @@
     <col min="8" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="37" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="37" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="18" t="s">
         <v>3</v>
@@ -3086,11 +3179,11 @@
       <c r="E1" s="19"/>
       <c r="F1" s="23" t="str">
         <f ca="1">'Target '!A2-'Target '!A1&amp;" days remaining"</f>
-        <v>-8 days remaining</v>
+        <v>-7 days remaining</v>
       </c>
       <c r="G1" s="24"/>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="20" t="s">
         <v>25</v>
@@ -3101,7 +3194,7 @@
       <c r="F2" s="21"/>
       <c r="G2" s="22"/>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="7" t="s">
         <v>0</v>
@@ -3122,285 +3215,305 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="C4" s="13">
-        <v>2.1527777777777778E-2</v>
+        <v>0.98611111111111116</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="26" t="s">
         <v>45</v>
       </c>
       <c r="G4" s="15">
-        <v>0.6</v>
-      </c>
+        <v>0.63</v>
+      </c>
+      <c r="I4" s="25"/>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="9">
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="C5" s="13">
-        <v>0.35138888888888886</v>
+        <v>2.1527777777777778E-2</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G5" s="15">
-        <v>0.57999999999999996</v>
+        <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
         <v>45364</v>
       </c>
       <c r="C6" s="13">
-        <v>0.22708333333333333</v>
+        <v>0.35138888888888886</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>40</v>
       </c>
       <c r="F6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="15">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="9">
+        <v>45364</v>
+      </c>
+      <c r="C7" s="13">
+        <v>0.22708333333333333</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="15">
+      <c r="F7" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="15">
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="9">
+    <row r="8" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="9">
         <v>45363</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C8" s="13">
         <v>0.56666666666666665</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D8" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="15">
+      <c r="F8" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="15">
         <v>0.54</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="9">
-        <v>45361</v>
-      </c>
-      <c r="C8" s="13">
-        <v>0.95208333333333328</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="15">
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="9">
         <v>45361</v>
       </c>
       <c r="C9" s="13">
-        <v>0.84236111111111112</v>
+        <v>0.95208333333333328</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>31</v>
       </c>
       <c r="G9" s="15">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="9">
         <v>45361</v>
       </c>
       <c r="C10" s="13">
-        <v>0.58819444444444446</v>
+        <v>0.84236111111111112</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>28</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G10" s="15">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9">
         <v>45361</v>
       </c>
       <c r="C11" s="13">
-        <v>0.15625</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G11" s="15">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="9">
         <v>45361</v>
       </c>
       <c r="C12" s="13">
+        <v>0.15625</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="15">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="9">
+        <v>45361</v>
+      </c>
+      <c r="C13" s="13">
         <v>9.7222222222222224E-3</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D13" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E13" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F13" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G13" s="15">
         <v>0.42</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="9">
-        <v>45360</v>
-      </c>
-      <c r="C13" s="13">
-        <v>0.27291666666666664</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="15">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="9">
         <v>45360</v>
       </c>
       <c r="C14" s="13">
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="15">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="9">
+        <v>45360</v>
+      </c>
+      <c r="C15" s="13">
         <v>0.21458333333333332</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D15" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E15" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F15" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G15" s="15">
         <v>0.34</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="9">
+    <row r="16" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="9">
         <v>45359</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C16" s="10">
         <v>20.32</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D16" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E16" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F16" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G16" s="15">
         <v>0.32</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="9">
+    <row r="17" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="9">
         <v>45357</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C17" s="10">
         <v>13.26</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D17" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E17" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F17" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G17" s="15">
         <v>0.22</v>
       </c>
     </row>
-    <row r="17" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="18" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="19" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="20" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="18" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="19" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="20" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:F16">
+  <conditionalFormatting sqref="B4:F17">
     <cfRule type="expression" dxfId="0" priority="12">
       <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G16">
+  <conditionalFormatting sqref="G4:G17">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -3437,7 +3550,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G16</xm:sqref>
+          <xm:sqref>G4:G17</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3468,7 +3581,7 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45365</v>
+        <v>45366</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
@@ -3480,6 +3593,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3779,36 +3921,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1101C2D-3F57-4FE3-804B-005C212162D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3829,26 +3962,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
BoardInit class - Refactor  to remove circular dependency, as BoardInit has a GamePlay instance, and GabePlay class has a BoardInit instance.
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68A69ED-CA10-7A4D-8D31-757AB7162ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283EBDB4-ED11-6445-931E-7B305CC125F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="32000" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>DATE</t>
   </si>
@@ -250,6 +250,18 @@
     haveBeer();
     chill();
 }</t>
+  </si>
+  <si>
+    <t>Resolve Circular Dependency between BoardInit and GamePlay</t>
+  </si>
+  <si>
+    <t>Logic is king.</t>
+  </si>
+  <si>
+    <t>Removed GamePlay instance as a member of BoardInit class, as GamePlay class also had a BoardInit instrance - creating a circular dependency.
+Starting to realise,  it’s not about coding, it’s about logic and game flow. You can copy code blocks (methods), move them around how you like, pass parameters into them and be very dynamic, but if the game flow is wrong (i.e., if you have tile methods in a BoardInit class) you can get lost in your code and get very messy very quickly.
+I realise it would have been less headach (before I even wrote one line of code) if I’d just written down the entire game flow on a piece of paper as a flow chart diagram.  Now I see the benefit of creating a flowchart before diving into coding.
+End of another tired day. Time for some rest/recuperation, watch a movie. Then dive into more coding afresh tomorrow morning.</t>
   </si>
 </sst>
 </file>
@@ -612,6 +624,12 @@
     <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -632,12 +650,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -2820,25 +2832,20 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>3521028</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>8293099</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>2705100</xdr:rowOff>
-    </xdr:to>
+    <xdr:ext cx="4772071" cy="2667000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F950584-6B19-EFDA-04AF-30341341CE70}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1C1EAC0-C056-8D40-B376-1E883A64AA99}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2880,7 +2887,7 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3154,7 +3161,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3171,28 +3178,28 @@
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="37" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="23" t="str">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="25" t="str">
         <f ca="1">'Target '!A2-'Target '!A1&amp;" days remaining"</f>
-        <v>-7 days remaining</v>
-      </c>
-      <c r="G1" s="24"/>
+        <v>-6 days remaining</v>
+      </c>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="22"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
@@ -3218,65 +3225,65 @@
     <row r="4" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="C4" s="13">
-        <v>0.98611111111111116</v>
+        <v>7.0833333333333331E-2</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>45</v>
+        <v>50</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>51</v>
       </c>
       <c r="G4" s="15">
-        <v>0.63</v>
-      </c>
-      <c r="I4" s="25"/>
+        <v>0.64</v>
+      </c>
+      <c r="I4" s="18"/>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="9">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="C5" s="13">
-        <v>2.1527777777777778E-2</v>
+        <v>0.98611111111111116</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>44</v>
+        <v>47</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>45</v>
       </c>
       <c r="G5" s="15">
-        <v>0.6</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="C6" s="13">
-        <v>0.35138888888888886</v>
+        <v>2.1527777777777778E-2</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G6" s="15">
-        <v>0.57999999999999996</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3284,59 +3291,59 @@
         <v>45364</v>
       </c>
       <c r="C7" s="13">
-        <v>0.22708333333333333</v>
+        <v>0.35138888888888886</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>37</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G7" s="15">
-        <v>0.56000000000000005</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="9">
-        <v>45363</v>
+        <v>45364</v>
       </c>
       <c r="C8" s="13">
-        <v>0.56666666666666665</v>
+        <v>0.22708333333333333</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G8" s="15">
-        <v>0.54</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="9">
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="C9" s="13">
-        <v>0.95208333333333328</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G9" s="15">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3344,19 +3351,19 @@
         <v>45361</v>
       </c>
       <c r="C10" s="13">
-        <v>0.84236111111111112</v>
+        <v>0.95208333333333328</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G10" s="15">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3364,19 +3371,19 @@
         <v>45361</v>
       </c>
       <c r="C11" s="13">
-        <v>0.58819444444444446</v>
+        <v>0.84236111111111112</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="G11" s="15">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3384,19 +3391,19 @@
         <v>45361</v>
       </c>
       <c r="C12" s="13">
-        <v>0.15625</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G12" s="15">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3404,39 +3411,39 @@
         <v>45361</v>
       </c>
       <c r="C13" s="13">
-        <v>9.7222222222222224E-3</v>
+        <v>0.15625</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="G13" s="15">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="9">
-        <v>45360</v>
+        <v>45361</v>
       </c>
       <c r="C14" s="13">
-        <v>0.27291666666666664</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="G14" s="15">
-        <v>0.37</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3444,62 +3451,81 @@
         <v>45360</v>
       </c>
       <c r="C15" s="13">
-        <v>0.21458333333333332</v>
+        <v>0.27291666666666664</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G15" s="15">
-        <v>0.34</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="9">
-        <v>45359</v>
-      </c>
-      <c r="C16" s="10">
-        <v>20.32</v>
+        <v>45360</v>
+      </c>
+      <c r="C16" s="13">
+        <v>0.21458333333333332</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G16" s="15">
-        <v>0.32</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="9">
+        <v>45359</v>
+      </c>
+      <c r="C17" s="10">
+        <v>20.32</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="15">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="9">
         <v>45357</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C18" s="10">
         <v>13.26</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D18" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E18" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F18" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G18" s="15">
         <v>0.22</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="19" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="20" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
@@ -3508,12 +3534,12 @@
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:F17">
+  <conditionalFormatting sqref="B4:F18">
     <cfRule type="expression" dxfId="0" priority="12">
       <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G17">
+  <conditionalFormatting sqref="G4:G18">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -3550,7 +3576,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G17</xm:sqref>
+          <xm:sqref>G4:G18</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3581,7 +3607,7 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45366</v>
+        <v>45367</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
@@ -3593,35 +3619,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3921,27 +3918,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1101C2D-3F57-4FE3-804B-005C212162D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3962,6 +3968,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
enterWordAndDirection() Implement logic to validate human players word, so can be placed on board (within dimensions.)
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BA710B-322D-6E4F-B533-A830626A6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283EBDB4-ED11-6445-931E-7B305CC125F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32000" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dev Log" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>DATE</t>
   </si>
@@ -158,11 +158,88 @@
     <t>12 days to go. Panic stations</t>
   </si>
   <si>
+    <t>Work on human and computer tiles</t>
+  </si>
+  <si>
+    <t>More work on human and computer tiles</t>
+  </si>
+  <si>
+    <t>Logic of tile distribution</t>
+  </si>
+  <si>
+    <t>Spent a lt of time finessing the Player() superclass, and the individual tiles to print the Human and Computer tileRack.
+Working to realise the GamePlay class should be abstracted from this, and only be concerned with calling fucntions to read wordlist, put valid words on the board, tot up score, and remove tiles from the board. This will be the focus of my next work in the coming days.</t>
+  </si>
+  <si>
+    <t>After stepping away from computer for a bit, I came back to realise i had just created the biggest bug in the entire game. For some reason, i had transposed the keyxalue pairs from the data on the breif. so in stead of 8 x [A1], it was showing 1 x [A8] - 1 tile of A8 worth 8 points ! his was the reason why everything was printing wrong, and i was going down such a rabbit whole not realising this.
+Could not believe this how a critical error, so crucial to the game could be missed. I realise this is where the benefit of working in teams or in pairs helps. Sometimes one's eyes just do not spot the most glaringly obvious of bugs.</t>
+  </si>
+  <si>
+    <t>Critical bug fix</t>
+  </si>
+  <si>
+    <t>Key-value pairs transposed. Step Back Away from the computer !</t>
+  </si>
+  <si>
+    <t>Begin logic for user to enter tiles</t>
+  </si>
+  <si>
+    <t>Work on logic for user to enter tiles</t>
+  </si>
+  <si>
+    <t>Onwards and upwards</t>
+  </si>
+  <si>
+    <t>enterWordAndTile()</t>
+  </si>
+  <si>
+    <t>Fixing logic using while loop to continuously prompt user, if they do not enter the correct format. - ine.m word, letter (or _) and up to two numbers.</t>
+  </si>
+  <si>
+    <t>trying out different loops and string formatting techniques</t>
+  </si>
+  <si>
+    <t>Testing validation against wordlist.txt</t>
+  </si>
+  <si>
+    <t>enterwordAndile() method Now verifes if first part of user string (the word), is in the directory. Although a lot of unit testing is needed.</t>
+  </si>
+  <si>
+    <t>GamePlay() and BoardUnit(0 - working to set element to board</t>
+  </si>
+  <si>
+    <t>Pedal to the metal.</t>
+  </si>
+  <si>
+    <t>With 8 days remaining, the effort to really push out a working version (at the cost of rigourous testing) is becoming apparent. A deep learning curve does not tie in the the luxury of having enough time. Hence, the 'brute force' approach to trying everything and seeing - throwing mud at the wall and see if it sticks, then commit/push, or roll back.
+I now see the benefit of systemic test-driven development. But at this stage, it's a case of getting it to work, just to show I do understand how to implement this - even if in a very rudimental way, THEN looking at testing or optimizing code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spent today working on the GamePlay 
+class and a created a new gameInPlay()
+method that handles all in-game logic 
+(human player move, validate, score, 
+computer move, validate, score, etc). 
+Code looking very ‘spaghetti-like’’ at 
+the moment, but is something I 
+understand and can clean up later.
+Lots of // TODO comments as I’m just 
+fleshing out logic Within the GameInPlay class.
+Also lots of roll backs ‘reset current branch to main’, as tried and things tested are thrown away. All in all, getting better at using git. If I get this working, will be a major jump in progress.
+  </t>
+  </si>
+  <si>
+    <t>GamePlay() gameInPlay() - Overall game logic</t>
+  </si>
+  <si>
+    <t>Working on the 'Meat and Veg' - Fleshing out the game.</t>
+  </si>
+  <si>
     <t>public void eatSleepCodeRepeat() {
     boolean notFinished = true;
     while (notFinished) {
         if (SkraBBKleGame() == notfinished) {
-            panic();
+            panic();  // Check if currentDay &lt;= CW_DEADLINE_22_MARCH
             eat();
             sleep();
             code();
@@ -175,61 +252,16 @@
 }</t>
   </si>
   <si>
-    <t>Work on human and computer tiles</t>
-  </si>
-  <si>
-    <t>More work on human and computer tiles</t>
-  </si>
-  <si>
-    <t>Logic of tile distribution</t>
-  </si>
-  <si>
-    <t>Spent a lt of time finessing the Player() superclass, and the individual tiles to print the Human and Computer tileRack.
-Working to realise the GamePlay class should be abstracted from this, and only be concerned with calling fucntions to read wordlist, put valid words on the board, tot up score, and remove tiles from the board. This will be the focus of my next work in the coming days.</t>
-  </si>
-  <si>
-    <t>After stepping away from computer for a bit, I came back to realise i had just created the biggest bug in the entire game. For some reason, i had transposed the keyxalue pairs from the data on the breif. so in stead of 8 x [A1], it was showing 1 x [A8] - 1 tile of A8 worth 8 points ! his was the reason why everything was printing wrong, and i was going down such a rabbit whole not realising this.
-Could not believe this how a critical error, so crucial to the game could be missed. I realise this is where the benefit of working in teams or in pairs helps. Sometimes one's eyes just do not spot the most glaringly obvious of bugs.</t>
-  </si>
-  <si>
-    <t>Critical bug fix</t>
-  </si>
-  <si>
-    <t>Key-value pairs transposed. Step Back Away from the computer !</t>
-  </si>
-  <si>
-    <t>Begin logic for user to enter tiles</t>
-  </si>
-  <si>
-    <t>Work on logic for user to enter tiles</t>
-  </si>
-  <si>
-    <t>Onwards and upwards</t>
-  </si>
-  <si>
-    <t>enterWordAndTile()</t>
-  </si>
-  <si>
-    <t>Fixing logic using while loop to continuously prompt user, if they do not enter the correct format. - ine.m word, letter (or _) and up to two numbers.</t>
-  </si>
-  <si>
-    <t>trying out different loops and string formatting techniques</t>
-  </si>
-  <si>
-    <t>Testing validation against wordlist.txt</t>
-  </si>
-  <si>
-    <t>enterwordAndile() method Now verifes if first part of user string (the word), is in the directory. Although a lot of unit testing is needed.</t>
-  </si>
-  <si>
-    <t>GamePlay() and BoardUnit(0 - working to set element to board</t>
-  </si>
-  <si>
-    <t>Pedal to the metal.</t>
-  </si>
-  <si>
-    <t>With 8 days remaining, the effort to really push out a working version (at the cost of rigourous testing) is becoming apparent. A deep learning curve does not tie in the the luxury of having enough time. Hence, the 'brute force' approach to trying everything and seeing - throwing mud at the wall and see if it sticks, then commit/push, or roll back.
-I now see the benefit of systemic test-driven development. But at this stage, it's a case of getting it to work, just to show I do understand how to implement this - even if in a very rudimental way, THEN looking at testing or optimizing code.</t>
+    <t>Resolve Circular Dependency between BoardInit and GamePlay</t>
+  </si>
+  <si>
+    <t>Logic is king.</t>
+  </si>
+  <si>
+    <t>Removed GamePlay instance as a member of BoardInit class, as GamePlay class also had a BoardInit instrance - creating a circular dependency.
+Starting to realise,  it’s not about coding, it’s about logic and game flow. You can copy code blocks (methods), move them around how you like, pass parameters into them and be very dynamic, but if the game flow is wrong (i.e., if you have tile methods in a BoardInit class) you can get lost in your code and get very messy very quickly.
+I realise it would have been less headach (before I even wrote one line of code) if I’d just written down the entire game flow on a piece of paper as a flow chart diagram.  Now I see the benefit of creating a flowchart before diving into coding.
+End of another tired day. Time for some rest/recuperation, watch a movie. Then dive into more coding afresh tomorrow morning.</t>
   </si>
 </sst>
 </file>
@@ -240,7 +272,7 @@
     <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
     <numFmt numFmtId="165" formatCode="&quot;Overdue&quot;;&quot;&quot;;&quot;&quot;"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.24994659260841701"/>
@@ -363,6 +395,12 @@
       <sz val="15"/>
       <color theme="3" tint="-0.24994659260841701"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="3" tint="-0.24994659260841701"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -531,7 +569,7 @@
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -585,6 +623,12 @@
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2788,6 +2832,62 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3521028</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4772071" cy="2667000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1C1EAC0-C056-8D40-B376-1E883A64AA99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9070928" y="2095500"/>
+          <a:ext cx="4772071" cy="2667000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3058,10 +3158,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3076,32 +3176,32 @@
     <col min="8" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="37" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="37" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="23" t="str">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="25" t="str">
         <f ca="1">'Target '!A2-'Target '!A1&amp;" days remaining"</f>
-        <v>-8 days remaining</v>
-      </c>
-      <c r="G1" s="24"/>
+        <v>-6 days remaining</v>
+      </c>
+      <c r="G1" s="26"/>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="22"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="7" t="s">
         <v>0</v>
@@ -3122,285 +3222,324 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
-        <v>45365</v>
+        <v>45367</v>
       </c>
       <c r="C4" s="13">
-        <v>2.1527777777777778E-2</v>
+        <v>7.0833333333333331E-2</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>45</v>
+        <v>50</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>51</v>
       </c>
       <c r="G4" s="15">
-        <v>0.6</v>
-      </c>
+        <v>0.64</v>
+      </c>
+      <c r="I4" s="18"/>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="9">
-        <v>45364</v>
+        <v>45366</v>
       </c>
       <c r="C5" s="13">
-        <v>0.35138888888888886</v>
+        <v>0.98611111111111116</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>42</v>
+        <v>47</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>45</v>
       </c>
       <c r="G5" s="15">
-        <v>0.57999999999999996</v>
+        <v>0.63</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
+        <v>45365</v>
+      </c>
+      <c r="C6" s="13">
+        <v>2.1527777777777778E-2</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="15">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="9">
         <v>45364</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C7" s="13">
+        <v>0.35138888888888886</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="15">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="9">
+        <v>45364</v>
+      </c>
+      <c r="C8" s="13">
         <v>0.22708333333333333</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D8" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="15">
+      <c r="G8" s="15">
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="9">
+    <row r="9" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="9">
         <v>45363</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C9" s="13">
         <v>0.56666666666666665</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D9" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="15">
+      <c r="F9" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="15">
         <v>0.54</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="9">
-        <v>45361</v>
-      </c>
-      <c r="C8" s="13">
-        <v>0.95208333333333328</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="15">
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="9">
-        <v>45361</v>
-      </c>
-      <c r="C9" s="13">
-        <v>0.84236111111111112</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="15">
-        <v>0.51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="9">
         <v>45361</v>
       </c>
       <c r="C10" s="13">
-        <v>0.58819444444444446</v>
+        <v>0.95208333333333328</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G10" s="15">
-        <v>0.48</v>
+        <v>0.52</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9">
         <v>45361</v>
       </c>
       <c r="C11" s="13">
-        <v>0.15625</v>
+        <v>0.84236111111111112</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="G11" s="15">
-        <v>0.46</v>
+        <v>0.51</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="9">
         <v>45361</v>
       </c>
       <c r="C12" s="13">
+        <v>0.58819444444444446</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="15">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="9">
+        <v>45361</v>
+      </c>
+      <c r="C13" s="13">
+        <v>0.15625</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="15">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="9">
+        <v>45361</v>
+      </c>
+      <c r="C14" s="13">
         <v>9.7222222222222224E-3</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D14" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E14" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F14" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G14" s="15">
         <v>0.42</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="9">
+    <row r="15" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="9">
         <v>45360</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C15" s="13">
         <v>0.27291666666666664</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D15" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E15" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F15" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G15" s="15">
         <v>0.37</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="9">
+    <row r="16" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="9">
         <v>45360</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C16" s="13">
         <v>0.21458333333333332</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D16" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F16" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G16" s="15">
         <v>0.34</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="9">
+    <row r="17" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="9">
         <v>45359</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C17" s="10">
         <v>20.32</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D17" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E17" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F17" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G17" s="15">
         <v>0.32</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="9">
+    <row r="18" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="9">
         <v>45357</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C18" s="10">
         <v>13.26</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D18" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E18" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F18" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G18" s="15">
         <v>0.22</v>
       </c>
     </row>
-    <row r="17" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="18" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="19" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="20" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="19" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="20" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:F16">
+  <conditionalFormatting sqref="B4:F18">
     <cfRule type="expression" dxfId="0" priority="12">
       <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G16">
+  <conditionalFormatting sqref="G4:G18">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -3437,7 +3576,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G16</xm:sqref>
+          <xm:sqref>G4:G18</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3468,7 +3607,7 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45365</v>
+        <v>45367</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
BoardInit() Improve game flow to BoardInit and GamePlay() class.
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283EBDB4-ED11-6445-931E-7B305CC125F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB7C540-8E93-F449-B441-A0E5E236A9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="32000" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dev Log" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>DATE</t>
   </si>
@@ -262,6 +262,18 @@
 Starting to realise,  it’s not about coding, it’s about logic and game flow. You can copy code blocks (methods), move them around how you like, pass parameters into them and be very dynamic, but if the game flow is wrong (i.e., if you have tile methods in a BoardInit class) you can get lost in your code and get very messy very quickly.
 I realise it would have been less headach (before I even wrote one line of code) if I’d just written down the entire game flow on a piece of paper as a flow chart diagram.  Now I see the benefit of creating a flowchart before diving into coding.
 End of another tired day. Time for some rest/recuperation, watch a movie. Then dive into more coding afresh tomorrow morning.</t>
+  </si>
+  <si>
+    <t>Too much time trying things out</t>
+  </si>
+  <si>
+    <t>Spent a lot of time getting too intricate in calculating board size …. Trying to figure out wehat happens if a user places a seven-letter wod on 15P (bottom right) of the defauly board). Got lost and ended up doing some weird branches, trying things out.  Did a lot of reading Java books and studying youtube, also took time. But ultimately, jumped in and played about. i.e., should i use abstract classes? abstract methods? should the Human control the board, or the game play instance? etc.
+Eventually had to roll back to main HEAD and lost a lot of time 'experimenting'.
+Now concentratying on overall game flow of modular methods. (Load board, choose option, take turn, etc.
+Good thing is - although i spent a lot of time, the additional study and jumping in and playing about, taught me a lot.</t>
+  </si>
+  <si>
+    <t>GamePlay()</t>
   </si>
 </sst>
 </file>
@@ -667,7 +679,14 @@
     <cellStyle name="Phone" xfId="8" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Title" xfId="7" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -747,10 +766,10 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Library Book Checkout Sheet" defaultPivotStyle="PivotStyleMedium9">
     <tableStyle name="Library Book Checkout Sheet" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="4"/>
-      <tableStyleElement type="headerRow" dxfId="3"/>
-      <tableStyleElement type="firstColumn" dxfId="2"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="1"/>
+      <tableStyleElement type="wholeTable" dxfId="5"/>
+      <tableStyleElement type="headerRow" dxfId="4"/>
+      <tableStyleElement type="firstColumn" dxfId="3"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="2"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2836,7 +2855,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>3521028</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4772071" cy="2667000"/>
@@ -3158,10 +3177,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3186,7 +3205,7 @@
       <c r="E1" s="21"/>
       <c r="F1" s="25" t="str">
         <f ca="1">'Target '!A2-'Target '!A1&amp;" days remaining"</f>
-        <v>-6 days remaining</v>
+        <v>-5 days remaining</v>
       </c>
       <c r="G1" s="26"/>
     </row>
@@ -3222,88 +3241,89 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="C4" s="13">
-        <v>7.0833333333333331E-2</v>
+        <v>0.44027777777777777</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G4" s="15">
-        <v>0.64</v>
-      </c>
-      <c r="I4" s="18"/>
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="9">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="C5" s="13">
-        <v>0.98611111111111116</v>
+        <v>7.0833333333333331E-2</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G5" s="15">
-        <v>0.63</v>
-      </c>
+        <v>0.64</v>
+      </c>
+      <c r="I5" s="18"/>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
+        <v>45366</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="15">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="1"/>
+      <c r="B7" s="9">
         <v>45365</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C7" s="13">
         <v>2.1527777777777778E-2</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D7" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F7" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G7" s="15">
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="9">
-        <v>45364</v>
-      </c>
-      <c r="C7" s="13">
-        <v>0.35138888888888886</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="15">
-        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3311,59 +3331,59 @@
         <v>45364</v>
       </c>
       <c r="C8" s="13">
-        <v>0.22708333333333333</v>
+        <v>0.35138888888888886</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>37</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G8" s="15">
-        <v>0.56000000000000005</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="9">
-        <v>45363</v>
+        <v>45364</v>
       </c>
       <c r="C9" s="13">
-        <v>0.56666666666666665</v>
+        <v>0.22708333333333333</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G9" s="15">
-        <v>0.54</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="9">
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="C10" s="13">
-        <v>0.95208333333333328</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G10" s="15">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3371,19 +3391,19 @@
         <v>45361</v>
       </c>
       <c r="C11" s="13">
-        <v>0.84236111111111112</v>
+        <v>0.95208333333333328</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G11" s="15">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3391,19 +3411,19 @@
         <v>45361</v>
       </c>
       <c r="C12" s="13">
-        <v>0.58819444444444446</v>
+        <v>0.84236111111111112</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="G12" s="15">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3411,19 +3431,19 @@
         <v>45361</v>
       </c>
       <c r="C13" s="13">
-        <v>0.15625</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G13" s="15">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3431,39 +3451,39 @@
         <v>45361</v>
       </c>
       <c r="C14" s="13">
-        <v>9.7222222222222224E-3</v>
+        <v>0.15625</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="G14" s="15">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="9">
-        <v>45360</v>
+        <v>45361</v>
       </c>
       <c r="C15" s="13">
-        <v>0.27291666666666664</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="G15" s="15">
-        <v>0.37</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3471,76 +3491,96 @@
         <v>45360</v>
       </c>
       <c r="C16" s="13">
-        <v>0.21458333333333332</v>
+        <v>0.27291666666666664</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G16" s="15">
-        <v>0.34</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="9">
-        <v>45359</v>
-      </c>
-      <c r="C17" s="10">
-        <v>20.32</v>
+        <v>45360</v>
+      </c>
+      <c r="C17" s="13">
+        <v>0.21458333333333332</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G17" s="15">
-        <v>0.32</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="9">
+        <v>45359</v>
+      </c>
+      <c r="C18" s="10">
+        <v>20.32</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="15">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="9">
         <v>45357</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C19" s="10">
         <v>13.26</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D19" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E19" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F19" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="15">
+      <c r="G19" s="15">
         <v>0.22</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="20" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="21" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:F18">
-    <cfRule type="expression" dxfId="0" priority="12">
-      <formula>$A4=1</formula>
+  <conditionalFormatting sqref="B5:F19">
+    <cfRule type="expression" dxfId="1" priority="13">
+      <formula>$A5=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G18">
-    <cfRule type="dataBar" priority="1">
+  <conditionalFormatting sqref="G4:G19">
+    <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3551,6 +3591,11 @@
           <x14:id>{272DF8F1-2D7A-C948-BB97-5E4DFA143735}</x14:id>
         </ext>
       </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:F4">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
@@ -3576,7 +3621,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G18</xm:sqref>
+          <xm:sqref>G4:G19</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3607,7 +3652,7 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45367</v>
+        <v>45368</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
@@ -3619,6 +3664,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3918,15 +3972,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3948,6 +3993,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1101C2D-3F57-4FE3-804B-005C212162D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3968,14 +4021,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
GamePlay() Major Refactor. Move isOpenGame() method from BoardInit to GamePlay class (this method is concerned with the type of game, not the board).  Flesh out game logic. Map out am 'isGameFinished() and endGame() scenario.
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB7C540-8E93-F449-B441-A0E5E236A9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC01306A-385C-6A45-8137-3D4D747FAA0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>DATE</t>
   </si>
@@ -274,6 +274,28 @@
   </si>
   <si>
     <t>GamePlay()</t>
+  </si>
+  <si>
+    <t>Lego</t>
+  </si>
+  <si>
+    <t>GamePlay() - Fleshed out game logic. Moved open/closed game option to the GamePlay class.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Things finally starting to piece together -
+like lego bricks. The code blocks (methods)
+I have written are really proving to be
+higlhy modular. easy to chop and change 
+and piece together, and I am really starting
+to understand the benefits and flexibility
+of object orientated programming.
+Moved isOpenGame() method from BoardInit 
+to GamePlay class (this method is concerned 
+with the type of game, not the board).
+Mapped out the gameInPlay logic.
+I also mapped out a 'isGameFinished()
+and endGame() scenario which i just need to flesh out with code. Again, what i've learnt is... build the overall blocks/structure, and the detail (code) will follow. With only 5 days remaining, I believe have about a third of work to go.
+</t>
   </si>
 </sst>
 </file>
@@ -581,7 +603,7 @@
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -641,6 +663,12 @@
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="12" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2855,7 +2883,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>3521028</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4772071" cy="2667000"/>
@@ -2907,6 +2935,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4025900</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>8229600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>3203575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D5C1976-2904-E894-313B-B7363BF89BAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9575800" y="2108200"/>
+          <a:ext cx="4203700" cy="3152775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3177,10 +3249,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3197,28 +3269,28 @@
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="37" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="25" t="str">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="27" t="str">
         <f ca="1">'Target '!A2-'Target '!A1&amp;" days remaining"</f>
         <v>-5 days remaining</v>
       </c>
-      <c r="G1" s="26"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="26"/>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
@@ -3241,109 +3313,110 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
         <v>45368</v>
       </c>
       <c r="C4" s="13">
-        <v>0.44027777777777777</v>
+        <v>0.79374999999999996</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>53</v>
+        <v>56</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="G4" s="15">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="9">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="C5" s="13">
-        <v>7.0833333333333331E-2</v>
+        <v>0.44027777777777777</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G5" s="15">
-        <v>0.64</v>
-      </c>
-      <c r="I5" s="18"/>
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="C6" s="13">
-        <v>0.98611111111111116</v>
+        <v>7.0833333333333331E-2</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G6" s="15">
-        <v>0.63</v>
-      </c>
+        <v>0.64</v>
+      </c>
+      <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="9">
+        <v>45366</v>
+      </c>
+      <c r="C7" s="13">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="15">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="1"/>
+      <c r="B8" s="9">
         <v>45365</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C8" s="13">
         <v>2.1527777777777778E-2</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D8" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E8" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F8" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G8" s="15">
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="9">
-        <v>45364</v>
-      </c>
-      <c r="C8" s="13">
-        <v>0.35138888888888886</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="15">
-        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3351,59 +3424,59 @@
         <v>45364</v>
       </c>
       <c r="C9" s="13">
-        <v>0.22708333333333333</v>
+        <v>0.35138888888888886</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>37</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G9" s="15">
-        <v>0.56000000000000005</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="9">
-        <v>45363</v>
+        <v>45364</v>
       </c>
       <c r="C10" s="13">
-        <v>0.56666666666666665</v>
+        <v>0.22708333333333333</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G10" s="15">
-        <v>0.54</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9">
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="C11" s="13">
-        <v>0.95208333333333328</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G11" s="15">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3411,19 +3484,19 @@
         <v>45361</v>
       </c>
       <c r="C12" s="13">
-        <v>0.84236111111111112</v>
+        <v>0.95208333333333328</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G12" s="15">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3431,19 +3504,19 @@
         <v>45361</v>
       </c>
       <c r="C13" s="13">
-        <v>0.58819444444444446</v>
+        <v>0.84236111111111112</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="G13" s="15">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3451,19 +3524,19 @@
         <v>45361</v>
       </c>
       <c r="C14" s="13">
-        <v>0.15625</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G14" s="15">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3471,39 +3544,39 @@
         <v>45361</v>
       </c>
       <c r="C15" s="13">
-        <v>9.7222222222222224E-3</v>
+        <v>0.15625</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="G15" s="15">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="9">
-        <v>45360</v>
+        <v>45361</v>
       </c>
       <c r="C16" s="13">
-        <v>0.27291666666666664</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="G16" s="15">
-        <v>0.37</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3511,76 +3584,101 @@
         <v>45360</v>
       </c>
       <c r="C17" s="13">
-        <v>0.21458333333333332</v>
+        <v>0.27291666666666664</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G17" s="15">
-        <v>0.34</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="9">
-        <v>45359</v>
-      </c>
-      <c r="C18" s="10">
-        <v>20.32</v>
+        <v>45360</v>
+      </c>
+      <c r="C18" s="13">
+        <v>0.21458333333333332</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G18" s="15">
-        <v>0.32</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="9">
+        <v>45359</v>
+      </c>
+      <c r="C19" s="10">
+        <v>20.32</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="15">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="9">
         <v>45357</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C20" s="10">
         <v>13.26</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D20" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E20" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F20" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="15">
+      <c r="G20" s="15">
         <v>0.22</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="21" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="22" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B5:F19">
-    <cfRule type="expression" dxfId="1" priority="13">
+  <conditionalFormatting sqref="B4:E4">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$A4=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:F20">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$A5=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G19">
-    <cfRule type="dataBar" priority="2">
+  <conditionalFormatting sqref="G4:G20">
+    <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3591,11 +3689,6 @@
           <x14:id>{272DF8F1-2D7A-C948-BB97-5E4DFA143735}</x14:id>
         </ext>
       </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4:F4">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
@@ -3621,7 +3714,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G19</xm:sqref>
+          <xm:sqref>G4:G20</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3664,15 +3757,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3972,6 +4056,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3993,14 +4086,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1101C2D-3F57-4FE3-804B-005C212162D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4021,6 +4106,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
GamePlay() Minor edits, trying things out, such as the takeTurn() method.Work in progress...
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC01306A-385C-6A45-8137-3D4D747FAA0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDC7DB9-E45E-D944-91FF-F3F8A680E441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>DATE</t>
   </si>
@@ -297,14 +297,35 @@
 and endGame() scenario which i just need to flesh out with code. Again, what i've learnt is... build the overall blocks/structure, and the detail (code) will follow. With only 5 days remaining, I believe have about a third of work to go.
 </t>
   </si>
+  <si>
+    <t>A lot of work, for very little progress</t>
+  </si>
+  <si>
+    <t>GamePlay() - fixed bug in isGame() method.</t>
+  </si>
+  <si>
+    <t>Fixed what was a small bug with isGame method, which newly occurred when the method was introduced to GamePlay class from BoardInit. 
+Spent  3 or four hours fixing this, and other little things. Although it seems not a lot of progress was made, the code does seeom more streamlined, and all seems to work as per the brief.</t>
+  </si>
+  <si>
+    <t>Still trying to figure out takeTurn() method in GamePlay class. Not as much progress maid as I'd have like. The flow and logic is in my head, but the skills, syntax and programming skills of how to implement it is not quite there just yet. Watching lots of Youtube videos, helps, as does Stack OverFlow. bug detecting i'm getting good at, and the scarey red text screaming NullPointerExceptions no longer scares me.
+Been coding for over 12 hours on and today. Probably better call it a day and pick this up afresh tomorrow morning.</t>
+  </si>
+  <si>
+    <t>GamePlay() - takTurn() method. Implementing human moves..</t>
+  </si>
+  <si>
+    <t>Still trying to get to grips with it</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
     <numFmt numFmtId="165" formatCode="&quot;Overdue&quot;;&quot;&quot;;&quot;&quot;"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -603,7 +624,7 @@
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -670,6 +691,12 @@
     <xf numFmtId="20" fontId="12" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="3" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -691,6 +718,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="3" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="6" builtinId="3" customBuiltin="1"/>
@@ -707,7 +737,14 @@
     <cellStyle name="Phone" xfId="8" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Title" xfId="7" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -794,10 +831,10 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Library Book Checkout Sheet" defaultPivotStyle="PivotStyleMedium9">
     <tableStyle name="Library Book Checkout Sheet" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="5"/>
-      <tableStyleElement type="headerRow" dxfId="4"/>
-      <tableStyleElement type="firstColumn" dxfId="3"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="2"/>
+      <tableStyleElement type="wholeTable" dxfId="6"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="firstColumn" dxfId="4"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="3"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2883,7 +2920,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>3521028</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4772071" cy="2667000"/>
@@ -2938,15 +2975,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>4025900</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:colOff>4241800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>403225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8229600</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>3203575</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>3394075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2969,8 +3006,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9575800" y="2108200"/>
-          <a:ext cx="4203700" cy="3152775"/>
+          <a:off x="9791700" y="5838825"/>
+          <a:ext cx="3987800" cy="2990850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3249,10 +3286,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3269,28 +3306,28 @@
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="37" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="27" t="str">
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="29" t="str">
         <f ca="1">'Target '!A2-'Target '!A1&amp;" days remaining"</f>
-        <v>-5 days remaining</v>
-      </c>
-      <c r="G1" s="28"/>
+        <v>-4 days remaining</v>
+      </c>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="28"/>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
@@ -3313,210 +3350,212 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="C4" s="13">
-        <v>0.79374999999999996</v>
+        <v>5.8333333333333334E-2</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="G4" s="15">
-        <v>0.67</v>
+        <v>63</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="31">
+        <v>0.69</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="9">
         <v>45368</v>
       </c>
       <c r="C5" s="13">
-        <v>0.44027777777777777</v>
+        <v>0.96458333333333335</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="15">
-        <v>0.65</v>
+        <v>59</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="22">
+        <v>0.68500000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="C6" s="13">
-        <v>7.0833333333333331E-2</v>
+        <v>0.79374999999999996</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>51</v>
+        <v>56</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="G6" s="15">
-        <v>0.64</v>
-      </c>
-      <c r="I6" s="18"/>
+        <v>0.67</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="9">
-        <v>45366</v>
+        <v>45368</v>
       </c>
       <c r="C7" s="13">
-        <v>0.98611111111111116</v>
+        <v>0.44027777777777777</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G7" s="15">
-        <v>0.63</v>
+        <v>0.65</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="9">
+        <v>45367</v>
+      </c>
+      <c r="C8" s="13">
+        <v>7.0833333333333331E-2</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="15">
+        <v>0.64</v>
+      </c>
+      <c r="I8" s="18"/>
+    </row>
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="1"/>
+      <c r="B9" s="9">
+        <v>45366</v>
+      </c>
+      <c r="C9" s="13">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="15">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="1"/>
+      <c r="B10" s="9">
         <v>45365</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C10" s="13">
         <v>2.1527777777777778E-2</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D10" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E10" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F10" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G10" s="15">
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="9">
-        <v>45364</v>
-      </c>
-      <c r="C9" s="13">
-        <v>0.35138888888888886</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="15">
-        <v>0.57999999999999996</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="9">
-        <v>45364</v>
-      </c>
-      <c r="C10" s="13">
-        <v>0.22708333333333333</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="15">
-        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9">
-        <v>45363</v>
+        <v>45364</v>
       </c>
       <c r="C11" s="13">
-        <v>0.56666666666666665</v>
+        <v>0.35138888888888886</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="G11" s="15">
-        <v>0.54</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="9">
-        <v>45361</v>
+        <v>45364</v>
       </c>
       <c r="C12" s="13">
-        <v>0.95208333333333328</v>
+        <v>0.22708333333333333</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G12" s="15">
-        <v>0.52</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="9">
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="C13" s="13">
-        <v>0.84236111111111112</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G13" s="15">
-        <v>0.51</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3524,19 +3563,19 @@
         <v>45361</v>
       </c>
       <c r="C14" s="13">
-        <v>0.58819444444444446</v>
+        <v>0.95208333333333328</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="G14" s="15">
-        <v>0.48</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3544,19 +3583,19 @@
         <v>45361</v>
       </c>
       <c r="C15" s="13">
-        <v>0.15625</v>
+        <v>0.84236111111111112</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="G15" s="15">
-        <v>0.46</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3564,121 +3603,161 @@
         <v>45361</v>
       </c>
       <c r="C16" s="13">
-        <v>9.7222222222222224E-3</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>17</v>
+        <v>27</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="G16" s="15">
-        <v>0.42</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="9">
-        <v>45360</v>
+        <v>45361</v>
       </c>
       <c r="C17" s="13">
-        <v>0.27291666666666664</v>
+        <v>0.15625</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>14</v>
+        <v>21</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>20</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G17" s="15">
-        <v>0.37</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="9">
-        <v>45360</v>
+        <v>45361</v>
       </c>
       <c r="C18" s="13">
-        <v>0.21458333333333332</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>12</v>
+        <v>19</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="G18" s="15">
-        <v>0.34</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="9">
-        <v>45359</v>
-      </c>
-      <c r="C19" s="10">
-        <v>20.32</v>
+        <v>45360</v>
+      </c>
+      <c r="C19" s="13">
+        <v>0.27291666666666664</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G19" s="15">
-        <v>0.32</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="9">
+        <v>45360</v>
+      </c>
+      <c r="C20" s="13">
+        <v>0.21458333333333332</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="15">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="9">
+        <v>45359</v>
+      </c>
+      <c r="C21" s="10">
+        <v>20.32</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="15">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="9">
         <v>45357</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C22" s="10">
         <v>13.26</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D22" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F22" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="15">
+      <c r="G22" s="15">
         <v>0.22</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="22" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="23" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="24" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:E4">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>$A4=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B5:F20">
-    <cfRule type="expression" dxfId="0" priority="2">
+  <conditionalFormatting sqref="B5:E6">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$A5=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G20">
-    <cfRule type="dataBar" priority="3">
+  <conditionalFormatting sqref="B7:F22">
+    <cfRule type="expression" dxfId="1" priority="5">
+      <formula>$A7=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5:G22">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3687,6 +3766,25 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{272DF8F1-2D7A-C948-BB97-5E4DFA143735}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:E4">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$A4=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FF00B050"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{7ED22953-26CA-4C4F-B423-42A85429F05B}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3714,7 +3812,22 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G20</xm:sqref>
+          <xm:sqref>G5:G22</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{7ED22953-26CA-4C4F-B423-42A85429F05B}">
+            <x14:dataBar minLength="0" maxLength="100">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G4</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3745,7 +3858,7 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45368</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
@@ -3757,6 +3870,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4056,7 +4189,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4065,27 +4198,19 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1101C2D-3F57-4FE3-804B-005C212162D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4106,7 +4231,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -4114,18 +4239,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
WordValidator() : Create new WordValidator() class to handle the validation of Player inputted word, and direction (in relation to board size).
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDC7DB9-E45E-D944-91FF-F3F8A680E441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B045BEA4-E34B-B144-82A6-C44BF7339C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <t>DATE</t>
   </si>
@@ -316,6 +316,16 @@
   </si>
   <si>
     <t>Still trying to get to grips with it</t>
+  </si>
+  <si>
+    <t>Lack of sleep, and dreaming of camelCases spurned me to wake up and work on the project. Introduced a new WordValidator class which handles all the functions of validating the user input. This has the effect of making the GamePlay class much cleaner and less cluttered.
+Not sure how i'm going to implement the computerPlayer's move yet but we'll cross that bridge when we get to it.  If I can get this working, I shall be in a really good place.</t>
+  </si>
+  <si>
+    <t>Introduce WordValidator() class</t>
+  </si>
+  <si>
+    <t>More complex (word validation), but cleaner GamePlay class</t>
   </si>
 </sst>
 </file>
@@ -624,7 +634,7 @@
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -717,9 +727,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="3" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -2920,7 +2927,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>3521028</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4772071" cy="2667000"/>
@@ -2976,13 +2983,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>4241800</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>403225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8229600</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>3394075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3286,7 +3293,7 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
@@ -3350,172 +3357,173 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
         <v>45369</v>
       </c>
       <c r="C4" s="13">
-        <v>5.8333333333333334E-2</v>
+        <v>0.22291666666666668</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" s="31">
-        <v>0.69</v>
+        <v>64</v>
+      </c>
+      <c r="G4" s="15">
+        <v>0.7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="9">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="C5" s="13">
-        <v>0.96458333333333335</v>
+        <v>5.8333333333333334E-2</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="22">
-        <v>0.68500000000000005</v>
+        <v>61</v>
+      </c>
+      <c r="G5" s="15">
+        <v>0.69</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
         <v>45368</v>
       </c>
       <c r="C6" s="13">
-        <v>0.79374999999999996</v>
+        <v>0.96458333333333335</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="G6" s="15">
-        <v>0.67</v>
+        <v>58</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="22">
+        <v>0.68500000000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="9">
         <v>45368</v>
       </c>
       <c r="C7" s="13">
-        <v>0.44027777777777777</v>
+        <v>0.79374999999999996</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>53</v>
+        <v>56</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="G7" s="15">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="9">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="C8" s="13">
-        <v>7.0833333333333331E-2</v>
+        <v>0.44027777777777777</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G8" s="15">
-        <v>0.64</v>
-      </c>
-      <c r="I8" s="18"/>
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="9">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="C9" s="13">
-        <v>0.98611111111111116</v>
+        <v>7.0833333333333331E-2</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G9" s="15">
-        <v>0.63</v>
-      </c>
+        <v>0.64</v>
+      </c>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="9">
+        <v>45366</v>
+      </c>
+      <c r="C10" s="13">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="15">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="1"/>
+      <c r="B11" s="9">
         <v>45365</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C11" s="13">
         <v>2.1527777777777778E-2</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D11" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E11" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F11" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G11" s="15">
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="9">
-        <v>45364</v>
-      </c>
-      <c r="C11" s="13">
-        <v>0.35138888888888886</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="15">
-        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3523,59 +3531,59 @@
         <v>45364</v>
       </c>
       <c r="C12" s="13">
-        <v>0.22708333333333333</v>
+        <v>0.35138888888888886</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>37</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G12" s="15">
-        <v>0.56000000000000005</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="9">
-        <v>45363</v>
+        <v>45364</v>
       </c>
       <c r="C13" s="13">
-        <v>0.56666666666666665</v>
+        <v>0.22708333333333333</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G13" s="15">
-        <v>0.54</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="9">
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="C14" s="13">
-        <v>0.95208333333333328</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G14" s="15">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3583,19 +3591,19 @@
         <v>45361</v>
       </c>
       <c r="C15" s="13">
-        <v>0.84236111111111112</v>
+        <v>0.95208333333333328</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G15" s="15">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3603,19 +3611,19 @@
         <v>45361</v>
       </c>
       <c r="C16" s="13">
-        <v>0.58819444444444446</v>
+        <v>0.84236111111111112</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="G16" s="15">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3623,19 +3631,19 @@
         <v>45361</v>
       </c>
       <c r="C17" s="13">
-        <v>0.15625</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G17" s="15">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3643,39 +3651,39 @@
         <v>45361</v>
       </c>
       <c r="C18" s="13">
-        <v>9.7222222222222224E-3</v>
+        <v>0.15625</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="G18" s="15">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="9">
-        <v>45360</v>
+        <v>45361</v>
       </c>
       <c r="C19" s="13">
-        <v>0.27291666666666664</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="G19" s="15">
-        <v>0.37</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3683,81 +3691,115 @@
         <v>45360</v>
       </c>
       <c r="C20" s="13">
-        <v>0.21458333333333332</v>
+        <v>0.27291666666666664</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G20" s="15">
-        <v>0.34</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="9">
-        <v>45359</v>
-      </c>
-      <c r="C21" s="10">
-        <v>20.32</v>
+        <v>45360</v>
+      </c>
+      <c r="C21" s="13">
+        <v>0.21458333333333332</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G21" s="15">
-        <v>0.32</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="9">
+        <v>45359</v>
+      </c>
+      <c r="C22" s="10">
+        <v>20.32</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="15">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="9">
         <v>45357</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C23" s="10">
         <v>13.26</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D23" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E23" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F23" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G22" s="15">
+      <c r="G23" s="15">
         <v>0.22</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="24" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="25" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B5:E6">
-    <cfRule type="expression" dxfId="2" priority="3">
+  <conditionalFormatting sqref="B5:E7">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$A5=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:F22">
-    <cfRule type="expression" dxfId="1" priority="5">
-      <formula>$A7=1</formula>
+  <conditionalFormatting sqref="B8:F23">
+    <cfRule type="expression" dxfId="1" priority="6">
+      <formula>$A8=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5:G22">
-    <cfRule type="dataBar" priority="6">
+  <conditionalFormatting sqref="G4:G5">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FF00B050"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{7ED22953-26CA-4C4F-B423-42A85429F05B}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6:G23">
+    <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3775,20 +3817,6 @@
       <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4">
-    <cfRule type="dataBar" priority="2">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FF00B050"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7ED22953-26CA-4C4F-B423-42A85429F05B}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
   <pageSetup scale="75" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -3799,6 +3827,21 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{7ED22953-26CA-4C4F-B423-42A85429F05B}">
+            <x14:dataBar minLength="0" maxLength="100">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G4:G5</xm:sqref>
+        </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{272DF8F1-2D7A-C948-BB97-5E4DFA143735}">
             <x14:dataBar minLength="0" maxLength="100">
@@ -3812,22 +3855,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G5:G22</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7ED22953-26CA-4C4F-B423-42A85429F05B}">
-            <x14:dataBar minLength="0" maxLength="100">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>G4</xm:sqref>
+          <xm:sqref>G6:G23</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3870,23 +3898,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4190,22 +4207,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4232,9 +4256,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
WordValidator() / GamePlay() : "Clean up gameInPlay logic, Work on word validation for human player.
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B045BEA4-E34B-B144-82A6-C44BF7339C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D8774B-233B-3448-BE91-3E76823FD315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
   <si>
     <t>DATE</t>
   </si>
@@ -327,6 +327,12 @@
   <si>
     <t>More complex (word validation), but cleaner GamePlay class</t>
   </si>
+  <si>
+    <t>Cleaned up gameInPlay logic, Just working on word validation for human player.</t>
+  </si>
+  <si>
+    <t>WordValidator() , gamePlay()</t>
+  </si>
 </sst>
 </file>
 
@@ -337,7 +343,7 @@
     <numFmt numFmtId="165" formatCode="&quot;Overdue&quot;;&quot;&quot;;&quot;&quot;"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.24994659260841701"/>
@@ -418,12 +424,6 @@
       <b/>
       <sz val="14"/>
       <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="3" tint="-0.24994659260841701"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -634,7 +634,7 @@
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -647,13 +647,13 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="16" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
@@ -662,34 +662,25 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="12" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="3" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="13" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="12" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="3" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="12" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -698,19 +689,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="20" fontId="12" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="3" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="3" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -722,11 +710,17 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="10" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="10" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -2927,7 +2921,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>3521028</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4772071" cy="2667000"/>
@@ -2983,13 +2977,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>4241800</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>403225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8229600</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>3394075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3293,9 +3287,9 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -3313,28 +3307,28 @@
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="37" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="29" t="str">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="25" t="str">
         <f ca="1">'Target '!A2-'Target '!A1&amp;" days remaining"</f>
         <v>-4 days remaining</v>
       </c>
-      <c r="G1" s="30"/>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="28"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
@@ -3357,435 +3351,456 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
         <v>45369</v>
       </c>
-      <c r="C4" s="13">
-        <v>0.22291666666666668</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="21" t="s">
+      <c r="C4" s="12">
+        <v>0.55277777777777781</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" s="15">
-        <v>0.7</v>
+      <c r="F4" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="13">
+        <v>0.71</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="9">
         <v>45369</v>
       </c>
-      <c r="C5" s="13">
-        <v>5.8333333333333334E-2</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5" s="15">
-        <v>0.69</v>
+      <c r="C5" s="12">
+        <v>0.22291666666666668</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="13">
+        <v>0.7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
-        <v>45368</v>
-      </c>
-      <c r="C6" s="13">
-        <v>0.96458333333333335</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" s="22">
-        <v>0.68500000000000005</v>
+        <v>45369</v>
+      </c>
+      <c r="C6" s="12">
+        <v>5.8333333333333334E-2</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="13">
+        <v>0.69</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="9">
         <v>45368</v>
       </c>
-      <c r="C7" s="13">
-        <v>0.79374999999999996</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="G7" s="15">
-        <v>0.67</v>
+      <c r="C7" s="12">
+        <v>0.96458333333333335</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" s="18">
+        <v>0.68500000000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="9">
         <v>45368</v>
       </c>
-      <c r="C8" s="13">
-        <v>0.44027777777777777</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" s="15">
-        <v>0.65</v>
+      <c r="C8" s="12">
+        <v>0.79374999999999996</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="13">
+        <v>0.67</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="9">
-        <v>45367</v>
-      </c>
-      <c r="C9" s="13">
-        <v>7.0833333333333331E-2</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" s="15">
-        <v>0.64</v>
-      </c>
-      <c r="I9" s="18"/>
+        <v>45368</v>
+      </c>
+      <c r="C9" s="12">
+        <v>0.44027777777777777</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="13">
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="9">
-        <v>45366</v>
-      </c>
-      <c r="C10" s="13">
-        <v>0.98611111111111116</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="15">
-        <v>0.63</v>
-      </c>
+        <v>45367</v>
+      </c>
+      <c r="C10" s="12">
+        <v>7.0833333333333331E-2</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="13">
+        <v>0.64</v>
+      </c>
+      <c r="I10" s="15"/>
     </row>
     <row r="11" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="9">
+        <v>45366</v>
+      </c>
+      <c r="C11" s="12">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="13">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="1"/>
+      <c r="B12" s="9">
         <v>45365</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C12" s="12">
         <v>2.1527777777777778E-2</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D12" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E12" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F12" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G12" s="13">
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="9">
-        <v>45364</v>
-      </c>
-      <c r="C12" s="13">
-        <v>0.35138888888888886</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" s="15">
-        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="9">
         <v>45364</v>
       </c>
-      <c r="C13" s="13">
-        <v>0.22708333333333333</v>
-      </c>
-      <c r="D13" s="16" t="s">
+      <c r="C13" s="12">
+        <v>0.35138888888888886</v>
+      </c>
+      <c r="D13" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="15">
-        <v>0.56000000000000005</v>
+      <c r="E13" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="13">
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="9">
-        <v>45363</v>
-      </c>
-      <c r="C14" s="13">
-        <v>0.56666666666666665</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" s="15">
-        <v>0.54</v>
+        <v>45364</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0.22708333333333333</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="13">
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="9">
-        <v>45361</v>
-      </c>
-      <c r="C15" s="13">
-        <v>0.95208333333333328</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15" s="15">
-        <v>0.52</v>
+        <v>45363</v>
+      </c>
+      <c r="C15" s="12">
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="13">
+        <v>0.54</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="9">
         <v>45361</v>
       </c>
-      <c r="C16" s="13">
-        <v>0.84236111111111112</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" s="15">
-        <v>0.51</v>
+      <c r="C16" s="12">
+        <v>0.95208333333333328</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="13">
+        <v>0.52</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="9">
         <v>45361</v>
       </c>
-      <c r="C17" s="13">
-        <v>0.58819444444444446</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" s="15">
-        <v>0.48</v>
+      <c r="C17" s="12">
+        <v>0.84236111111111112</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="13">
+        <v>0.51</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="9">
         <v>45361</v>
       </c>
-      <c r="C18" s="13">
-        <v>0.15625</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G18" s="15">
-        <v>0.46</v>
+      <c r="C18" s="12">
+        <v>0.58819444444444446</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="13">
+        <v>0.48</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="9">
         <v>45361</v>
       </c>
-      <c r="C19" s="13">
-        <v>9.7222222222222224E-3</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="15">
-        <v>0.42</v>
+      <c r="C19" s="12">
+        <v>0.15625</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="13">
+        <v>0.46</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="9">
-        <v>45360</v>
-      </c>
-      <c r="C20" s="13">
-        <v>0.27291666666666664</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="15">
-        <v>0.37</v>
+        <v>45361</v>
+      </c>
+      <c r="C20" s="12">
+        <v>9.7222222222222224E-3</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="13">
+        <v>0.42</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="9">
         <v>45360</v>
       </c>
-      <c r="C21" s="13">
-        <v>0.21458333333333332</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="15">
-        <v>0.34</v>
+      <c r="C21" s="12">
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="13">
+        <v>0.37</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="9">
-        <v>45359</v>
-      </c>
-      <c r="C22" s="10">
-        <v>20.32</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="15">
-        <v>0.32</v>
+        <v>45360</v>
+      </c>
+      <c r="C22" s="12">
+        <v>0.21458333333333332</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="13">
+        <v>0.34</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="9">
+        <v>45359</v>
+      </c>
+      <c r="C23" s="10">
+        <v>20.32</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="13">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="9">
         <v>45357</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C24" s="10">
         <v>13.26</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D24" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E24" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F24" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G23" s="15">
+      <c r="G24" s="13">
         <v>0.22</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="25" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="26" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B5:E7">
+  <conditionalFormatting sqref="B5:E8">
     <cfRule type="expression" dxfId="2" priority="2">
       <formula>$A5=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8:F23">
-    <cfRule type="expression" dxfId="1" priority="6">
-      <formula>$A8=1</formula>
+  <conditionalFormatting sqref="B9:F24">
+    <cfRule type="expression" dxfId="1" priority="7">
+      <formula>$A9=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G5">
-    <cfRule type="dataBar" priority="3">
+  <conditionalFormatting sqref="G4:G6">
+    <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3798,8 +3813,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:G23">
-    <cfRule type="dataBar" priority="7">
+  <conditionalFormatting sqref="G7:G24">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3840,7 +3855,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G5</xm:sqref>
+          <xm:sqref>G4:G6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{272DF8F1-2D7A-C948-BB97-5E4DFA143735}">
@@ -3855,7 +3870,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G6:G23</xm:sqref>
+          <xm:sqref>G7:G24</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3898,15 +3913,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4206,6 +4212,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4227,14 +4242,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1101C2D-3F57-4FE3-804B-005C212162D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4255,6 +4262,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
WordValidator() : Implement more robost validation checking (for squares).
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D8774B-233B-3448-BE91-3E76823FD315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A583D0-1CD2-6F43-A5AC-DFE658287F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="71">
   <si>
     <t>DATE</t>
   </si>
@@ -332,6 +332,12 @@
   </si>
   <si>
     <t>WordValidator() , gamePlay()</t>
+  </si>
+  <si>
+    <t>More  (word and squaare validation with WordValidator class</t>
+  </si>
+  <si>
+    <t>Implement more robost validation checking (for squares)</t>
   </si>
 </sst>
 </file>
@@ -695,6 +701,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="20" fontId="10" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="10" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -715,12 +727,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="10" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="10" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -2921,7 +2927,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>3521028</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4772071" cy="2667000"/>
@@ -2977,13 +2983,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>4241800</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>403225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8229600</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>3394075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3287,10 +3293,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3307,28 +3313,28 @@
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="37" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="25" t="str">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="27" t="str">
         <f ca="1">'Target '!A2-'Target '!A1&amp;" days remaining"</f>
         <v>-4 days remaining</v>
       </c>
-      <c r="G1" s="26"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="26"/>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
@@ -3351,214 +3357,215 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
         <v>45369</v>
       </c>
       <c r="C4" s="12">
-        <v>0.55277777777777781</v>
-      </c>
-      <c r="D4" s="28" t="s">
+        <v>0.72430555555555554</v>
+      </c>
+      <c r="D4" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="27" t="s">
-        <v>66</v>
+      <c r="E4" s="20" t="s">
+        <v>69</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G4" s="13">
-        <v>0.71</v>
+        <v>0.73</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="9">
         <v>45369</v>
       </c>
       <c r="C5" s="12">
-        <v>0.22291666666666668</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" s="27" t="s">
+        <v>0.55277777777777781</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="20" t="s">
         <v>66</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G5" s="13">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
         <v>45369</v>
       </c>
       <c r="C6" s="12">
-        <v>5.8333333333333334E-2</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>63</v>
+        <v>0.22291666666666668</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>66</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G6" s="13">
-        <v>0.69</v>
+        <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="9">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="C7" s="12">
-        <v>0.96458333333333335</v>
-      </c>
-      <c r="D7" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>58</v>
+        <v>5.8333333333333334E-2</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>63</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="G7" s="18">
-        <v>0.68500000000000005</v>
+        <v>61</v>
+      </c>
+      <c r="G7" s="13">
+        <v>0.69</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="9">
         <v>45368</v>
       </c>
       <c r="C8" s="12">
-        <v>0.79374999999999996</v>
-      </c>
-      <c r="D8" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G8" s="13">
-        <v>0.67</v>
+        <v>0.96458333333333335</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="18">
+        <v>0.68500000000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="9">
         <v>45368</v>
       </c>
       <c r="C9" s="12">
-        <v>0.44027777777777777</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>53</v>
+        <v>0.79374999999999996</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="G9" s="13">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="9">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="C10" s="12">
-        <v>7.0833333333333331E-2</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>50</v>
+        <v>0.44027777777777777</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>52</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G10" s="13">
-        <v>0.64</v>
-      </c>
-      <c r="I10" s="15"/>
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="9">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="C11" s="12">
-        <v>0.98611111111111116</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>47</v>
+        <v>7.0833333333333331E-2</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>50</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G11" s="13">
-        <v>0.63</v>
-      </c>
+        <v>0.64</v>
+      </c>
+      <c r="I11" s="15"/>
     </row>
     <row r="12" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="9">
+        <v>45366</v>
+      </c>
+      <c r="C12" s="12">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="13">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="1"/>
+      <c r="B13" s="9">
         <v>45365</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C13" s="12">
         <v>2.1527777777777778E-2</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D13" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E13" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F13" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G13" s="13">
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="9">
-        <v>45364</v>
-      </c>
-      <c r="C13" s="12">
-        <v>0.35138888888888886</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" s="13">
-        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3566,59 +3573,59 @@
         <v>45364</v>
       </c>
       <c r="C14" s="12">
-        <v>0.22708333333333333</v>
-      </c>
-      <c r="D14" s="28" t="s">
+        <v>0.35138888888888886</v>
+      </c>
+      <c r="D14" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="27" t="s">
-        <v>39</v>
+      <c r="E14" s="20" t="s">
+        <v>40</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G14" s="13">
-        <v>0.56000000000000005</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="9">
-        <v>45363</v>
+        <v>45364</v>
       </c>
       <c r="C15" s="12">
-        <v>0.56666666666666665</v>
-      </c>
-      <c r="D15" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="27" t="s">
-        <v>36</v>
+        <v>0.22708333333333333</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>39</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G15" s="13">
-        <v>0.54</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="9">
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="C16" s="12">
-        <v>0.95208333333333328</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="27" t="s">
-        <v>33</v>
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>36</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G16" s="13">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3626,19 +3633,19 @@
         <v>45361</v>
       </c>
       <c r="C17" s="12">
-        <v>0.84236111111111112</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="27" t="s">
-        <v>29</v>
+        <v>0.95208333333333328</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>33</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G17" s="13">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3646,19 +3653,19 @@
         <v>45361</v>
       </c>
       <c r="C18" s="12">
-        <v>0.58819444444444446</v>
-      </c>
-      <c r="D18" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="27" t="s">
-        <v>26</v>
+        <v>0.84236111111111112</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>29</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="G18" s="13">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3666,19 +3673,19 @@
         <v>45361</v>
       </c>
       <c r="C19" s="12">
-        <v>0.15625</v>
-      </c>
-      <c r="D19" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="27" t="s">
-        <v>20</v>
+        <v>0.58819444444444446</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G19" s="13">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3686,39 +3693,39 @@
         <v>45361</v>
       </c>
       <c r="C20" s="12">
-        <v>9.7222222222222224E-3</v>
-      </c>
-      <c r="D20" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>17</v>
+        <v>0.15625</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="G20" s="13">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="9">
-        <v>45360</v>
+        <v>45361</v>
       </c>
       <c r="C21" s="12">
-        <v>0.27291666666666664</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>16</v>
+        <v>9.7222222222222224E-3</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="G21" s="13">
-        <v>0.37</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3726,81 +3733,101 @@
         <v>45360</v>
       </c>
       <c r="C22" s="12">
-        <v>0.21458333333333332</v>
-      </c>
-      <c r="D22" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="28" t="s">
-        <v>11</v>
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G22" s="13">
-        <v>0.34</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="9">
-        <v>45359</v>
-      </c>
-      <c r="C23" s="10">
-        <v>20.32</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="28" t="s">
-        <v>9</v>
+        <v>45360</v>
+      </c>
+      <c r="C23" s="12">
+        <v>0.21458333333333332</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>11</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G23" s="13">
-        <v>0.32</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="9">
+        <v>45359</v>
+      </c>
+      <c r="C24" s="10">
+        <v>20.32</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="13">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="9">
         <v>45357</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C25" s="10">
         <v>13.26</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="D25" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E24" s="28" t="s">
+      <c r="E25" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F25" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G25" s="13">
         <v>0.22</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="26" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="27" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B5:E8">
+  <conditionalFormatting sqref="B5:E9">
     <cfRule type="expression" dxfId="2" priority="2">
       <formula>$A5=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9:F24">
-    <cfRule type="expression" dxfId="1" priority="7">
-      <formula>$A9=1</formula>
+  <conditionalFormatting sqref="B10:F25">
+    <cfRule type="expression" dxfId="1" priority="8">
+      <formula>$A10=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G6">
-    <cfRule type="dataBar" priority="4">
+  <conditionalFormatting sqref="G4:G7">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3813,8 +3840,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7:G24">
-    <cfRule type="dataBar" priority="8">
+  <conditionalFormatting sqref="G8:G25">
+    <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3855,7 +3882,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G6</xm:sqref>
+          <xm:sqref>G4:G7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{272DF8F1-2D7A-C948-BB97-5E4DFA143735}">
@@ -3870,7 +3897,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G7:G24</xm:sqref>
+          <xm:sqref>G8:G25</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3913,6 +3940,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4212,15 +4248,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4242,6 +4269,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1101C2D-3F57-4FE3-804B-005C212162D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4262,14 +4297,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
"GamePLay() : Work on calling the instance board into the current game, so tiles (which have been validated) can be placed on the board, then score tallied up."
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A583D0-1CD2-6F43-A5AC-DFE658287F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC66B1E-77D7-4141-9D16-FB3D77EAE66E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
   <si>
     <t>DATE</t>
   </si>
@@ -338,6 +338,13 @@
   </si>
   <si>
     <t>Implement more robost validation checking (for squares)</t>
+  </si>
+  <si>
+    <t>Substitution Principle, Overiding and Overloading</t>
+  </si>
+  <si>
+    <t>Really getting to grips with the substitution principle with regard to classes and interchanging methods with Player and HumanPlayer class.
+Also, realsied I've been overriding and overloading a lot, without realising. Overriding methods from WordValidator, extended to HumanPlayer subclass, and Overrloading methods -  putting different parameters in.</t>
   </si>
 </sst>
 </file>
@@ -2927,7 +2934,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>3521028</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4772071" cy="2667000"/>
@@ -2983,13 +2990,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>4241800</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>403225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8229600</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>3394075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3293,10 +3300,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3357,235 +3364,236 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
         <v>45369</v>
       </c>
       <c r="C4" s="12">
-        <v>0.72430555555555554</v>
+        <v>0.79652777777777772</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G4" s="13">
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="9">
         <v>45369</v>
       </c>
       <c r="C5" s="12">
-        <v>0.55277777777777781</v>
+        <v>0.72430555555555554</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G5" s="13">
-        <v>0.71</v>
+        <v>0.73</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
         <v>45369</v>
       </c>
       <c r="C6" s="12">
-        <v>0.22291666666666668</v>
+        <v>0.55277777777777781</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>66</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G6" s="13">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="9">
         <v>45369</v>
       </c>
       <c r="C7" s="12">
-        <v>5.8333333333333334E-2</v>
+        <v>0.22291666666666668</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G7" s="13">
-        <v>0.69</v>
+        <v>0.7</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="9">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="C8" s="12">
-        <v>0.96458333333333335</v>
+        <v>5.8333333333333334E-2</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" s="18">
-        <v>0.68500000000000005</v>
+        <v>61</v>
+      </c>
+      <c r="G8" s="13">
+        <v>0.69</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="9">
         <v>45368</v>
       </c>
       <c r="C9" s="12">
-        <v>0.79374999999999996</v>
+        <v>0.96458333333333335</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="13">
-        <v>0.67</v>
+        <v>58</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="18">
+        <v>0.68500000000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="9">
         <v>45368</v>
       </c>
       <c r="C10" s="12">
-        <v>0.44027777777777777</v>
+        <v>0.79374999999999996</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="G10" s="13">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="9">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="C11" s="12">
-        <v>7.0833333333333331E-2</v>
+        <v>0.44027777777777777</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G11" s="13">
-        <v>0.64</v>
-      </c>
-      <c r="I11" s="15"/>
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="12" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="9">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="C12" s="12">
-        <v>0.98611111111111116</v>
+        <v>7.0833333333333331E-2</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G12" s="13">
-        <v>0.63</v>
-      </c>
+        <v>0.64</v>
+      </c>
+      <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="9">
+        <v>45366</v>
+      </c>
+      <c r="C13" s="12">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="13">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="1"/>
+      <c r="B14" s="9">
         <v>45365</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C14" s="12">
         <v>2.1527777777777778E-2</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D14" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E14" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F14" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G14" s="13">
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="9">
-        <v>45364</v>
-      </c>
-      <c r="C14" s="12">
-        <v>0.35138888888888886</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="13">
-        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3593,59 +3601,59 @@
         <v>45364</v>
       </c>
       <c r="C15" s="12">
-        <v>0.22708333333333333</v>
+        <v>0.35138888888888886</v>
       </c>
       <c r="D15" s="21" t="s">
         <v>37</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G15" s="13">
-        <v>0.56000000000000005</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="9">
-        <v>45363</v>
+        <v>45364</v>
       </c>
       <c r="C16" s="12">
-        <v>0.56666666666666665</v>
+        <v>0.22708333333333333</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G16" s="13">
-        <v>0.54</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="9">
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="C17" s="12">
-        <v>0.95208333333333328</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G17" s="13">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3653,19 +3661,19 @@
         <v>45361</v>
       </c>
       <c r="C18" s="12">
-        <v>0.84236111111111112</v>
+        <v>0.95208333333333328</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G18" s="13">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3673,19 +3681,19 @@
         <v>45361</v>
       </c>
       <c r="C19" s="12">
-        <v>0.58819444444444446</v>
+        <v>0.84236111111111112</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="G19" s="13">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3693,19 +3701,19 @@
         <v>45361</v>
       </c>
       <c r="C20" s="12">
-        <v>0.15625</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G20" s="13">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3713,39 +3721,39 @@
         <v>45361</v>
       </c>
       <c r="C21" s="12">
-        <v>9.7222222222222224E-3</v>
+        <v>0.15625</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="G21" s="13">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="9">
-        <v>45360</v>
+        <v>45361</v>
       </c>
       <c r="C22" s="12">
-        <v>0.27291666666666664</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="G22" s="13">
-        <v>0.37</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3753,81 +3761,101 @@
         <v>45360</v>
       </c>
       <c r="C23" s="12">
-        <v>0.21458333333333332</v>
+        <v>0.27291666666666664</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G23" s="13">
-        <v>0.34</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="9">
-        <v>45359</v>
-      </c>
-      <c r="C24" s="10">
-        <v>20.32</v>
+        <v>45360</v>
+      </c>
+      <c r="C24" s="12">
+        <v>0.21458333333333332</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G24" s="13">
-        <v>0.32</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="9">
+        <v>45359</v>
+      </c>
+      <c r="C25" s="10">
+        <v>20.32</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="13">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="9">
         <v>45357</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C26" s="10">
         <v>13.26</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="D26" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="E26" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="F26" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="13">
+      <c r="G26" s="13">
         <v>0.22</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="27" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="28" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B5:E9">
+  <conditionalFormatting sqref="B5:E10">
     <cfRule type="expression" dxfId="2" priority="2">
       <formula>$A5=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B10:F25">
-    <cfRule type="expression" dxfId="1" priority="8">
-      <formula>$A10=1</formula>
+  <conditionalFormatting sqref="B11:F26">
+    <cfRule type="expression" dxfId="1" priority="9">
+      <formula>$A11=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G7">
-    <cfRule type="dataBar" priority="5">
+  <conditionalFormatting sqref="G4:G8">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3840,8 +3868,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G8:G25">
-    <cfRule type="dataBar" priority="9">
+  <conditionalFormatting sqref="G9:G26">
+    <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3882,7 +3910,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G7</xm:sqref>
+          <xm:sqref>G4:G8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{272DF8F1-2D7A-C948-BB97-5E4DFA143735}">
@@ -3897,7 +3925,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G8:G25</xm:sqref>
+          <xm:sqref>G9:G26</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3940,15 +3968,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4248,6 +4267,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4269,14 +4297,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1101C2D-3F57-4FE3-804B-005C212162D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4297,6 +4317,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
BoardInit() : Tidy up and streamling BoardInit to reduce code repitition and streamline game logic game flow.
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC66B1E-77D7-4141-9D16-FB3D77EAE66E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDEE0CCD-B536-2843-91DE-F1A7E72A4410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="76">
   <si>
     <t>DATE</t>
   </si>
@@ -345,6 +345,15 @@
   <si>
     <t>Really getting to grips with the substitution principle with regard to classes and interchanging methods with Player and HumanPlayer class.
 Also, realsied I've been overriding and overloading a lot, without realising. Overriding methods from WordValidator, extended to HumanPlayer subclass, and Overrloading methods -  putting different parameters in.</t>
+  </si>
+  <si>
+    <t>BoardInit()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Just tidying up and streamling BoardInit to reduce code repitition and streamline game logic game flow. </t>
+  </si>
+  <si>
+    <t>Housekeeping</t>
   </si>
 </sst>
 </file>
@@ -2934,7 +2943,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>3521028</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4772071" cy="2667000"/>
@@ -2990,13 +2999,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>4241800</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>403225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8229600</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>3394075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3300,10 +3309,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3328,7 +3337,7 @@
       <c r="E1" s="23"/>
       <c r="F1" s="27" t="str">
         <f ca="1">'Target '!A2-'Target '!A1&amp;" days remaining"</f>
-        <v>-4 days remaining</v>
+        <v>-3 days remaining</v>
       </c>
       <c r="G1" s="28"/>
     </row>
@@ -3367,253 +3376,254 @@
     <row r="4" spans="1:9" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="C4" s="12">
-        <v>0.79652777777777772</v>
+        <v>0.10138888888888889</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G4" s="13">
-        <v>0.74</v>
+        <v>0.75</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="9">
         <v>45369</v>
       </c>
       <c r="C5" s="12">
-        <v>0.72430555555555554</v>
+        <v>0.79652777777777772</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G5" s="13">
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
         <v>45369</v>
       </c>
       <c r="C6" s="12">
-        <v>0.55277777777777781</v>
+        <v>0.72430555555555554</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G6" s="13">
-        <v>0.71</v>
+        <v>0.73</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="9">
         <v>45369</v>
       </c>
       <c r="C7" s="12">
-        <v>0.22291666666666668</v>
+        <v>0.55277777777777781</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>66</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G7" s="13">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="9">
         <v>45369</v>
       </c>
       <c r="C8" s="12">
-        <v>5.8333333333333334E-2</v>
+        <v>0.22291666666666668</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G8" s="13">
-        <v>0.69</v>
+        <v>0.7</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="9">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="C9" s="12">
-        <v>0.96458333333333335</v>
+        <v>5.8333333333333334E-2</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" s="18">
-        <v>0.68500000000000005</v>
+        <v>61</v>
+      </c>
+      <c r="G9" s="13">
+        <v>0.69</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="9">
         <v>45368</v>
       </c>
       <c r="C10" s="12">
-        <v>0.79374999999999996</v>
+        <v>0.96458333333333335</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G10" s="13">
-        <v>0.67</v>
+        <v>58</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="18">
+        <v>0.68500000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="9">
         <v>45368</v>
       </c>
       <c r="C11" s="12">
-        <v>0.44027777777777777</v>
+        <v>0.79374999999999996</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="G11" s="13">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="9">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="C12" s="12">
-        <v>7.0833333333333331E-2</v>
+        <v>0.44027777777777777</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G12" s="13">
-        <v>0.64</v>
-      </c>
-      <c r="I12" s="15"/>
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="13" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="9">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="C13" s="12">
-        <v>0.98611111111111116</v>
+        <v>7.0833333333333331E-2</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G13" s="13">
-        <v>0.63</v>
-      </c>
+        <v>0.64</v>
+      </c>
+      <c r="I13" s="15"/>
     </row>
     <row r="14" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="9">
+        <v>45366</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="13">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="1"/>
+      <c r="B15" s="9">
         <v>45365</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C15" s="12">
         <v>2.1527777777777778E-2</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D15" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E15" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F15" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G15" s="13">
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="9">
-        <v>45364</v>
-      </c>
-      <c r="C15" s="12">
-        <v>0.35138888888888886</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="13">
-        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3621,59 +3631,59 @@
         <v>45364</v>
       </c>
       <c r="C16" s="12">
-        <v>0.22708333333333333</v>
+        <v>0.35138888888888886</v>
       </c>
       <c r="D16" s="21" t="s">
         <v>37</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G16" s="13">
-        <v>0.56000000000000005</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="9">
-        <v>45363</v>
+        <v>45364</v>
       </c>
       <c r="C17" s="12">
-        <v>0.56666666666666665</v>
+        <v>0.22708333333333333</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G17" s="13">
-        <v>0.54</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="9">
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="C18" s="12">
-        <v>0.95208333333333328</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G18" s="13">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3681,19 +3691,19 @@
         <v>45361</v>
       </c>
       <c r="C19" s="12">
-        <v>0.84236111111111112</v>
+        <v>0.95208333333333328</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G19" s="13">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3701,19 +3711,19 @@
         <v>45361</v>
       </c>
       <c r="C20" s="12">
-        <v>0.58819444444444446</v>
+        <v>0.84236111111111112</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="G20" s="13">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3721,19 +3731,19 @@
         <v>45361</v>
       </c>
       <c r="C21" s="12">
-        <v>0.15625</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G21" s="13">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3741,39 +3751,39 @@
         <v>45361</v>
       </c>
       <c r="C22" s="12">
-        <v>9.7222222222222224E-3</v>
+        <v>0.15625</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="G22" s="13">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="9">
-        <v>45360</v>
+        <v>45361</v>
       </c>
       <c r="C23" s="12">
-        <v>0.27291666666666664</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="G23" s="13">
-        <v>0.37</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3781,81 +3791,101 @@
         <v>45360</v>
       </c>
       <c r="C24" s="12">
-        <v>0.21458333333333332</v>
+        <v>0.27291666666666664</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G24" s="13">
-        <v>0.34</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="9">
-        <v>45359</v>
-      </c>
-      <c r="C25" s="10">
-        <v>20.32</v>
+        <v>45360</v>
+      </c>
+      <c r="C25" s="12">
+        <v>0.21458333333333332</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G25" s="13">
-        <v>0.32</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="9">
+        <v>45359</v>
+      </c>
+      <c r="C26" s="10">
+        <v>20.32</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="13">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="9">
         <v>45357</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C27" s="10">
         <v>13.26</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D27" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="E27" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F27" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G26" s="13">
+      <c r="G27" s="13">
         <v>0.22</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="28" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="29" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B5:E10">
+  <conditionalFormatting sqref="B5:E11">
     <cfRule type="expression" dxfId="2" priority="2">
       <formula>$A5=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11:F26">
-    <cfRule type="expression" dxfId="1" priority="9">
-      <formula>$A11=1</formula>
+  <conditionalFormatting sqref="B12:F27">
+    <cfRule type="expression" dxfId="1" priority="10">
+      <formula>$A12=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G8">
-    <cfRule type="dataBar" priority="6">
+  <conditionalFormatting sqref="G4:G9">
+    <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3868,8 +3898,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G9:G26">
-    <cfRule type="dataBar" priority="10">
+  <conditionalFormatting sqref="G10:G27">
+    <cfRule type="dataBar" priority="11">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3910,7 +3940,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G8</xm:sqref>
+          <xm:sqref>G4:G9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{272DF8F1-2D7A-C948-BB97-5E4DFA143735}">
@@ -3925,7 +3955,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G9:G26</xm:sqref>
+          <xm:sqref>G10:G27</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3956,7 +3986,7 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45369</v>
+        <v>45370</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
@@ -3968,6 +3998,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4267,15 +4306,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4297,6 +4327,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1101C2D-3F57-4FE3-804B-005C212162D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4317,14 +4355,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
BoardInit() / GamePlay() : Major breakthrough. Every time BoardInit class constructed a new board, the The takeTurn() method in GamePlay class always loads back and initialises default board (even if user chooses custom board). This initialization didn't consider any previous choice made by the user regarding custom or default board selection. Now Resolved so that one game instance can use one (the same) board.
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDEE0CCD-B536-2843-91DE-F1A7E72A4410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC8E547-1F6D-4543-AA27-4BCBC114C974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="78">
   <si>
     <t>DATE</t>
   </si>
@@ -354,6 +354,13 @@
   </si>
   <si>
     <t>Housekeeping</t>
+  </si>
+  <si>
+    <t>Major Breakthrough in understanding instance creation</t>
+  </si>
+  <si>
+    <t>Solved major problem.Everytime the BoardInit class constructed a new board, the The takeTurn() method in  GamePlay class always loads back the default board (even if user chooses custom board) because it directly initializes a new BoardInit object inside the method. This initialization didn't consider any previous choice made by the user regarding custom or default board selection.
+After days of racking my hair out, i finally solved this. a very emotional moment, where i started crying. Onwards and upwards</t>
   </si>
 </sst>
 </file>
@@ -2943,7 +2950,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>3521028</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4772071" cy="2667000"/>
@@ -2999,13 +3006,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>4241800</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>403225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8229600</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>3394075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3309,10 +3316,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3373,277 +3380,278 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
         <v>45370</v>
       </c>
       <c r="C4" s="12">
-        <v>0.10138888888888889</v>
+        <v>0.53055555555555556</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>73</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G4" s="13">
-        <v>0.75</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="9">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="C5" s="12">
-        <v>0.79652777777777772</v>
+        <v>0.10138888888888889</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G5" s="13">
-        <v>0.74</v>
+        <v>0.75</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
         <v>45369</v>
       </c>
       <c r="C6" s="12">
-        <v>0.72430555555555554</v>
+        <v>0.79652777777777772</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G6" s="13">
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="9">
         <v>45369</v>
       </c>
       <c r="C7" s="12">
-        <v>0.55277777777777781</v>
+        <v>0.72430555555555554</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G7" s="13">
-        <v>0.71</v>
+        <v>0.73</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="9">
         <v>45369</v>
       </c>
       <c r="C8" s="12">
-        <v>0.22291666666666668</v>
+        <v>0.55277777777777781</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>66</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G8" s="13">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="9">
         <v>45369</v>
       </c>
       <c r="C9" s="12">
-        <v>5.8333333333333334E-2</v>
+        <v>0.22291666666666668</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G9" s="13">
-        <v>0.69</v>
+        <v>0.7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="9">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="C10" s="12">
-        <v>0.96458333333333335</v>
+        <v>5.8333333333333334E-2</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" s="18">
-        <v>0.68500000000000005</v>
+        <v>61</v>
+      </c>
+      <c r="G10" s="13">
+        <v>0.69</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="9">
         <v>45368</v>
       </c>
       <c r="C11" s="12">
-        <v>0.79374999999999996</v>
+        <v>0.96458333333333335</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" s="13">
-        <v>0.67</v>
+        <v>58</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="18">
+        <v>0.68500000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="9">
         <v>45368</v>
       </c>
       <c r="C12" s="12">
-        <v>0.44027777777777777</v>
+        <v>0.79374999999999996</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="G12" s="13">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="9">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="C13" s="12">
-        <v>7.0833333333333331E-2</v>
+        <v>0.44027777777777777</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G13" s="13">
-        <v>0.64</v>
-      </c>
-      <c r="I13" s="15"/>
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="14" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="9">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="C14" s="12">
-        <v>0.98611111111111116</v>
+        <v>7.0833333333333331E-2</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G14" s="13">
-        <v>0.63</v>
-      </c>
+        <v>0.64</v>
+      </c>
+      <c r="I14" s="15"/>
     </row>
     <row r="15" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="9">
+        <v>45366</v>
+      </c>
+      <c r="C15" s="12">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="13">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="1"/>
+      <c r="B16" s="9">
         <v>45365</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C16" s="12">
         <v>2.1527777777777778E-2</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D16" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E16" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F16" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G16" s="13">
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="9">
-        <v>45364</v>
-      </c>
-      <c r="C16" s="12">
-        <v>0.35138888888888886</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" s="13">
-        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3651,59 +3659,59 @@
         <v>45364</v>
       </c>
       <c r="C17" s="12">
-        <v>0.22708333333333333</v>
+        <v>0.35138888888888886</v>
       </c>
       <c r="D17" s="21" t="s">
         <v>37</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G17" s="13">
-        <v>0.56000000000000005</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="9">
-        <v>45363</v>
+        <v>45364</v>
       </c>
       <c r="C18" s="12">
-        <v>0.56666666666666665</v>
+        <v>0.22708333333333333</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G18" s="13">
-        <v>0.54</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="9">
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="C19" s="12">
-        <v>0.95208333333333328</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G19" s="13">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3711,19 +3719,19 @@
         <v>45361</v>
       </c>
       <c r="C20" s="12">
-        <v>0.84236111111111112</v>
+        <v>0.95208333333333328</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G20" s="13">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3731,19 +3739,19 @@
         <v>45361</v>
       </c>
       <c r="C21" s="12">
-        <v>0.58819444444444446</v>
+        <v>0.84236111111111112</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="G21" s="13">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3751,19 +3759,19 @@
         <v>45361</v>
       </c>
       <c r="C22" s="12">
-        <v>0.15625</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G22" s="13">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3771,39 +3779,39 @@
         <v>45361</v>
       </c>
       <c r="C23" s="12">
-        <v>9.7222222222222224E-3</v>
+        <v>0.15625</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="G23" s="13">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="9">
-        <v>45360</v>
+        <v>45361</v>
       </c>
       <c r="C24" s="12">
-        <v>0.27291666666666664</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="G24" s="13">
-        <v>0.37</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3811,81 +3819,101 @@
         <v>45360</v>
       </c>
       <c r="C25" s="12">
-        <v>0.21458333333333332</v>
+        <v>0.27291666666666664</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G25" s="13">
-        <v>0.34</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="9">
-        <v>45359</v>
-      </c>
-      <c r="C26" s="10">
-        <v>20.32</v>
+        <v>45360</v>
+      </c>
+      <c r="C26" s="12">
+        <v>0.21458333333333332</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G26" s="13">
-        <v>0.32</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="9">
+        <v>45359</v>
+      </c>
+      <c r="C27" s="10">
+        <v>20.32</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="13">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B28" s="9">
         <v>45357</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C28" s="10">
         <v>13.26</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D28" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="E28" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F28" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G27" s="13">
+      <c r="G28" s="13">
         <v>0.22</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="29" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="30" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B5:E11">
+  <conditionalFormatting sqref="B5:E12">
     <cfRule type="expression" dxfId="2" priority="2">
       <formula>$A5=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12:F27">
-    <cfRule type="expression" dxfId="1" priority="10">
-      <formula>$A12=1</formula>
+  <conditionalFormatting sqref="B13:F28">
+    <cfRule type="expression" dxfId="1" priority="11">
+      <formula>$A13=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G9">
-    <cfRule type="dataBar" priority="7">
+  <conditionalFormatting sqref="G4:G10">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3898,8 +3926,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G10:G27">
-    <cfRule type="dataBar" priority="11">
+  <conditionalFormatting sqref="G11:G28">
+    <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3940,7 +3968,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G9</xm:sqref>
+          <xm:sqref>G4:G10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{272DF8F1-2D7A-C948-BB97-5E4DFA143735}">
@@ -3955,7 +3983,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G10:G27</xm:sqref>
+          <xm:sqref>G11:G28</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3998,15 +4026,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4306,6 +4325,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4327,14 +4355,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1101C2D-3F57-4FE3-804B-005C212162D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4355,6 +4375,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
BoardInit() : Created a new placeWordOnBoard()  method. Very detailed and intense work on getting the word tiles to display on the board and in write direction, so I can move to Score() class and methods.
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC8E547-1F6D-4543-AA27-4BCBC114C974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E03969-B14F-2344-BE47-C8B76BDB8150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="81">
   <si>
     <t>DATE</t>
   </si>
@@ -361,6 +361,18 @@
   <si>
     <t>Solved major problem.Everytime the BoardInit class constructed a new board, the The takeTurn() method in  GamePlay class always loads back the default board (even if user chooses custom board) because it directly initializes a new BoardInit object inside the method. This initialization didn't consider any previous choice made by the user regarding custom or default board selection.
 After days of racking my hair out, i finally solved this. a very emotional moment, where i started crying. Onwards and upwards</t>
+  </si>
+  <si>
+    <t>Tile Placement</t>
+  </si>
+  <si>
+    <t>BoardInit - setElement()</t>
+  </si>
+  <si>
+    <t>Very detailed and intense work on getting the word tiles to 
+display on the board and in write direction, so I can move to 
+Score() class and methods.
+Created a new placeWordOnBoard() to achieve this.</t>
   </si>
 </sst>
 </file>
@@ -2950,7 +2962,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>3521028</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4772071" cy="2667000"/>
@@ -3006,13 +3018,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>4241800</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>403225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8229600</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>3394075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3038,6 +3050,50 @@
         <a:xfrm>
           <a:off x="9791700" y="5838825"/>
           <a:ext cx="3987800" cy="2990850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5448300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>8242300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2133600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE66C3A5-DF7F-207B-693F-D7EB96A5C5BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10998200" y="2095500"/>
+          <a:ext cx="2794000" cy="2095500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3316,10 +3372,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3380,540 +3436,561 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
         <v>45370</v>
       </c>
       <c r="C4" s="12">
-        <v>0.53055555555555556</v>
+        <v>0.67708333333333337</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G4" s="13">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="9">
         <v>45370</v>
       </c>
       <c r="C5" s="12">
-        <v>0.10138888888888889</v>
+        <v>0.53055555555555556</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>73</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G5" s="13">
-        <v>0.75</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="C6" s="12">
-        <v>0.79652777777777772</v>
+        <v>0.10138888888888889</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G6" s="13">
-        <v>0.74</v>
+        <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="9">
         <v>45369</v>
       </c>
       <c r="C7" s="12">
-        <v>0.72430555555555554</v>
+        <v>0.79652777777777772</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G7" s="13">
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="9">
         <v>45369</v>
       </c>
       <c r="C8" s="12">
-        <v>0.55277777777777781</v>
+        <v>0.72430555555555554</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G8" s="13">
-        <v>0.71</v>
+        <v>0.73</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="9">
         <v>45369</v>
       </c>
       <c r="C9" s="12">
-        <v>0.22291666666666668</v>
+        <v>0.55277777777777781</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>66</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G9" s="13">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="9">
         <v>45369</v>
       </c>
       <c r="C10" s="12">
-        <v>5.8333333333333334E-2</v>
+        <v>0.22291666666666668</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G10" s="13">
-        <v>0.69</v>
+        <v>0.7</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="9">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="C11" s="12">
-        <v>0.96458333333333335</v>
+        <v>5.8333333333333334E-2</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11" s="18">
-        <v>0.68500000000000005</v>
+        <v>61</v>
+      </c>
+      <c r="G11" s="13">
+        <v>0.69</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="9">
         <v>45368</v>
       </c>
       <c r="C12" s="12">
-        <v>0.79374999999999996</v>
+        <v>0.96458333333333335</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="13">
-        <v>0.67</v>
+        <v>58</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="18">
+        <v>0.68500000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="9">
         <v>45368</v>
       </c>
       <c r="C13" s="12">
-        <v>0.44027777777777777</v>
+        <v>0.79374999999999996</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="G13" s="13">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="9">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="C14" s="12">
-        <v>7.0833333333333331E-2</v>
+        <v>0.44027777777777777</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G14" s="13">
-        <v>0.64</v>
-      </c>
-      <c r="I14" s="15"/>
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="15" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="9">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="C15" s="12">
-        <v>0.98611111111111116</v>
+        <v>7.0833333333333331E-2</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G15" s="13">
-        <v>0.63</v>
-      </c>
+        <v>0.64</v>
+      </c>
+      <c r="I15" s="15"/>
     </row>
     <row r="16" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="9">
+        <v>45366</v>
+      </c>
+      <c r="C16" s="12">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="13">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="1"/>
+      <c r="B17" s="9">
         <v>45365</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C17" s="12">
         <v>2.1527777777777778E-2</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D17" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E17" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F17" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G17" s="13">
         <v>0.6</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="9">
-        <v>45364</v>
-      </c>
-      <c r="C17" s="12">
-        <v>0.35138888888888886</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G17" s="13">
-        <v>0.57999999999999996</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="9">
         <v>45364</v>
       </c>
       <c r="C18" s="12">
-        <v>0.22708333333333333</v>
+        <v>0.35138888888888886</v>
       </c>
       <c r="D18" s="21" t="s">
         <v>37</v>
       </c>
       <c r="E18" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="13">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="9">
+        <v>45364</v>
+      </c>
+      <c r="C19" s="12">
+        <v>0.22708333333333333</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F19" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G19" s="13">
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="9">
+    <row r="20" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="9">
         <v>45363</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C20" s="12">
         <v>0.56666666666666665</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D20" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E20" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F20" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G20" s="13">
         <v>0.54</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="9">
-        <v>45361</v>
-      </c>
-      <c r="C20" s="12">
-        <v>0.95208333333333328</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" s="13">
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="9">
         <v>45361</v>
       </c>
       <c r="C21" s="12">
-        <v>0.84236111111111112</v>
+        <v>0.95208333333333328</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G21" s="13">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="9">
         <v>45361</v>
       </c>
       <c r="C22" s="12">
-        <v>0.58819444444444446</v>
+        <v>0.84236111111111112</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="G22" s="13">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="9">
         <v>45361</v>
       </c>
       <c r="C23" s="12">
-        <v>0.15625</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G23" s="13">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="9">
         <v>45361</v>
       </c>
       <c r="C24" s="12">
+        <v>0.15625</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="13">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="9">
+        <v>45361</v>
+      </c>
+      <c r="C25" s="12">
         <v>9.7222222222222224E-3</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D25" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="21" t="s">
+      <c r="E25" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F25" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G25" s="13">
         <v>0.42</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="9">
-        <v>45360</v>
-      </c>
-      <c r="C25" s="12">
-        <v>0.27291666666666664</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G25" s="13">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="9">
         <v>45360</v>
       </c>
       <c r="C26" s="12">
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="13">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="9">
+        <v>45360</v>
+      </c>
+      <c r="C27" s="12">
         <v>0.21458333333333332</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D27" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="E27" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F27" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G26" s="13">
+      <c r="G27" s="13">
         <v>0.34</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="9">
+    <row r="28" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B28" s="9">
         <v>45359</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C28" s="10">
         <v>20.32</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D28" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="E28" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F28" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G27" s="13">
+      <c r="G28" s="13">
         <v>0.32</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B28" s="9">
+    <row r="29" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B29" s="9">
         <v>45357</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C29" s="10">
         <v>13.26</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D29" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E29" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F29" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G28" s="13">
+      <c r="G29" s="13">
         <v>0.22</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="30" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="30" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="31" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B5:E12">
+  <conditionalFormatting sqref="B5:E13">
     <cfRule type="expression" dxfId="2" priority="2">
       <formula>$A5=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13:F28">
-    <cfRule type="expression" dxfId="1" priority="11">
-      <formula>$A13=1</formula>
+  <conditionalFormatting sqref="B14:F29">
+    <cfRule type="expression" dxfId="1" priority="12">
+      <formula>$A14=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G10">
-    <cfRule type="dataBar" priority="8">
+  <conditionalFormatting sqref="G4:G11">
+    <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3926,8 +4003,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G11:G28">
-    <cfRule type="dataBar" priority="12">
+  <conditionalFormatting sqref="G12:G29">
+    <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3968,7 +4045,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G10</xm:sqref>
+          <xm:sqref>G4:G11</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{272DF8F1-2D7A-C948-BB97-5E4DFA143735}">
@@ -3983,7 +4060,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G11:G28</xm:sqref>
+          <xm:sqref>G12:G29</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4026,6 +4103,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4325,15 +4411,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4355,6 +4432,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1101C2D-3F57-4FE3-804B-005C212162D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4375,14 +4460,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
WordValidator(), HumanPlayer() Housekeeping / Bug fixing.
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E03969-B14F-2344-BE47-C8B76BDB8150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24ABC67-AE28-B647-91DB-96763AF4A338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="84">
   <si>
     <t>DATE</t>
   </si>
@@ -373,6 +373,18 @@
 display on the board and in write direction, so I can move to 
 Score() class and methods.
 Created a new placeWordOnBoard() to achieve this.</t>
+  </si>
+  <si>
+    <t>Hosekeeping, code cleaning. Needed to get my house in order (code working great) before
+introducing any more complex code.
+Going into my own Sprint Cycle to produce deliverables - now.  Requirements are locked down.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+House Keeping - dusting off bugs !</t>
+  </si>
+  <si>
+    <t>WordValidator() , HumanPlayer()</t>
   </si>
 </sst>
 </file>
@@ -675,7 +687,7 @@
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -763,6 +775,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="10" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="6" builtinId="3" customBuiltin="1"/>
@@ -779,14 +794,7 @@
     <cellStyle name="Phone" xfId="8" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Title" xfId="7" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <b/>
@@ -873,10 +881,10 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Library Book Checkout Sheet" defaultPivotStyle="PivotStyleMedium9">
     <tableStyle name="Library Book Checkout Sheet" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="6"/>
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="firstColumn" dxfId="4"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="3"/>
+      <tableStyleElement type="wholeTable" dxfId="5"/>
+      <tableStyleElement type="headerRow" dxfId="4"/>
+      <tableStyleElement type="firstColumn" dxfId="3"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="2"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2962,7 +2970,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>3521028</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4772071" cy="2667000"/>
@@ -3018,13 +3026,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>4241800</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>403225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8229600</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>3394075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3062,13 +3070,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>5448300</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8242300</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>2133600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3092,8 +3100,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10998200" y="2095500"/>
+          <a:off x="10998200" y="2844800"/>
           <a:ext cx="2794000" cy="2095500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>241376</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1155700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1511300</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEF47469-2266-7FBE-F072-1E49EECBB6A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4064076" y="3213100"/>
+          <a:ext cx="1269924" cy="1358900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3372,10 +3424,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3400,7 +3452,7 @@
       <c r="E1" s="23"/>
       <c r="F1" s="27" t="str">
         <f ca="1">'Target '!A2-'Target '!A1&amp;" days remaining"</f>
-        <v>-3 days remaining</v>
+        <v>-2 days remaining</v>
       </c>
       <c r="G1" s="28"/>
     </row>
@@ -3436,319 +3488,320 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="C4" s="12">
-        <v>0.67708333333333337</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>78</v>
+        <v>83</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>82</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G4" s="13">
-        <v>0.8</v>
+        <v>0.81</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="9">
         <v>45370</v>
       </c>
       <c r="C5" s="12">
-        <v>0.53055555555555556</v>
+        <v>0.67708333333333337</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G5" s="13">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
         <v>45370</v>
       </c>
       <c r="C6" s="12">
-        <v>0.10138888888888889</v>
+        <v>0.53055555555555556</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>73</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G6" s="13">
-        <v>0.75</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="9">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="C7" s="12">
-        <v>0.79652777777777772</v>
+        <v>0.10138888888888889</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G7" s="13">
-        <v>0.74</v>
+        <v>0.75</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="9">
         <v>45369</v>
       </c>
       <c r="C8" s="12">
-        <v>0.72430555555555554</v>
+        <v>0.79652777777777772</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G8" s="13">
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="9">
         <v>45369</v>
       </c>
       <c r="C9" s="12">
-        <v>0.55277777777777781</v>
+        <v>0.72430555555555554</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G9" s="13">
-        <v>0.71</v>
+        <v>0.73</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="9">
         <v>45369</v>
       </c>
       <c r="C10" s="12">
-        <v>0.22291666666666668</v>
+        <v>0.55277777777777781</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>66</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G10" s="13">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="9">
         <v>45369</v>
       </c>
       <c r="C11" s="12">
-        <v>5.8333333333333334E-2</v>
+        <v>0.22291666666666668</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G11" s="13">
-        <v>0.69</v>
+        <v>0.7</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="9">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="C12" s="12">
-        <v>0.96458333333333335</v>
+        <v>5.8333333333333334E-2</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="G12" s="18">
-        <v>0.68500000000000005</v>
+        <v>61</v>
+      </c>
+      <c r="G12" s="13">
+        <v>0.69</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="9">
         <v>45368</v>
       </c>
       <c r="C13" s="12">
-        <v>0.79374999999999996</v>
+        <v>0.96458333333333335</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" s="13">
-        <v>0.67</v>
+        <v>58</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="18">
+        <v>0.68500000000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="9">
         <v>45368</v>
       </c>
       <c r="C14" s="12">
-        <v>0.44027777777777777</v>
+        <v>0.79374999999999996</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="G14" s="13">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="9">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="C15" s="12">
-        <v>7.0833333333333331E-2</v>
+        <v>0.44027777777777777</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G15" s="13">
-        <v>0.64</v>
-      </c>
-      <c r="I15" s="15"/>
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="16" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="9">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="C16" s="12">
-        <v>0.98611111111111116</v>
+        <v>7.0833333333333331E-2</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G16" s="13">
-        <v>0.63</v>
-      </c>
+        <v>0.64</v>
+      </c>
+      <c r="I16" s="15"/>
     </row>
     <row r="17" spans="1:7" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="9">
+        <v>45366</v>
+      </c>
+      <c r="C17" s="12">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="13">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="1"/>
+      <c r="B18" s="9">
         <v>45365</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C18" s="12">
         <v>2.1527777777777778E-2</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D18" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E18" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F18" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G18" s="13">
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="9">
-        <v>45364</v>
-      </c>
-      <c r="C18" s="12">
-        <v>0.35138888888888886</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G18" s="13">
-        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3756,59 +3809,59 @@
         <v>45364</v>
       </c>
       <c r="C19" s="12">
-        <v>0.22708333333333333</v>
+        <v>0.35138888888888886</v>
       </c>
       <c r="D19" s="21" t="s">
         <v>37</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G19" s="13">
-        <v>0.56000000000000005</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="9">
-        <v>45363</v>
+        <v>45364</v>
       </c>
       <c r="C20" s="12">
-        <v>0.56666666666666665</v>
+        <v>0.22708333333333333</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G20" s="13">
-        <v>0.54</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="9">
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="C21" s="12">
-        <v>0.95208333333333328</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G21" s="13">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3816,19 +3869,19 @@
         <v>45361</v>
       </c>
       <c r="C22" s="12">
-        <v>0.84236111111111112</v>
+        <v>0.95208333333333328</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G22" s="13">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3836,19 +3889,19 @@
         <v>45361</v>
       </c>
       <c r="C23" s="12">
-        <v>0.58819444444444446</v>
+        <v>0.84236111111111112</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="G23" s="13">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3856,19 +3909,19 @@
         <v>45361</v>
       </c>
       <c r="C24" s="12">
-        <v>0.15625</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G24" s="13">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3876,39 +3929,39 @@
         <v>45361</v>
       </c>
       <c r="C25" s="12">
-        <v>9.7222222222222224E-3</v>
+        <v>0.15625</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="G25" s="13">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="9">
-        <v>45360</v>
+        <v>45361</v>
       </c>
       <c r="C26" s="12">
-        <v>0.27291666666666664</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="G26" s="13">
-        <v>0.37</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3916,81 +3969,101 @@
         <v>45360</v>
       </c>
       <c r="C27" s="12">
-        <v>0.21458333333333332</v>
+        <v>0.27291666666666664</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G27" s="13">
-        <v>0.34</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="9">
-        <v>45359</v>
-      </c>
-      <c r="C28" s="10">
-        <v>20.32</v>
+        <v>45360</v>
+      </c>
+      <c r="C28" s="12">
+        <v>0.21458333333333332</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G28" s="13">
-        <v>0.32</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="9">
+        <v>45359</v>
+      </c>
+      <c r="C29" s="10">
+        <v>20.32</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="13">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B30" s="9">
         <v>45357</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C30" s="10">
         <v>13.26</v>
       </c>
-      <c r="D29" s="21" t="s">
+      <c r="D30" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E29" s="21" t="s">
+      <c r="E30" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F30" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G29" s="13">
+      <c r="G30" s="13">
         <v>0.22</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="31" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="32" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B5:E13">
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>$A5=1</formula>
+  <conditionalFormatting sqref="B4:E14">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14:F29">
-    <cfRule type="expression" dxfId="1" priority="12">
-      <formula>$A14=1</formula>
+  <conditionalFormatting sqref="B15:F30">
+    <cfRule type="expression" dxfId="0" priority="13">
+      <formula>$A15=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G11">
-    <cfRule type="dataBar" priority="9">
+  <conditionalFormatting sqref="G4:G12">
+    <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4003,8 +4076,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G12:G29">
-    <cfRule type="dataBar" priority="13">
+  <conditionalFormatting sqref="G13:G30">
+    <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4015,11 +4088,6 @@
           <x14:id>{272DF8F1-2D7A-C948-BB97-5E4DFA143735}</x14:id>
         </ext>
       </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4:E4">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
@@ -4045,7 +4113,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G11</xm:sqref>
+          <xm:sqref>G4:G12</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{272DF8F1-2D7A-C948-BB97-5E4DFA143735}">
@@ -4060,7 +4128,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G12:G29</xm:sqref>
+          <xm:sqref>G13:G30</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4091,7 +4159,7 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45370</v>
+        <v>45371</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
@@ -4103,15 +4171,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4411,6 +4470,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4432,14 +4500,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1101C2D-3F57-4FE3-804B-005C212162D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4460,6 +4520,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
WordValidator() Moved V&V methods (validation) from HumanPlayer class to its dedicated WordValidator class to promote code reuse and readability.
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24ABC67-AE28-B647-91DB-96763AF4A338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FA4740-6ED5-E346-B19A-16BF2F99929C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="86">
   <si>
     <t>DATE</t>
   </si>
@@ -385,6 +385,17 @@
   </si>
   <si>
     <t>WordValidator() , HumanPlayer()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The 'housekeeping' in my last update paid off. It allowed me to dust off the cobweb skeletons of
+some old legacy code, get rid of niggly things and really understand the bigger pictire.
+One outcome of this, I realised all my validation methods (V&amp;V) were not robust enough, and all
+my validation methods were in the HumanPlayer class - making it unweidely, and unusable should 
+any other clas (ComputerPLayer) wish to use them. THis was bad for code reusability. So i ended up moving everything to the dedicated WordfValidator class. Lost a lot of time doing this, and progress wasn't really made. Howdver, i'm starting to see the bigger picture. Most important is my learning and understanding, over my rush to get something done just for the sake of it. By mthodically trying things out and slowlyt reading up while applying in practice, i'm developing a depper understanding of what i'm doing.
+I'd like to think that even if i doon't finish the game, i'd get some marks for showing some creativity in problem-solving, and using the softwar design principles (inheritance, polymorphism,e tc). </t>
+  </si>
+  <si>
+    <t>Slow turtle race, not a fast rabbit race.</t>
   </si>
 </sst>
 </file>
@@ -687,7 +698,7 @@
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -754,6 +765,9 @@
     <xf numFmtId="20" fontId="10" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="10" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -776,7 +790,7 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="10" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -794,7 +808,14 @@
     <cellStyle name="Phone" xfId="8" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Title" xfId="7" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -881,10 +902,10 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Library Book Checkout Sheet" defaultPivotStyle="PivotStyleMedium9">
     <tableStyle name="Library Book Checkout Sheet" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="5"/>
-      <tableStyleElement type="headerRow" dxfId="4"/>
-      <tableStyleElement type="firstColumn" dxfId="3"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="2"/>
+      <tableStyleElement type="wholeTable" dxfId="6"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="firstColumn" dxfId="4"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="3"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2970,7 +2991,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>3521028</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4772071" cy="2667000"/>
@@ -3026,13 +3047,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>4241800</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>403225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8229600</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>3394075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3070,13 +3091,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>5448300</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8242300</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>2133600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3114,13 +3135,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>241376</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>1155700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1511300</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3424,10 +3445,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3442,32 +3463,32 @@
     <col min="8" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="37" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="37" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="27" t="str">
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="28" t="str">
         <f ca="1">'Target '!A2-'Target '!A1&amp;" days remaining"</f>
         <v>-2 days remaining</v>
       </c>
-      <c r="G1" s="28"/>
+      <c r="G1" s="29"/>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="27"/>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="7" t="s">
         <v>0</v>
@@ -3488,582 +3509,603 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" s="2" customFormat="1" ht="320" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
         <v>45371</v>
       </c>
       <c r="C4" s="12">
-        <v>9.7222222222222224E-3</v>
+        <v>0.18055555555555555</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="E4" s="29" t="s">
-        <v>82</v>
+      <c r="E4" s="30" t="s">
+        <v>85</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="G4" s="13">
-        <v>0.81</v>
+        <v>84</v>
+      </c>
+      <c r="G4" s="18">
+        <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="9">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="C5" s="12">
-        <v>0.67708333333333337</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>78</v>
+        <v>83</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>82</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G5" s="13">
-        <v>0.8</v>
+        <v>0.81</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
         <v>45370</v>
       </c>
       <c r="C6" s="12">
-        <v>0.53055555555555556</v>
+        <v>0.67708333333333337</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G6" s="13">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" s="2" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="9">
         <v>45370</v>
       </c>
       <c r="C7" s="12">
-        <v>0.10138888888888889</v>
+        <v>0.53055555555555556</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>73</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G7" s="13">
-        <v>0.75</v>
+        <v>0.78</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="9">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="C8" s="12">
-        <v>0.79652777777777772</v>
+        <v>0.10138888888888889</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G8" s="13">
-        <v>0.74</v>
+        <v>0.75</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="9">
         <v>45369</v>
       </c>
       <c r="C9" s="12">
-        <v>0.72430555555555554</v>
+        <v>0.79652777777777772</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G9" s="13">
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="9">
         <v>45369</v>
       </c>
       <c r="C10" s="12">
-        <v>0.55277777777777781</v>
+        <v>0.72430555555555554</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G10" s="13">
-        <v>0.71</v>
+        <v>0.73</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="9">
         <v>45369</v>
       </c>
       <c r="C11" s="12">
-        <v>0.22291666666666668</v>
+        <v>0.55277777777777781</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>66</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G11" s="13">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="9">
         <v>45369</v>
       </c>
       <c r="C12" s="12">
-        <v>5.8333333333333334E-2</v>
+        <v>0.22291666666666668</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G12" s="13">
-        <v>0.69</v>
+        <v>0.7</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="9">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="C13" s="12">
-        <v>0.96458333333333335</v>
+        <v>5.8333333333333334E-2</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="18">
-        <v>0.68500000000000005</v>
+        <v>61</v>
+      </c>
+      <c r="G13" s="13">
+        <v>0.69</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="9">
         <v>45368</v>
       </c>
       <c r="C14" s="12">
-        <v>0.79374999999999996</v>
+        <v>0.96458333333333335</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="13">
-        <v>0.67</v>
+        <v>58</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="18">
+        <v>0.68500000000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="9">
         <v>45368</v>
       </c>
       <c r="C15" s="12">
-        <v>0.44027777777777777</v>
+        <v>0.79374999999999996</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="G15" s="13">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="9">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="C16" s="12">
-        <v>7.0833333333333331E-2</v>
+        <v>0.44027777777777777</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G16" s="13">
-        <v>0.64</v>
-      </c>
-      <c r="I16" s="15"/>
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="17" spans="1:7" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="9">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="C17" s="12">
-        <v>0.98611111111111116</v>
+        <v>7.0833333333333331E-2</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G17" s="13">
-        <v>0.63</v>
-      </c>
+        <v>0.64</v>
+      </c>
+      <c r="I17" s="15"/>
     </row>
-    <row r="18" spans="1:7" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
       <c r="B18" s="9">
+        <v>45366</v>
+      </c>
+      <c r="C18" s="12">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="13">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="1"/>
+      <c r="B19" s="9">
         <v>45365</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C19" s="12">
         <v>2.1527777777777778E-2</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="D19" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E19" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F19" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G19" s="13">
         <v>0.6</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="9">
-        <v>45364</v>
-      </c>
-      <c r="C19" s="12">
-        <v>0.35138888888888886</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G19" s="13">
-        <v>0.57999999999999996</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="9">
         <v>45364</v>
       </c>
       <c r="C20" s="12">
-        <v>0.22708333333333333</v>
+        <v>0.35138888888888886</v>
       </c>
       <c r="D20" s="21" t="s">
         <v>37</v>
       </c>
       <c r="E20" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="13">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="9">
+        <v>45364</v>
+      </c>
+      <c r="C21" s="12">
+        <v>0.22708333333333333</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F21" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G21" s="13">
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="9">
+    <row r="22" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="9">
         <v>45363</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C22" s="12">
         <v>0.56666666666666665</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="D22" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E22" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F22" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G22" s="13">
         <v>0.54</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="9">
-        <v>45361</v>
-      </c>
-      <c r="C22" s="12">
-        <v>0.95208333333333328</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G22" s="13">
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="9">
         <v>45361</v>
       </c>
       <c r="C23" s="12">
-        <v>0.84236111111111112</v>
+        <v>0.95208333333333328</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G23" s="13">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="9">
         <v>45361</v>
       </c>
       <c r="C24" s="12">
-        <v>0.58819444444444446</v>
+        <v>0.84236111111111112</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="G24" s="13">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="9">
         <v>45361</v>
       </c>
       <c r="C25" s="12">
-        <v>0.15625</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G25" s="13">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="9">
         <v>45361</v>
       </c>
       <c r="C26" s="12">
+        <v>0.15625</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" s="13">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="9">
+        <v>45361</v>
+      </c>
+      <c r="C27" s="12">
         <v>9.7222222222222224E-3</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D27" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="E27" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F27" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G26" s="13">
+      <c r="G27" s="13">
         <v>0.42</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="9">
-        <v>45360</v>
-      </c>
-      <c r="C27" s="12">
-        <v>0.27291666666666664</v>
-      </c>
-      <c r="D27" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" s="13">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="9">
         <v>45360</v>
       </c>
       <c r="C28" s="12">
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="13">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B29" s="9">
+        <v>45360</v>
+      </c>
+      <c r="C29" s="12">
         <v>0.21458333333333332</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D29" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E29" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F29" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G28" s="13">
+      <c r="G29" s="13">
         <v>0.34</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="9">
+    <row r="30" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B30" s="9">
         <v>45359</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C30" s="10">
         <v>20.32</v>
       </c>
-      <c r="D29" s="21" t="s">
+      <c r="D30" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="21" t="s">
+      <c r="E30" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F30" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G29" s="13">
+      <c r="G30" s="13">
         <v>0.32</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B30" s="9">
+    <row r="31" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B31" s="9">
         <v>45357</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C31" s="10">
         <v>13.26</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D31" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E31" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F30" s="11" t="s">
+      <c r="F31" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G30" s="13">
+      <c r="G31" s="13">
         <v>0.22</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="32" spans="1:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="32" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="33" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:E14">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>$A4=1</formula>
+  <conditionalFormatting sqref="B5:E15">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$A5=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15:F30">
-    <cfRule type="expression" dxfId="0" priority="13">
-      <formula>$A15=1</formula>
+  <conditionalFormatting sqref="B16:F31">
+    <cfRule type="expression" dxfId="1" priority="14">
+      <formula>$A16=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G12">
-    <cfRule type="dataBar" priority="10">
+  <conditionalFormatting sqref="G4:G13">
+    <cfRule type="dataBar" priority="11">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4076,8 +4118,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G13:G30">
-    <cfRule type="dataBar" priority="14">
+  <conditionalFormatting sqref="G14:G31">
+    <cfRule type="dataBar" priority="15">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4088,6 +4130,11 @@
           <x14:id>{272DF8F1-2D7A-C948-BB97-5E4DFA143735}</x14:id>
         </ext>
       </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:E4">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
@@ -4113,7 +4160,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G12</xm:sqref>
+          <xm:sqref>G4:G13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{272DF8F1-2D7A-C948-BB97-5E4DFA143735}">
@@ -4128,7 +4175,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G13:G30</xm:sqref>
+          <xm:sqref>G14:G31</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4171,6 +4218,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4470,36 +4546,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1101C2D-3F57-4FE3-804B-005C212162D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4520,26 +4587,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
MoveValidator() Created this new class which validates moves made by the human player on the game board.  It utilizes information about the current  game board size, the player's entered word, and the required direction of placement of their tiles (e.g., H4) to perform various checks. Also created isWithinBoard() and other methods - currently commented out whilst testing).
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FA4740-6ED5-E346-B19A-16BF2F99929C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E062CB4-4FDE-CD4F-A83C-411900923569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="89">
   <si>
     <t>DATE</t>
   </si>
@@ -396,6 +396,17 @@
   </si>
   <si>
     <t>Slow turtle race, not a fast rabbit race.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work furthering the principles of encapsulation and separation of concerns,  dividing the program into smaller, more focused modules. I've created a MoveValidator class (in the same mould as WordValidator class. 
+This MoveValidator validates moves made by the human player on the game board.  It utilizes information about the current  game board size, the player's entered word, and the required direction of placement of their tiles (e.g., H4) to perform various checks.
+  </t>
+  </si>
+  <si>
+    <t>Seperate Lives, just one mind.</t>
+  </si>
+  <si>
+    <t>MoveValidator()</t>
   </si>
 </sst>
 </file>
@@ -768,6 +779,9 @@
     <xf numFmtId="20" fontId="10" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="10" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -788,9 +802,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="10" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -2991,7 +3002,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>3521028</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4772071" cy="2667000"/>
@@ -3047,13 +3058,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>4241800</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>403225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8229600</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>3394075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3091,13 +3102,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>5448300</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8242300</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>2133600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3135,13 +3146,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>241376</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>1155700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1511300</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3445,10 +3456,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3465,28 +3476,28 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="37" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="28" t="str">
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="29" t="str">
         <f ca="1">'Target '!A2-'Target '!A1&amp;" days remaining"</f>
         <v>-2 days remaining</v>
       </c>
-      <c r="G1" s="29"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="28"/>
     </row>
     <row r="3" spans="1:7" s="2" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
@@ -3509,361 +3520,362 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="320" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" s="2" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
         <v>45371</v>
       </c>
       <c r="C4" s="12">
-        <v>0.18055555555555555</v>
+        <v>0.51180555555555551</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>85</v>
+        <v>88</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>87</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G4" s="18">
-        <v>0.81399999999999995</v>
+        <v>0.82</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="320" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="9">
         <v>45371</v>
       </c>
       <c r="C5" s="12">
-        <v>9.7222222222222224E-3</v>
+        <v>0.18055555555555555</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="E5" s="22" t="s">
-        <v>82</v>
+      <c r="E5" s="23" t="s">
+        <v>85</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="G5" s="13">
-        <v>0.81</v>
+        <v>84</v>
+      </c>
+      <c r="G5" s="18">
+        <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="C6" s="12">
-        <v>0.67708333333333337</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>78</v>
+        <v>83</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>82</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G6" s="13">
-        <v>0.8</v>
+        <v>0.81</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" s="2" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="9">
         <v>45370</v>
       </c>
       <c r="C7" s="12">
-        <v>0.53055555555555556</v>
+        <v>0.67708333333333337</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G7" s="13">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" s="2" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="9">
         <v>45370</v>
       </c>
       <c r="C8" s="12">
-        <v>0.10138888888888889</v>
+        <v>0.53055555555555556</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>73</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G8" s="13">
-        <v>0.75</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="9">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="C9" s="12">
-        <v>0.79652777777777772</v>
+        <v>0.10138888888888889</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G9" s="13">
-        <v>0.74</v>
+        <v>0.75</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="9">
         <v>45369</v>
       </c>
       <c r="C10" s="12">
-        <v>0.72430555555555554</v>
+        <v>0.79652777777777772</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G10" s="13">
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="9">
         <v>45369</v>
       </c>
       <c r="C11" s="12">
-        <v>0.55277777777777781</v>
+        <v>0.72430555555555554</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G11" s="13">
-        <v>0.71</v>
+        <v>0.73</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="9">
         <v>45369</v>
       </c>
       <c r="C12" s="12">
-        <v>0.22291666666666668</v>
+        <v>0.55277777777777781</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>66</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G12" s="13">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="9">
         <v>45369</v>
       </c>
       <c r="C13" s="12">
-        <v>5.8333333333333334E-2</v>
+        <v>0.22291666666666668</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G13" s="13">
-        <v>0.69</v>
+        <v>0.7</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="9">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="C14" s="12">
-        <v>0.96458333333333335</v>
+        <v>5.8333333333333334E-2</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="G14" s="18">
-        <v>0.68500000000000005</v>
+        <v>61</v>
+      </c>
+      <c r="G14" s="13">
+        <v>0.69</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="9">
         <v>45368</v>
       </c>
       <c r="C15" s="12">
-        <v>0.79374999999999996</v>
+        <v>0.96458333333333335</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" s="13">
-        <v>0.67</v>
+        <v>58</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="18">
+        <v>0.68500000000000005</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="9">
         <v>45368</v>
       </c>
       <c r="C16" s="12">
-        <v>0.44027777777777777</v>
+        <v>0.79374999999999996</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="G16" s="13">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="9">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="C17" s="12">
-        <v>7.0833333333333331E-2</v>
+        <v>0.44027777777777777</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G17" s="13">
-        <v>0.64</v>
-      </c>
-      <c r="I17" s="15"/>
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="18" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
       <c r="B18" s="9">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="C18" s="12">
-        <v>0.98611111111111116</v>
+        <v>7.0833333333333331E-2</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G18" s="13">
-        <v>0.63</v>
-      </c>
+        <v>0.64</v>
+      </c>
+      <c r="I18" s="15"/>
     </row>
     <row r="19" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
       <c r="B19" s="9">
+        <v>45366</v>
+      </c>
+      <c r="C19" s="12">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="13">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="1"/>
+      <c r="B20" s="9">
         <v>45365</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C20" s="12">
         <v>2.1527777777777778E-2</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D20" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E20" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F20" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G20" s="13">
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="9">
-        <v>45364</v>
-      </c>
-      <c r="C20" s="12">
-        <v>0.35138888888888886</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G20" s="13">
-        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3871,59 +3883,59 @@
         <v>45364</v>
       </c>
       <c r="C21" s="12">
-        <v>0.22708333333333333</v>
+        <v>0.35138888888888886</v>
       </c>
       <c r="D21" s="21" t="s">
         <v>37</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G21" s="13">
-        <v>0.56000000000000005</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="9">
-        <v>45363</v>
+        <v>45364</v>
       </c>
       <c r="C22" s="12">
-        <v>0.56666666666666665</v>
+        <v>0.22708333333333333</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G22" s="13">
-        <v>0.54</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="9">
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="C23" s="12">
-        <v>0.95208333333333328</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G23" s="13">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3931,19 +3943,19 @@
         <v>45361</v>
       </c>
       <c r="C24" s="12">
-        <v>0.84236111111111112</v>
+        <v>0.95208333333333328</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G24" s="13">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3951,19 +3963,19 @@
         <v>45361</v>
       </c>
       <c r="C25" s="12">
-        <v>0.58819444444444446</v>
+        <v>0.84236111111111112</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="G25" s="13">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3971,19 +3983,19 @@
         <v>45361</v>
       </c>
       <c r="C26" s="12">
-        <v>0.15625</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G26" s="13">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3991,39 +4003,39 @@
         <v>45361</v>
       </c>
       <c r="C27" s="12">
-        <v>9.7222222222222224E-3</v>
+        <v>0.15625</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E27" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="G27" s="13">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="9">
-        <v>45360</v>
+        <v>45361</v>
       </c>
       <c r="C28" s="12">
-        <v>0.27291666666666664</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="G28" s="13">
-        <v>0.37</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4031,81 +4043,101 @@
         <v>45360</v>
       </c>
       <c r="C29" s="12">
-        <v>0.21458333333333332</v>
+        <v>0.27291666666666664</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G29" s="13">
-        <v>0.34</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="9">
-        <v>45359</v>
-      </c>
-      <c r="C30" s="10">
-        <v>20.32</v>
+        <v>45360</v>
+      </c>
+      <c r="C30" s="12">
+        <v>0.21458333333333332</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G30" s="13">
-        <v>0.32</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="9">
+        <v>45359</v>
+      </c>
+      <c r="C31" s="10">
+        <v>20.32</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="13">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B32" s="9">
         <v>45357</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C32" s="10">
         <v>13.26</v>
       </c>
-      <c r="D31" s="21" t="s">
+      <c r="D32" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E32" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F32" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G31" s="13">
+      <c r="G32" s="13">
         <v>0.22</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="33" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="34" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B5:E15">
+  <conditionalFormatting sqref="B5:E16">
     <cfRule type="expression" dxfId="2" priority="2">
       <formula>$A5=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16:F31">
-    <cfRule type="expression" dxfId="1" priority="14">
-      <formula>$A16=1</formula>
+  <conditionalFormatting sqref="B17:F32">
+    <cfRule type="expression" dxfId="1" priority="15">
+      <formula>$A17=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G13">
-    <cfRule type="dataBar" priority="11">
+  <conditionalFormatting sqref="G4:G14">
+    <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4118,8 +4150,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G14:G31">
-    <cfRule type="dataBar" priority="15">
+  <conditionalFormatting sqref="G15:G32">
+    <cfRule type="dataBar" priority="16">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4160,7 +4192,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G13</xm:sqref>
+          <xm:sqref>G4:G14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{272DF8F1-2D7A-C948-BB97-5E4DFA143735}">
@@ -4175,7 +4207,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G14:G31</xm:sqref>
+          <xm:sqref>G15:G32</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4218,6 +4250,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -4235,15 +4276,6 @@
     <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4547,6 +4579,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4554,14 +4594,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
     <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
GamePla(). Major Refactor. Created getPointsSwitchCase() switch case for score. Completed isEndGameCriteriaMet(0 and endGame() methods. Work on human/computer turn movement.
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E062CB4-4FDE-CD4F-A83C-411900923569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4E6B41-4EA2-9B40-88AE-939A9EC444DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
   <si>
     <t>DATE</t>
   </si>
@@ -407,6 +407,17 @@
   </si>
   <si>
     <t>MoveValidator()</t>
+  </si>
+  <si>
+    <t>endGame()</t>
+  </si>
+  <si>
+    <t>I now realise I'm not going to completely finish this project in its entirety. I realise it's about the journey - the learning, the frustration, and the joy when you've solved a problem. My concentration was so much on getting all the validation checks, I lost a lot of days. It's analogous to a 2-hour exam with 8 questions you know you can do, and two questions you can't. I was stuck and focused on the two questions I couldn't solve quickly - spending valuable time reading text material, watching youtube videos, going over past lecture notes, etc.
+Two this end, I’ve accepted that I probably won't get all the validation / placement on board, and entire game finished in time, so I’m now focused on getting as much other methods/tasks done. a possible score switch case class and pseudo coding some endgame scenarios. At least the hope is I might pick up some points here. 
+Tomorrow afternoon will purely be on getting 20 suitable J-Unit tests.</t>
+  </si>
+  <si>
+    <t>Make hay while the sun shines</t>
   </si>
 </sst>
 </file>
@@ -3002,7 +3013,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>3521028</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4772071" cy="2667000"/>
@@ -3058,13 +3069,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>4241800</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>403225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8229600</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>3394075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3102,13 +3113,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>5448300</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8242300</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>2133600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3146,13 +3157,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>241376</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>1155700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1511300</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3456,10 +3467,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3520,382 +3531,383 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" s="2" customFormat="1" ht="240" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
         <v>45371</v>
       </c>
       <c r="C4" s="12">
-        <v>0.51180555555555551</v>
+        <v>0.94305555555555554</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>87</v>
+        <v>89</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>91</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="G4" s="18">
-        <v>0.82</v>
+        <v>0.86</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="320" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="9">
         <v>45371</v>
       </c>
       <c r="C5" s="12">
-        <v>0.18055555555555555</v>
+        <v>0.51180555555555551</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G5" s="18">
-        <v>0.81399999999999995</v>
+        <v>0.82</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="320" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
         <v>45371</v>
       </c>
       <c r="C6" s="12">
-        <v>9.7222222222222224E-3</v>
+        <v>0.18055555555555555</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="22" t="s">
-        <v>82</v>
+      <c r="E6" s="23" t="s">
+        <v>85</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" s="13">
-        <v>0.81</v>
+        <v>84</v>
+      </c>
+      <c r="G6" s="18">
+        <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" s="2" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="9">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="C7" s="12">
-        <v>0.67708333333333337</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>78</v>
+        <v>83</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>82</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G7" s="13">
-        <v>0.8</v>
+        <v>0.81</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" s="2" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="9">
         <v>45370</v>
       </c>
       <c r="C8" s="12">
-        <v>0.53055555555555556</v>
+        <v>0.67708333333333337</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G8" s="13">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" s="2" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="9">
         <v>45370</v>
       </c>
       <c r="C9" s="12">
-        <v>0.10138888888888889</v>
+        <v>0.53055555555555556</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>73</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G9" s="13">
-        <v>0.75</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="9">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="C10" s="12">
-        <v>0.79652777777777772</v>
+        <v>0.10138888888888889</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G10" s="13">
-        <v>0.74</v>
+        <v>0.75</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="9">
         <v>45369</v>
       </c>
       <c r="C11" s="12">
-        <v>0.72430555555555554</v>
+        <v>0.79652777777777772</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G11" s="13">
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="9">
         <v>45369</v>
       </c>
       <c r="C12" s="12">
-        <v>0.55277777777777781</v>
+        <v>0.72430555555555554</v>
       </c>
       <c r="D12" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G12" s="13">
-        <v>0.71</v>
+        <v>0.73</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="9">
         <v>45369</v>
       </c>
       <c r="C13" s="12">
-        <v>0.22291666666666668</v>
+        <v>0.55277777777777781</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>66</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G13" s="13">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="9">
         <v>45369</v>
       </c>
       <c r="C14" s="12">
-        <v>5.8333333333333334E-2</v>
+        <v>0.22291666666666668</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G14" s="13">
-        <v>0.69</v>
+        <v>0.7</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="9">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="C15" s="12">
-        <v>0.96458333333333335</v>
+        <v>5.8333333333333334E-2</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="18">
-        <v>0.68500000000000005</v>
+        <v>61</v>
+      </c>
+      <c r="G15" s="13">
+        <v>0.69</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="9">
         <v>45368</v>
       </c>
       <c r="C16" s="12">
-        <v>0.79374999999999996</v>
+        <v>0.96458333333333335</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G16" s="13">
-        <v>0.67</v>
+        <v>58</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="18">
+        <v>0.68500000000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="9">
         <v>45368</v>
       </c>
       <c r="C17" s="12">
-        <v>0.44027777777777777</v>
+        <v>0.79374999999999996</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="G17" s="13">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
       <c r="B18" s="9">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="C18" s="12">
-        <v>7.0833333333333331E-2</v>
+        <v>0.44027777777777777</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G18" s="13">
-        <v>0.64</v>
-      </c>
-      <c r="I18" s="15"/>
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="19" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
       <c r="B19" s="9">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="C19" s="12">
-        <v>0.98611111111111116</v>
+        <v>7.0833333333333331E-2</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G19" s="13">
-        <v>0.63</v>
-      </c>
+        <v>0.64</v>
+      </c>
+      <c r="I19" s="15"/>
     </row>
     <row r="20" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
       <c r="B20" s="9">
+        <v>45366</v>
+      </c>
+      <c r="C20" s="12">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="13">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="1"/>
+      <c r="B21" s="9">
         <v>45365</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C21" s="12">
         <v>2.1527777777777778E-2</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D21" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E21" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F21" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G21" s="13">
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="9">
-        <v>45364</v>
-      </c>
-      <c r="C21" s="12">
-        <v>0.35138888888888886</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G21" s="13">
-        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3903,59 +3915,59 @@
         <v>45364</v>
       </c>
       <c r="C22" s="12">
-        <v>0.22708333333333333</v>
+        <v>0.35138888888888886</v>
       </c>
       <c r="D22" s="21" t="s">
         <v>37</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G22" s="13">
-        <v>0.56000000000000005</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="9">
-        <v>45363</v>
+        <v>45364</v>
       </c>
       <c r="C23" s="12">
-        <v>0.56666666666666665</v>
+        <v>0.22708333333333333</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G23" s="13">
-        <v>0.54</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="9">
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="C24" s="12">
-        <v>0.95208333333333328</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G24" s="13">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3963,19 +3975,19 @@
         <v>45361</v>
       </c>
       <c r="C25" s="12">
-        <v>0.84236111111111112</v>
+        <v>0.95208333333333328</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G25" s="13">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3983,19 +3995,19 @@
         <v>45361</v>
       </c>
       <c r="C26" s="12">
-        <v>0.58819444444444446</v>
+        <v>0.84236111111111112</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="G26" s="13">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4003,19 +4015,19 @@
         <v>45361</v>
       </c>
       <c r="C27" s="12">
-        <v>0.15625</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G27" s="13">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4023,39 +4035,39 @@
         <v>45361</v>
       </c>
       <c r="C28" s="12">
-        <v>9.7222222222222224E-3</v>
+        <v>0.15625</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="G28" s="13">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="9">
-        <v>45360</v>
+        <v>45361</v>
       </c>
       <c r="C29" s="12">
-        <v>0.27291666666666664</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="G29" s="13">
-        <v>0.37</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4063,81 +4075,101 @@
         <v>45360</v>
       </c>
       <c r="C30" s="12">
-        <v>0.21458333333333332</v>
+        <v>0.27291666666666664</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G30" s="13">
-        <v>0.34</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="9">
-        <v>45359</v>
-      </c>
-      <c r="C31" s="10">
-        <v>20.32</v>
+        <v>45360</v>
+      </c>
+      <c r="C31" s="12">
+        <v>0.21458333333333332</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G31" s="13">
-        <v>0.32</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="9">
+        <v>45359</v>
+      </c>
+      <c r="C32" s="10">
+        <v>20.32</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="13">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B33" s="9">
         <v>45357</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C33" s="10">
         <v>13.26</v>
       </c>
-      <c r="D32" s="21" t="s">
+      <c r="D33" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E32" s="21" t="s">
+      <c r="E33" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F33" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G32" s="13">
+      <c r="G33" s="13">
         <v>0.22</v>
       </c>
     </row>
-    <row r="33" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="34" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="34" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="35" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B5:E16">
+  <conditionalFormatting sqref="B5:E17">
     <cfRule type="expression" dxfId="2" priority="2">
       <formula>$A5=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17:F32">
-    <cfRule type="expression" dxfId="1" priority="15">
-      <formula>$A17=1</formula>
+  <conditionalFormatting sqref="B18:F33">
+    <cfRule type="expression" dxfId="1" priority="16">
+      <formula>$A18=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G14">
-    <cfRule type="dataBar" priority="12">
+  <conditionalFormatting sqref="G4:G15">
+    <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4150,8 +4182,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G15:G32">
-    <cfRule type="dataBar" priority="16">
+  <conditionalFormatting sqref="G16:G33">
+    <cfRule type="dataBar" priority="17">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4192,7 +4224,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G14</xm:sqref>
+          <xm:sqref>G4:G15</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{272DF8F1-2D7A-C948-BB97-5E4DFA143735}">
@@ -4207,7 +4239,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G15:G32</xm:sqref>
+          <xm:sqref>G16:G33</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4250,15 +4282,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -4276,6 +4299,15 @@
     <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4579,14 +4611,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4594,6 +4618,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
     <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
ComputerPlayer() : AI and Logic.  Built a solution was to implement some kind of pattern matching function for AI  and  a HashMap data structure. The  AI would use  this by extracting numbers and letters from its tiles with a regex and matching the integers against the integers in my newly created switch case statement. Also plan to utilise the switch case statement in Player class for score tallying.
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4E6B41-4EA2-9B40-88AE-939A9EC444DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DD487C-12CF-EB46-B569-366CEA7A434D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="95">
   <si>
     <t>DATE</t>
   </si>
@@ -412,12 +412,34 @@
     <t>endGame()</t>
   </si>
   <si>
+    <t>Make hay while the sun shines</t>
+  </si>
+  <si>
+    <t>Do Robots dream of sheep?</t>
+  </si>
+  <si>
+    <t>ComputerPlayer()  logic and AI</t>
+  </si>
+  <si>
     <t>I now realise I'm not going to completely finish this project in its entirety. I realise it's about the journey - the learning, the frustration, and the joy when you've solved a problem. My concentration was so much on getting all the validation checks, I lost a lot of days. It's analogous to a 2-hour exam with 8 questions you know you can do, and two questions you can't. I was stuck and focused on the two questions I couldn't solve quickly - spending valuable time reading text material, watching youtube videos, going over past lecture notes, etc.
-Two this end, I’ve accepted that I probably won't get all the validation / placement on board, and entire game finished in time, so I’m now focused on getting as much other methods/tasks done. a possible score switch case class and pseudo coding some endgame scenarios. At least the hope is I might pick up some points here. 
+To this end, I’ve accepted that I probably won't get all the validation / placement on board, and entire game finished in time, so I’m now focused on getting as much other methods/tasks done. a possible score switch case class and pseudo coding some endgame scenarios. At least the hope is I might pick up some points here. 
 Tomorrow afternoon will purely be on getting 20 suitable J-Unit tests.</t>
   </si>
   <si>
-    <t>Make hay while the sun shines</t>
+    <t>I've been feeling like a robot lately, and certainly had not much 
+sleep. Philip K. Dick would be proud.
+Been doing a lot of reading as to how I can get the computer to 
+dream of a word, not only just a word, but the highest scoring word. 
+My idea for a solution was to implement some kind of pattern 
+matching function for AI  and  a HashMap data structure. The  
+AI would use  this by extracting numbers and letters from its tiles 
+with a regex and matching the integers against the integers in my 
+newly created switch case statement. Initially thought that with 
+seven tiles, a bin srearch data structure to split pick tiles 
+recursively - but quickly realised - they are not ordered. So as only seven tiles, iteratiing over a simple ArrayList will do. 
+Also, having implemented the getPointsSwitchCase switch case method in 
+the Player class - my thinking is to use this to calculate scores when tiles placed on the board. 
+Vey much a work in progress and very novel for me. With one day to go, i realise i'm not going to pull this off and complete the whole game. But have had fun trying and learning (and pulling my hair out !) - Reminds me of all those old Hackathon weekends ...</t>
   </si>
 </sst>
 </file>
@@ -830,14 +852,7 @@
     <cellStyle name="Phone" xfId="8" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Title" xfId="7" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <b/>
@@ -924,10 +939,10 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Library Book Checkout Sheet" defaultPivotStyle="PivotStyleMedium9">
     <tableStyle name="Library Book Checkout Sheet" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="6"/>
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="firstColumn" dxfId="4"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="3"/>
+      <tableStyleElement type="wholeTable" dxfId="5"/>
+      <tableStyleElement type="headerRow" dxfId="4"/>
+      <tableStyleElement type="firstColumn" dxfId="3"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="2"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -3013,7 +3028,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>3521028</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4772071" cy="2667000"/>
@@ -3069,13 +3084,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>4241800</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>403225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8229600</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>3394075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3113,13 +3128,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>5448300</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8242300</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>2133600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3157,13 +3172,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>241376</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>1155700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1511300</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3189,6 +3204,50 @@
         <a:xfrm>
           <a:off x="4064076" y="3213100"/>
           <a:ext cx="1269924" cy="1358900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5664200</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>215900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>8204200</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2603500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FAACEE1-E6EE-FA00-ED86-69395E6D043A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11214100" y="2273300"/>
+          <a:ext cx="2540000" cy="2387600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3467,10 +3526,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3478,7 +3537,7 @@
     <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="93.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="24.140625" style="1" customWidth="1"/>
@@ -3495,7 +3554,7 @@
       <c r="E1" s="25"/>
       <c r="F1" s="29" t="str">
         <f ca="1">'Target '!A2-'Target '!A1&amp;" days remaining"</f>
-        <v>-2 days remaining</v>
+        <v>-1 days remaining</v>
       </c>
       <c r="G1" s="30"/>
     </row>
@@ -3531,403 +3590,404 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="240" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" s="2" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="C4" s="12">
-        <v>0.94305555555555554</v>
+        <v>0.28472222222222221</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E4" s="20" t="s">
         <v>91</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="G4" s="18">
-        <v>0.86</v>
+        <v>0.87</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="240" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="9">
         <v>45371</v>
       </c>
       <c r="C5" s="12">
-        <v>0.51180555555555551</v>
+        <v>0.94305555555555554</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>87</v>
+        <v>89</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>90</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="G5" s="18">
-        <v>0.82</v>
+        <v>0.86</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" ht="320" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
         <v>45371</v>
       </c>
       <c r="C6" s="12">
-        <v>0.18055555555555555</v>
+        <v>0.51180555555555551</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G6" s="18">
-        <v>0.81399999999999995</v>
+        <v>0.82</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" s="2" customFormat="1" ht="320" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="9">
         <v>45371</v>
       </c>
       <c r="C7" s="12">
-        <v>9.7222222222222224E-3</v>
+        <v>0.18055555555555555</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="22" t="s">
-        <v>82</v>
+      <c r="E7" s="23" t="s">
+        <v>85</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="G7" s="13">
-        <v>0.81</v>
+        <v>84</v>
+      </c>
+      <c r="G7" s="18">
+        <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" s="2" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="9">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="C8" s="12">
-        <v>0.67708333333333337</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>78</v>
+        <v>83</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>82</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G8" s="13">
-        <v>0.8</v>
+        <v>0.81</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" s="2" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="9">
         <v>45370</v>
       </c>
       <c r="C9" s="12">
-        <v>0.53055555555555556</v>
+        <v>0.67708333333333337</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G9" s="13">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" s="2" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="9">
         <v>45370</v>
       </c>
       <c r="C10" s="12">
-        <v>0.10138888888888889</v>
+        <v>0.53055555555555556</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>73</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G10" s="13">
-        <v>0.75</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="9">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="C11" s="12">
-        <v>0.79652777777777772</v>
+        <v>0.10138888888888889</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G11" s="13">
-        <v>0.74</v>
+        <v>0.75</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="9">
         <v>45369</v>
       </c>
       <c r="C12" s="12">
-        <v>0.72430555555555554</v>
+        <v>0.79652777777777772</v>
       </c>
       <c r="D12" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G12" s="13">
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="9">
         <v>45369</v>
       </c>
       <c r="C13" s="12">
-        <v>0.55277777777777781</v>
+        <v>0.72430555555555554</v>
       </c>
       <c r="D13" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G13" s="13">
-        <v>0.71</v>
+        <v>0.73</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="9">
         <v>45369</v>
       </c>
       <c r="C14" s="12">
-        <v>0.22291666666666668</v>
+        <v>0.55277777777777781</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E14" s="20" t="s">
         <v>66</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G14" s="13">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="9">
         <v>45369</v>
       </c>
       <c r="C15" s="12">
-        <v>5.8333333333333334E-2</v>
+        <v>0.22291666666666668</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G15" s="13">
-        <v>0.69</v>
+        <v>0.7</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="9">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="C16" s="12">
-        <v>0.96458333333333335</v>
+        <v>5.8333333333333334E-2</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" s="18">
-        <v>0.68500000000000005</v>
+        <v>61</v>
+      </c>
+      <c r="G16" s="13">
+        <v>0.69</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="9">
         <v>45368</v>
       </c>
       <c r="C17" s="12">
-        <v>0.79374999999999996</v>
+        <v>0.96458333333333335</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G17" s="13">
-        <v>0.67</v>
+        <v>58</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="18">
+        <v>0.68500000000000005</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
       <c r="B18" s="9">
         <v>45368</v>
       </c>
       <c r="C18" s="12">
-        <v>0.44027777777777777</v>
+        <v>0.79374999999999996</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="G18" s="13">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
       <c r="B19" s="9">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="C19" s="12">
-        <v>7.0833333333333331E-2</v>
+        <v>0.44027777777777777</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G19" s="13">
-        <v>0.64</v>
-      </c>
-      <c r="I19" s="15"/>
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="20" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
       <c r="B20" s="9">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="C20" s="12">
-        <v>0.98611111111111116</v>
+        <v>7.0833333333333331E-2</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G20" s="13">
-        <v>0.63</v>
-      </c>
+        <v>0.64</v>
+      </c>
+      <c r="I20" s="15"/>
     </row>
     <row r="21" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
       <c r="B21" s="9">
+        <v>45366</v>
+      </c>
+      <c r="C21" s="12">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="13">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="1"/>
+      <c r="B22" s="9">
         <v>45365</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C22" s="12">
         <v>2.1527777777777778E-2</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="D22" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E22" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F22" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G22" s="13">
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="9">
-        <v>45364</v>
-      </c>
-      <c r="C22" s="12">
-        <v>0.35138888888888886</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G22" s="13">
-        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3935,59 +3995,59 @@
         <v>45364</v>
       </c>
       <c r="C23" s="12">
-        <v>0.22708333333333333</v>
+        <v>0.35138888888888886</v>
       </c>
       <c r="D23" s="21" t="s">
         <v>37</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G23" s="13">
-        <v>0.56000000000000005</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="9">
-        <v>45363</v>
+        <v>45364</v>
       </c>
       <c r="C24" s="12">
-        <v>0.56666666666666665</v>
+        <v>0.22708333333333333</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G24" s="13">
-        <v>0.54</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="9">
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="C25" s="12">
-        <v>0.95208333333333328</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G25" s="13">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -3995,19 +4055,19 @@
         <v>45361</v>
       </c>
       <c r="C26" s="12">
-        <v>0.84236111111111112</v>
+        <v>0.95208333333333328</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G26" s="13">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4015,19 +4075,19 @@
         <v>45361</v>
       </c>
       <c r="C27" s="12">
-        <v>0.58819444444444446</v>
+        <v>0.84236111111111112</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="G27" s="13">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4035,19 +4095,19 @@
         <v>45361</v>
       </c>
       <c r="C28" s="12">
-        <v>0.15625</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G28" s="13">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4055,39 +4115,39 @@
         <v>45361</v>
       </c>
       <c r="C29" s="12">
-        <v>9.7222222222222224E-3</v>
+        <v>0.15625</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="G29" s="13">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="9">
-        <v>45360</v>
+        <v>45361</v>
       </c>
       <c r="C30" s="12">
-        <v>0.27291666666666664</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="G30" s="13">
-        <v>0.37</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4095,81 +4155,101 @@
         <v>45360</v>
       </c>
       <c r="C31" s="12">
-        <v>0.21458333333333332</v>
+        <v>0.27291666666666664</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G31" s="13">
-        <v>0.34</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="9">
-        <v>45359</v>
-      </c>
-      <c r="C32" s="10">
-        <v>20.32</v>
+        <v>45360</v>
+      </c>
+      <c r="C32" s="12">
+        <v>0.21458333333333332</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G32" s="13">
-        <v>0.32</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="9">
+        <v>45359</v>
+      </c>
+      <c r="C33" s="10">
+        <v>20.32</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="13">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B34" s="9">
         <v>45357</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C34" s="10">
         <v>13.26</v>
       </c>
-      <c r="D33" s="21" t="s">
+      <c r="D34" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E33" s="21" t="s">
+      <c r="E34" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="F34" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G33" s="13">
+      <c r="G34" s="13">
         <v>0.22</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="35" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="36" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B5:E17">
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>$A5=1</formula>
+  <conditionalFormatting sqref="B4:E18">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B18:F33">
-    <cfRule type="expression" dxfId="1" priority="16">
-      <formula>$A18=1</formula>
+  <conditionalFormatting sqref="B19:F34">
+    <cfRule type="expression" dxfId="0" priority="17">
+      <formula>$A19=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G15">
-    <cfRule type="dataBar" priority="13">
+  <conditionalFormatting sqref="G4:G16">
+    <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4182,8 +4262,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G16:G33">
-    <cfRule type="dataBar" priority="17">
+  <conditionalFormatting sqref="G17:G34">
+    <cfRule type="dataBar" priority="18">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4194,11 +4274,6 @@
           <x14:id>{272DF8F1-2D7A-C948-BB97-5E4DFA143735}</x14:id>
         </ext>
       </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4:E4">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
@@ -4224,7 +4299,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G15</xm:sqref>
+          <xm:sqref>G4:G16</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{272DF8F1-2D7A-C948-BB97-5E4DFA143735}">
@@ -4239,7 +4314,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G16:G33</xm:sqref>
+          <xm:sqref>G17:G34</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4270,7 +4345,7 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45371</v>
+        <v>45372</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
ComputerPlayer() : Work through computer AI logic. Clean up some of the game logic regarding validation. Focus on board placement, scoring, and computer turn.
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DD487C-12CF-EB46-B569-366CEA7A434D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7166AE12-650A-8C47-AF49-127ED094099F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="97">
   <si>
     <t>DATE</t>
   </si>
@@ -440,6 +440,14 @@
 Also, having implemented the getPointsSwitchCase switch case method in 
 the Player class - my thinking is to use this to calculate scores when tiles placed on the board. 
 Vey much a work in progress and very novel for me. With one day to go, i realise i'm not going to pull this off and complete the whole game. But have had fun trying and learning (and pulling my hair out !) - Reminds me of all those old Hackathon weekends ...</t>
+  </si>
+  <si>
+    <t>OK Computer !</t>
+  </si>
+  <si>
+    <t>Still working through computer AI logic… and listening to some mournful Radiohead.
+Cleaned up some of the game logic regarding validation. Need to really focus on board placement, scoring, and computer turn.
+God loves his children !</t>
   </si>
 </sst>
 </file>
@@ -852,7 +860,14 @@
     <cellStyle name="Phone" xfId="8" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Title" xfId="7" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -939,10 +954,10 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Library Book Checkout Sheet" defaultPivotStyle="PivotStyleMedium9">
     <tableStyle name="Library Book Checkout Sheet" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="5"/>
-      <tableStyleElement type="headerRow" dxfId="4"/>
-      <tableStyleElement type="firstColumn" dxfId="3"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="2"/>
+      <tableStyleElement type="wholeTable" dxfId="6"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="firstColumn" dxfId="4"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="3"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -3028,7 +3043,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>3521028</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4772071" cy="2667000"/>
@@ -3084,13 +3099,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>4241800</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>403225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8229600</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>3394075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3128,13 +3143,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>5448300</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8242300</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>2133600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3172,13 +3187,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>241376</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>1155700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1511300</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3216,13 +3231,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>5664200</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>215900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8204200</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>2603500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3526,10 +3541,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3590,424 +3605,425 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" s="2" customFormat="1" ht="201" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
         <v>45372</v>
       </c>
       <c r="C4" s="12">
-        <v>0.28472222222222221</v>
+        <v>0.60972222222222228</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>92</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G4" s="18">
-        <v>0.87</v>
+        <v>0.88</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="240" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="9">
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="C5" s="12">
-        <v>0.94305555555555554</v>
+        <v>0.28472222222222221</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G5" s="18">
-        <v>0.86</v>
+        <v>0.87</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="240" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
         <v>45371</v>
       </c>
       <c r="C6" s="12">
-        <v>0.51180555555555551</v>
+        <v>0.94305555555555554</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>87</v>
+        <v>89</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>90</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="G6" s="18">
-        <v>0.82</v>
+        <v>0.86</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="320" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" s="2" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="9">
         <v>45371</v>
       </c>
       <c r="C7" s="12">
-        <v>0.18055555555555555</v>
+        <v>0.51180555555555551</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G7" s="18">
-        <v>0.81399999999999995</v>
+        <v>0.82</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" s="2" customFormat="1" ht="320" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="9">
         <v>45371</v>
       </c>
       <c r="C8" s="12">
-        <v>9.7222222222222224E-3</v>
+        <v>0.18055555555555555</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="22" t="s">
-        <v>82</v>
+      <c r="E8" s="23" t="s">
+        <v>85</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="G8" s="13">
-        <v>0.81</v>
+        <v>84</v>
+      </c>
+      <c r="G8" s="18">
+        <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" s="2" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="9">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="C9" s="12">
-        <v>0.67708333333333337</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>78</v>
+        <v>83</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>82</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G9" s="13">
-        <v>0.8</v>
+        <v>0.81</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" s="2" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="9">
         <v>45370</v>
       </c>
       <c r="C10" s="12">
-        <v>0.53055555555555556</v>
+        <v>0.67708333333333337</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G10" s="13">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" s="2" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="9">
         <v>45370</v>
       </c>
       <c r="C11" s="12">
-        <v>0.10138888888888889</v>
+        <v>0.53055555555555556</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>73</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G11" s="13">
-        <v>0.75</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="9">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="C12" s="12">
-        <v>0.79652777777777772</v>
+        <v>0.10138888888888889</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G12" s="13">
-        <v>0.74</v>
+        <v>0.75</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="9">
         <v>45369</v>
       </c>
       <c r="C13" s="12">
-        <v>0.72430555555555554</v>
+        <v>0.79652777777777772</v>
       </c>
       <c r="D13" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G13" s="13">
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="9">
         <v>45369</v>
       </c>
       <c r="C14" s="12">
-        <v>0.55277777777777781</v>
+        <v>0.72430555555555554</v>
       </c>
       <c r="D14" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G14" s="13">
-        <v>0.71</v>
+        <v>0.73</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="9">
         <v>45369</v>
       </c>
       <c r="C15" s="12">
-        <v>0.22291666666666668</v>
+        <v>0.55277777777777781</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E15" s="20" t="s">
         <v>66</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G15" s="13">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="9">
         <v>45369</v>
       </c>
       <c r="C16" s="12">
-        <v>5.8333333333333334E-2</v>
+        <v>0.22291666666666668</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G16" s="13">
-        <v>0.69</v>
+        <v>0.7</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="9">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="C17" s="12">
-        <v>0.96458333333333335</v>
+        <v>5.8333333333333334E-2</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="G17" s="18">
-        <v>0.68500000000000005</v>
+        <v>61</v>
+      </c>
+      <c r="G17" s="13">
+        <v>0.69</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
       <c r="B18" s="9">
         <v>45368</v>
       </c>
       <c r="C18" s="12">
-        <v>0.79374999999999996</v>
+        <v>0.96458333333333335</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G18" s="13">
-        <v>0.67</v>
+        <v>58</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" s="18">
+        <v>0.68500000000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
       <c r="B19" s="9">
         <v>45368</v>
       </c>
       <c r="C19" s="12">
-        <v>0.44027777777777777</v>
+        <v>0.79374999999999996</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="G19" s="13">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
       <c r="B20" s="9">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="C20" s="12">
-        <v>7.0833333333333331E-2</v>
+        <v>0.44027777777777777</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G20" s="13">
-        <v>0.64</v>
-      </c>
-      <c r="I20" s="15"/>
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="21" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
       <c r="B21" s="9">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="C21" s="12">
-        <v>0.98611111111111116</v>
+        <v>7.0833333333333331E-2</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G21" s="13">
-        <v>0.63</v>
-      </c>
+        <v>0.64</v>
+      </c>
+      <c r="I21" s="15"/>
     </row>
     <row r="22" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
       <c r="B22" s="9">
+        <v>45366</v>
+      </c>
+      <c r="C22" s="12">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22" s="13">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="1"/>
+      <c r="B23" s="9">
         <v>45365</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C23" s="12">
         <v>2.1527777777777778E-2</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="D23" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E23" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F23" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G23" s="13">
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="9">
-        <v>45364</v>
-      </c>
-      <c r="C23" s="12">
-        <v>0.35138888888888886</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G23" s="13">
-        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4015,59 +4031,59 @@
         <v>45364</v>
       </c>
       <c r="C24" s="12">
-        <v>0.22708333333333333</v>
+        <v>0.35138888888888886</v>
       </c>
       <c r="D24" s="21" t="s">
         <v>37</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G24" s="13">
-        <v>0.56000000000000005</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="9">
-        <v>45363</v>
+        <v>45364</v>
       </c>
       <c r="C25" s="12">
-        <v>0.56666666666666665</v>
+        <v>0.22708333333333333</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G25" s="13">
-        <v>0.54</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="9">
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="C26" s="12">
-        <v>0.95208333333333328</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G26" s="13">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4075,19 +4091,19 @@
         <v>45361</v>
       </c>
       <c r="C27" s="12">
-        <v>0.84236111111111112</v>
+        <v>0.95208333333333328</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G27" s="13">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4095,19 +4111,19 @@
         <v>45361</v>
       </c>
       <c r="C28" s="12">
-        <v>0.58819444444444446</v>
+        <v>0.84236111111111112</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="G28" s="13">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4115,19 +4131,19 @@
         <v>45361</v>
       </c>
       <c r="C29" s="12">
-        <v>0.15625</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G29" s="13">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4135,39 +4151,39 @@
         <v>45361</v>
       </c>
       <c r="C30" s="12">
-        <v>9.7222222222222224E-3</v>
+        <v>0.15625</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E30" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="G30" s="13">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="9">
-        <v>45360</v>
+        <v>45361</v>
       </c>
       <c r="C31" s="12">
-        <v>0.27291666666666664</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="G31" s="13">
-        <v>0.37</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4175,81 +4191,101 @@
         <v>45360</v>
       </c>
       <c r="C32" s="12">
-        <v>0.21458333333333332</v>
+        <v>0.27291666666666664</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G32" s="13">
-        <v>0.34</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="9">
-        <v>45359</v>
-      </c>
-      <c r="C33" s="10">
-        <v>20.32</v>
+        <v>45360</v>
+      </c>
+      <c r="C33" s="12">
+        <v>0.21458333333333332</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G33" s="13">
-        <v>0.32</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="9">
+        <v>45359</v>
+      </c>
+      <c r="C34" s="10">
+        <v>20.32</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" s="13">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B35" s="9">
         <v>45357</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C35" s="10">
         <v>13.26</v>
       </c>
-      <c r="D34" s="21" t="s">
+      <c r="D35" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="21" t="s">
+      <c r="E35" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F34" s="11" t="s">
+      <c r="F35" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G34" s="13">
+      <c r="G35" s="13">
         <v>0.22</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="36" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="37" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:E18">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>$A4=1</formula>
+  <conditionalFormatting sqref="B5:E19">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$A5=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19:F34">
-    <cfRule type="expression" dxfId="0" priority="17">
-      <formula>$A19=1</formula>
+  <conditionalFormatting sqref="B20:F35">
+    <cfRule type="expression" dxfId="1" priority="18">
+      <formula>$A20=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G16">
-    <cfRule type="dataBar" priority="14">
+  <conditionalFormatting sqref="G4:G17">
+    <cfRule type="dataBar" priority="15">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4262,8 +4298,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G17:G34">
-    <cfRule type="dataBar" priority="18">
+  <conditionalFormatting sqref="G18:G35">
+    <cfRule type="dataBar" priority="19">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4274,6 +4310,11 @@
           <x14:id>{272DF8F1-2D7A-C948-BB97-5E4DFA143735}</x14:id>
         </ext>
       </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:E4">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
@@ -4299,7 +4340,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G16</xm:sqref>
+          <xm:sqref>G4:G17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{272DF8F1-2D7A-C948-BB97-5E4DFA143735}">
@@ -4314,7 +4355,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G17:G34</xm:sqref>
+          <xm:sqref>G18:G35</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4357,6 +4398,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -4374,15 +4424,6 @@
     <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4686,6 +4727,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4693,14 +4742,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
     <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
GamePlay() : Work on gameplay logic, and slowly working computer moves into the game. One thing I've learned - Preventing null references by assigning an empty string, is a thing of beauty !
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7166AE12-650A-8C47-AF49-127ED094099F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFAE1E7-8177-E846-B909-35EA7EF2FE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="99">
   <si>
     <t>DATE</t>
   </si>
@@ -448,6 +448,12 @@
     <t>Still working through computer AI logic… and listening to some mournful Radiohead.
 Cleaned up some of the game logic regarding validation. Need to really focus on board placement, scoring, and computer turn.
 God loves his children !</t>
+  </si>
+  <si>
+    <t>One thing I've learned - Preventing null references by assigning an empty string, is a thing of beauty !</t>
+  </si>
+  <si>
+    <t>String theory</t>
   </si>
 </sst>
 </file>
@@ -3043,7 +3049,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>3521028</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4772071" cy="2667000"/>
@@ -3099,13 +3105,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>4241800</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>403225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8229600</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>3394075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3143,13 +3149,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>5448300</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8242300</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>2133600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3187,13 +3193,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>241376</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>1155700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1511300</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3231,13 +3237,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>5664200</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>215900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8204200</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>2603500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3541,10 +3547,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3605,445 +3611,446 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="201" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" s="2" customFormat="1" ht="169" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
         <v>45372</v>
       </c>
       <c r="C4" s="12">
-        <v>0.60972222222222228</v>
+        <v>0.61944444444444446</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G4" s="18">
-        <v>0.88</v>
+        <v>0.88500000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="201" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="9">
         <v>45372</v>
       </c>
       <c r="C5" s="12">
-        <v>0.28472222222222221</v>
+        <v>0.60972222222222228</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>92</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G5" s="18">
-        <v>0.87</v>
+        <v>0.88</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" ht="240" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="C6" s="12">
-        <v>0.94305555555555554</v>
+        <v>0.28472222222222221</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G6" s="18">
-        <v>0.86</v>
+        <v>0.87</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" s="2" customFormat="1" ht="240" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="9">
         <v>45371</v>
       </c>
       <c r="C7" s="12">
-        <v>0.51180555555555551</v>
+        <v>0.94305555555555554</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>87</v>
+        <v>89</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>90</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="G7" s="18">
-        <v>0.82</v>
+        <v>0.86</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" ht="320" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" s="2" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="9">
         <v>45371</v>
       </c>
       <c r="C8" s="12">
-        <v>0.18055555555555555</v>
+        <v>0.51180555555555551</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G8" s="18">
-        <v>0.81399999999999995</v>
+        <v>0.82</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" s="2" customFormat="1" ht="320" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="9">
         <v>45371</v>
       </c>
       <c r="C9" s="12">
-        <v>9.7222222222222224E-3</v>
+        <v>0.18055555555555555</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="E9" s="22" t="s">
-        <v>82</v>
+      <c r="E9" s="23" t="s">
+        <v>85</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="G9" s="13">
-        <v>0.81</v>
+        <v>84</v>
+      </c>
+      <c r="G9" s="18">
+        <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" s="2" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="9">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="C10" s="12">
-        <v>0.67708333333333337</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>78</v>
+        <v>83</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>82</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G10" s="13">
-        <v>0.8</v>
+        <v>0.81</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" s="2" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="9">
         <v>45370</v>
       </c>
       <c r="C11" s="12">
-        <v>0.53055555555555556</v>
+        <v>0.67708333333333337</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G11" s="13">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" s="2" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="9">
         <v>45370</v>
       </c>
       <c r="C12" s="12">
-        <v>0.10138888888888889</v>
+        <v>0.53055555555555556</v>
       </c>
       <c r="D12" s="21" t="s">
         <v>73</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G12" s="13">
-        <v>0.75</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="9">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="C13" s="12">
-        <v>0.79652777777777772</v>
+        <v>0.10138888888888889</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G13" s="13">
-        <v>0.74</v>
+        <v>0.75</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="9">
         <v>45369</v>
       </c>
       <c r="C14" s="12">
-        <v>0.72430555555555554</v>
+        <v>0.79652777777777772</v>
       </c>
       <c r="D14" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G14" s="13">
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="9">
         <v>45369</v>
       </c>
       <c r="C15" s="12">
-        <v>0.55277777777777781</v>
+        <v>0.72430555555555554</v>
       </c>
       <c r="D15" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G15" s="13">
-        <v>0.71</v>
+        <v>0.73</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="9">
         <v>45369</v>
       </c>
       <c r="C16" s="12">
-        <v>0.22291666666666668</v>
+        <v>0.55277777777777781</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>66</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G16" s="13">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="9">
         <v>45369</v>
       </c>
       <c r="C17" s="12">
-        <v>5.8333333333333334E-2</v>
+        <v>0.22291666666666668</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G17" s="13">
-        <v>0.69</v>
+        <v>0.7</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
       <c r="B18" s="9">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="C18" s="12">
-        <v>0.96458333333333335</v>
+        <v>5.8333333333333334E-2</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="G18" s="18">
-        <v>0.68500000000000005</v>
+        <v>61</v>
+      </c>
+      <c r="G18" s="13">
+        <v>0.69</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
       <c r="B19" s="9">
         <v>45368</v>
       </c>
       <c r="C19" s="12">
-        <v>0.79374999999999996</v>
+        <v>0.96458333333333335</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" s="13">
-        <v>0.67</v>
+        <v>58</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" s="18">
+        <v>0.68500000000000005</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
       <c r="B20" s="9">
         <v>45368</v>
       </c>
       <c r="C20" s="12">
-        <v>0.44027777777777777</v>
+        <v>0.79374999999999996</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="G20" s="13">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
       <c r="B21" s="9">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="C21" s="12">
-        <v>7.0833333333333331E-2</v>
+        <v>0.44027777777777777</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G21" s="13">
-        <v>0.64</v>
-      </c>
-      <c r="I21" s="15"/>
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="22" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
       <c r="B22" s="9">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="C22" s="12">
-        <v>0.98611111111111116</v>
+        <v>7.0833333333333331E-2</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G22" s="13">
-        <v>0.63</v>
-      </c>
+        <v>0.64</v>
+      </c>
+      <c r="I22" s="15"/>
     </row>
     <row r="23" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
       <c r="B23" s="9">
+        <v>45366</v>
+      </c>
+      <c r="C23" s="12">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" s="13">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="1"/>
+      <c r="B24" s="9">
         <v>45365</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C24" s="12">
         <v>2.1527777777777778E-2</v>
       </c>
-      <c r="D23" s="21" t="s">
+      <c r="D24" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E24" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F24" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G23" s="13">
+      <c r="G24" s="13">
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="9">
-        <v>45364</v>
-      </c>
-      <c r="C24" s="12">
-        <v>0.35138888888888886</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G24" s="13">
-        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4051,59 +4058,59 @@
         <v>45364</v>
       </c>
       <c r="C25" s="12">
-        <v>0.22708333333333333</v>
+        <v>0.35138888888888886</v>
       </c>
       <c r="D25" s="21" t="s">
         <v>37</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G25" s="13">
-        <v>0.56000000000000005</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="9">
-        <v>45363</v>
+        <v>45364</v>
       </c>
       <c r="C26" s="12">
-        <v>0.56666666666666665</v>
+        <v>0.22708333333333333</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G26" s="13">
-        <v>0.54</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="9">
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="C27" s="12">
-        <v>0.95208333333333328</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G27" s="13">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4111,19 +4118,19 @@
         <v>45361</v>
       </c>
       <c r="C28" s="12">
-        <v>0.84236111111111112</v>
+        <v>0.95208333333333328</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G28" s="13">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4131,19 +4138,19 @@
         <v>45361</v>
       </c>
       <c r="C29" s="12">
-        <v>0.58819444444444446</v>
+        <v>0.84236111111111112</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="G29" s="13">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4151,19 +4158,19 @@
         <v>45361</v>
       </c>
       <c r="C30" s="12">
-        <v>0.15625</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G30" s="13">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4171,39 +4178,39 @@
         <v>45361</v>
       </c>
       <c r="C31" s="12">
-        <v>9.7222222222222224E-3</v>
+        <v>0.15625</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E31" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="G31" s="13">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="9">
-        <v>45360</v>
+        <v>45361</v>
       </c>
       <c r="C32" s="12">
-        <v>0.27291666666666664</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="G32" s="13">
-        <v>0.37</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4211,81 +4218,101 @@
         <v>45360</v>
       </c>
       <c r="C33" s="12">
-        <v>0.21458333333333332</v>
+        <v>0.27291666666666664</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G33" s="13">
-        <v>0.34</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="9">
-        <v>45359</v>
-      </c>
-      <c r="C34" s="10">
-        <v>20.32</v>
+        <v>45360</v>
+      </c>
+      <c r="C34" s="12">
+        <v>0.21458333333333332</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G34" s="13">
-        <v>0.32</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B35" s="9">
+        <v>45359</v>
+      </c>
+      <c r="C35" s="10">
+        <v>20.32</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" s="13">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B36" s="9">
         <v>45357</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C36" s="10">
         <v>13.26</v>
       </c>
-      <c r="D35" s="21" t="s">
+      <c r="D36" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E35" s="21" t="s">
+      <c r="E36" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F36" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G35" s="13">
+      <c r="G36" s="13">
         <v>0.22</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="37" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="38" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B5:E19">
+  <conditionalFormatting sqref="B5:E20">
     <cfRule type="expression" dxfId="2" priority="2">
       <formula>$A5=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B20:F35">
-    <cfRule type="expression" dxfId="1" priority="18">
-      <formula>$A20=1</formula>
+  <conditionalFormatting sqref="B21:F36">
+    <cfRule type="expression" dxfId="1" priority="19">
+      <formula>$A21=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G17">
-    <cfRule type="dataBar" priority="15">
+  <conditionalFormatting sqref="G4:G18">
+    <cfRule type="dataBar" priority="16">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4298,8 +4325,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G18:G35">
-    <cfRule type="dataBar" priority="19">
+  <conditionalFormatting sqref="G19:G36">
+    <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4340,7 +4367,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G17</xm:sqref>
+          <xm:sqref>G4:G18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{272DF8F1-2D7A-C948-BB97-5E4DFA143735}">
@@ -4355,7 +4382,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G18:G35</xm:sqref>
+          <xm:sqref>G19:G36</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4398,15 +4425,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -4424,6 +4442,15 @@
     <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4727,14 +4754,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4742,6 +4761,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
     <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
randomAIWaitTime() : Created a fun game feature to Just to bit of fun to add atmosphere to the AI. It adds a user-adjustable random 'thining...' effect whilst the computer player is taking it's turn.
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFAE1E7-8177-E846-B909-35EA7EF2FE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3DB84B-7587-C443-A8E6-1429CE2559DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="102">
   <si>
     <t>DATE</t>
   </si>
@@ -454,6 +454,16 @@
   </si>
   <si>
     <t>String theory</t>
+  </si>
+  <si>
+    <t>Final push now, with just over 17 hour to go. Pedal to the metal.
+Working to get as much doe as possible, AI, game moves, scoiring (which I haven't even looked at yet). And of course, testing. But I hope my intense work on validation would make testing for edge cases easier and less to fix.</t>
+  </si>
+  <si>
+    <t>General clearing up of classes.</t>
+  </si>
+  <si>
+    <t>Minor updates to all classes</t>
   </si>
 </sst>
 </file>
@@ -3049,7 +3059,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>3521028</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4772071" cy="2667000"/>
@@ -3105,13 +3115,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>4241800</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>403225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8229600</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>3394075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3149,13 +3159,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>5448300</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8242300</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>2133600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3193,13 +3203,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>241376</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>1155700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1511300</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3237,13 +3247,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>5664200</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>215900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8204200</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>2603500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3547,10 +3557,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3617,460 +3627,461 @@
         <v>45372</v>
       </c>
       <c r="C4" s="12">
-        <v>0.61944444444444446</v>
+        <v>0.87083333333333335</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>54</v>
+        <v>101</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G4" s="18">
-        <v>0.88500000000000001</v>
+        <v>0.89</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="201" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="169" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="9">
         <v>45372</v>
       </c>
       <c r="C5" s="12">
-        <v>0.60972222222222228</v>
+        <v>0.61944444444444446</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G5" s="18">
-        <v>0.88</v>
+        <v>0.88500000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="201" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
         <v>45372</v>
       </c>
       <c r="C6" s="12">
-        <v>0.28472222222222221</v>
+        <v>0.60972222222222228</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>92</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G6" s="18">
-        <v>0.87</v>
+        <v>0.88</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="240" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" s="2" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="9">
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="C7" s="12">
-        <v>0.94305555555555554</v>
+        <v>0.28472222222222221</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G7" s="18">
-        <v>0.86</v>
+        <v>0.87</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" s="2" customFormat="1" ht="240" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="9">
         <v>45371</v>
       </c>
       <c r="C8" s="12">
-        <v>0.51180555555555551</v>
+        <v>0.94305555555555554</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>87</v>
+        <v>89</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>90</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="G8" s="18">
-        <v>0.82</v>
+        <v>0.86</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" ht="320" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" s="2" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="9">
         <v>45371</v>
       </c>
       <c r="C9" s="12">
-        <v>0.18055555555555555</v>
+        <v>0.51180555555555551</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G9" s="18">
-        <v>0.81399999999999995</v>
+        <v>0.82</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" s="2" customFormat="1" ht="320" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="9">
         <v>45371</v>
       </c>
       <c r="C10" s="12">
-        <v>9.7222222222222224E-3</v>
+        <v>0.18055555555555555</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="E10" s="22" t="s">
-        <v>82</v>
+      <c r="E10" s="23" t="s">
+        <v>85</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="G10" s="13">
-        <v>0.81</v>
+        <v>84</v>
+      </c>
+      <c r="G10" s="18">
+        <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" s="2" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="9">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="C11" s="12">
-        <v>0.67708333333333337</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>78</v>
+        <v>83</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>82</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G11" s="13">
-        <v>0.8</v>
+        <v>0.81</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" s="2" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="9">
         <v>45370</v>
       </c>
       <c r="C12" s="12">
-        <v>0.53055555555555556</v>
+        <v>0.67708333333333337</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G12" s="13">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" s="2" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="9">
         <v>45370</v>
       </c>
       <c r="C13" s="12">
-        <v>0.10138888888888889</v>
+        <v>0.53055555555555556</v>
       </c>
       <c r="D13" s="21" t="s">
         <v>73</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G13" s="13">
-        <v>0.75</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="9">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="C14" s="12">
-        <v>0.79652777777777772</v>
+        <v>0.10138888888888889</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G14" s="13">
-        <v>0.74</v>
+        <v>0.75</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="9">
         <v>45369</v>
       </c>
       <c r="C15" s="12">
-        <v>0.72430555555555554</v>
+        <v>0.79652777777777772</v>
       </c>
       <c r="D15" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G15" s="13">
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="9">
         <v>45369</v>
       </c>
       <c r="C16" s="12">
-        <v>0.55277777777777781</v>
+        <v>0.72430555555555554</v>
       </c>
       <c r="D16" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G16" s="13">
-        <v>0.71</v>
+        <v>0.73</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="9">
         <v>45369</v>
       </c>
       <c r="C17" s="12">
-        <v>0.22291666666666668</v>
+        <v>0.55277777777777781</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E17" s="20" t="s">
         <v>66</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G17" s="13">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
       <c r="B18" s="9">
         <v>45369</v>
       </c>
       <c r="C18" s="12">
-        <v>5.8333333333333334E-2</v>
+        <v>0.22291666666666668</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G18" s="13">
-        <v>0.69</v>
+        <v>0.7</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
       <c r="B19" s="9">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="C19" s="12">
-        <v>0.96458333333333335</v>
+        <v>5.8333333333333334E-2</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="G19" s="18">
-        <v>0.68500000000000005</v>
+        <v>61</v>
+      </c>
+      <c r="G19" s="13">
+        <v>0.69</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
       <c r="B20" s="9">
         <v>45368</v>
       </c>
       <c r="C20" s="12">
-        <v>0.79374999999999996</v>
+        <v>0.96458333333333335</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G20" s="13">
-        <v>0.67</v>
+        <v>58</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" s="18">
+        <v>0.68500000000000005</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
       <c r="B21" s="9">
         <v>45368</v>
       </c>
       <c r="C21" s="12">
-        <v>0.44027777777777777</v>
+        <v>0.79374999999999996</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="G21" s="13">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
       <c r="B22" s="9">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="C22" s="12">
-        <v>7.0833333333333331E-2</v>
+        <v>0.44027777777777777</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G22" s="13">
-        <v>0.64</v>
-      </c>
-      <c r="I22" s="15"/>
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="23" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
       <c r="B23" s="9">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="C23" s="12">
-        <v>0.98611111111111116</v>
+        <v>7.0833333333333331E-2</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G23" s="13">
-        <v>0.63</v>
-      </c>
+        <v>0.64</v>
+      </c>
+      <c r="I23" s="15"/>
     </row>
     <row r="24" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
       <c r="B24" s="9">
+        <v>45366</v>
+      </c>
+      <c r="C24" s="12">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G24" s="13">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="1"/>
+      <c r="B25" s="9">
         <v>45365</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C25" s="12">
         <v>2.1527777777777778E-2</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D25" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="20" t="s">
+      <c r="E25" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F25" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G25" s="13">
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="9">
-        <v>45364</v>
-      </c>
-      <c r="C25" s="12">
-        <v>0.35138888888888886</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G25" s="13">
-        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4078,59 +4089,59 @@
         <v>45364</v>
       </c>
       <c r="C26" s="12">
-        <v>0.22708333333333333</v>
+        <v>0.35138888888888886</v>
       </c>
       <c r="D26" s="21" t="s">
         <v>37</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G26" s="13">
-        <v>0.56000000000000005</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="9">
-        <v>45363</v>
+        <v>45364</v>
       </c>
       <c r="C27" s="12">
-        <v>0.56666666666666665</v>
+        <v>0.22708333333333333</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G27" s="13">
-        <v>0.54</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="9">
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="C28" s="12">
-        <v>0.95208333333333328</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G28" s="13">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4138,19 +4149,19 @@
         <v>45361</v>
       </c>
       <c r="C29" s="12">
-        <v>0.84236111111111112</v>
+        <v>0.95208333333333328</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G29" s="13">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4158,19 +4169,19 @@
         <v>45361</v>
       </c>
       <c r="C30" s="12">
-        <v>0.58819444444444446</v>
+        <v>0.84236111111111112</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="G30" s="13">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4178,19 +4189,19 @@
         <v>45361</v>
       </c>
       <c r="C31" s="12">
-        <v>0.15625</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G31" s="13">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4198,39 +4209,39 @@
         <v>45361</v>
       </c>
       <c r="C32" s="12">
-        <v>9.7222222222222224E-3</v>
+        <v>0.15625</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E32" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="G32" s="13">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="9">
-        <v>45360</v>
+        <v>45361</v>
       </c>
       <c r="C33" s="12">
-        <v>0.27291666666666664</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="G33" s="13">
-        <v>0.37</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4238,81 +4249,101 @@
         <v>45360</v>
       </c>
       <c r="C34" s="12">
-        <v>0.21458333333333332</v>
+        <v>0.27291666666666664</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G34" s="13">
-        <v>0.34</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B35" s="9">
-        <v>45359</v>
-      </c>
-      <c r="C35" s="10">
-        <v>20.32</v>
+        <v>45360</v>
+      </c>
+      <c r="C35" s="12">
+        <v>0.21458333333333332</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G35" s="13">
-        <v>0.32</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="9">
+        <v>45359</v>
+      </c>
+      <c r="C36" s="10">
+        <v>20.32</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="13">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B37" s="9">
         <v>45357</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C37" s="10">
         <v>13.26</v>
       </c>
-      <c r="D36" s="21" t="s">
+      <c r="D37" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E36" s="21" t="s">
+      <c r="E37" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F36" s="11" t="s">
+      <c r="F37" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G36" s="13">
+      <c r="G37" s="13">
         <v>0.22</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="38" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="39" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B5:E20">
+  <conditionalFormatting sqref="B5:E21">
     <cfRule type="expression" dxfId="2" priority="2">
       <formula>$A5=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B21:F36">
-    <cfRule type="expression" dxfId="1" priority="19">
-      <formula>$A21=1</formula>
+  <conditionalFormatting sqref="B22:F37">
+    <cfRule type="expression" dxfId="1" priority="20">
+      <formula>$A22=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G18">
-    <cfRule type="dataBar" priority="16">
+  <conditionalFormatting sqref="G4:G19">
+    <cfRule type="dataBar" priority="17">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4325,8 +4356,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G19:G36">
-    <cfRule type="dataBar" priority="20">
+  <conditionalFormatting sqref="G20:G37">
+    <cfRule type="dataBar" priority="21">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4367,7 +4398,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G18</xm:sqref>
+          <xm:sqref>G4:G19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{272DF8F1-2D7A-C948-BB97-5E4DFA143735}">
@@ -4382,7 +4413,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G19:G36</xm:sqref>
+          <xm:sqref>G20:G37</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4425,6 +4456,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -4442,15 +4482,6 @@
     <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4754,6 +4785,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4761,14 +4800,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
     <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
GamePlay() / ComputerPlayer() / BoardUnit() - Revisited a lot of old 'legacy' code unused methods. reset and started some classes afrtesh - with my newer found knowledge.
</commit_message>
<xml_diff>
--- a/Ancillary Docs/Development Log.xlsx
+++ b/Ancillary Docs/Development Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3DB84B-7587-C443-A8E6-1429CE2559DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE15B75-6536-794D-A77B-AB11D245E8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="105">
   <si>
     <t>DATE</t>
   </si>
@@ -464,6 +464,16 @@
   </si>
   <si>
     <t>Minor updates to all classes</t>
+  </si>
+  <si>
+    <t>Step By Step</t>
+  </si>
+  <si>
+    <t>Lots of minor bug fixes, resetting and starting classes afresh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Had a LOT of restarts. Through chunks of code away (especially spome idea I had about the AI. My codebase was really starting to get messy and convaluted, so spend enourmous time taking it back to basics. Step by step, seeing what works and incrementally improving.
+Only a few hours to go now. </t>
   </si>
 </sst>
 </file>
@@ -3059,7 +3069,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>3521028</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4772071" cy="2667000"/>
@@ -3115,13 +3125,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>4241800</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>403225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8229600</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>3394075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3159,13 +3169,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>5448300</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8242300</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>2133600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3203,13 +3213,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>241376</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>1155700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1511300</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3247,13 +3257,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>5664200</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>215900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8204200</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>2603500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3557,10 +3567,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3585,7 +3595,7 @@
       <c r="E1" s="25"/>
       <c r="F1" s="29" t="str">
         <f ca="1">'Target '!A2-'Target '!A1&amp;" days remaining"</f>
-        <v>-1 days remaining</v>
+        <v>0 days remaining</v>
       </c>
       <c r="G1" s="30"/>
     </row>
@@ -3621,25 +3631,25 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="169" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" s="2" customFormat="1" ht="217" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9">
         <v>45372</v>
       </c>
       <c r="C4" s="12">
-        <v>0.87083333333333335</v>
+        <v>0.24097222222222223</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="G4" s="18">
-        <v>0.89</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="2" customFormat="1" ht="169" customHeight="1" x14ac:dyDescent="0.15">
@@ -3648,460 +3658,461 @@
         <v>45372</v>
       </c>
       <c r="C5" s="12">
-        <v>0.61944444444444446</v>
+        <v>0.87083333333333335</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>54</v>
+        <v>101</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G5" s="18">
-        <v>0.88500000000000001</v>
+        <v>0.89</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" ht="201" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="169" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="9">
         <v>45372</v>
       </c>
       <c r="C6" s="12">
-        <v>0.60972222222222228</v>
+        <v>0.61944444444444446</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G6" s="18">
-        <v>0.88</v>
+        <v>0.88500000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" s="2" customFormat="1" ht="201" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="9">
         <v>45372</v>
       </c>
       <c r="C7" s="12">
-        <v>0.28472222222222221</v>
+        <v>0.60972222222222228</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>92</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G7" s="18">
-        <v>0.87</v>
+        <v>0.88</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" ht="240" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" s="2" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="9">
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="C8" s="12">
-        <v>0.94305555555555554</v>
+        <v>0.28472222222222221</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G8" s="18">
-        <v>0.86</v>
+        <v>0.87</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" s="2" customFormat="1" ht="240" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="9">
         <v>45371</v>
       </c>
       <c r="C9" s="12">
-        <v>0.51180555555555551</v>
+        <v>0.94305555555555554</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>87</v>
+        <v>89</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>90</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="G9" s="18">
-        <v>0.82</v>
+        <v>0.86</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" ht="320" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" s="2" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="9">
         <v>45371</v>
       </c>
       <c r="C10" s="12">
-        <v>0.18055555555555555</v>
+        <v>0.51180555555555551</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G10" s="18">
-        <v>0.81399999999999995</v>
+        <v>0.82</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" s="2" customFormat="1" ht="320" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="9">
         <v>45371</v>
       </c>
       <c r="C11" s="12">
-        <v>9.7222222222222224E-3</v>
+        <v>0.18055555555555555</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="E11" s="22" t="s">
-        <v>82</v>
+      <c r="E11" s="23" t="s">
+        <v>85</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="G11" s="13">
-        <v>0.81</v>
+        <v>84</v>
+      </c>
+      <c r="G11" s="18">
+        <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" s="2" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="9">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="C12" s="12">
-        <v>0.67708333333333337</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>78</v>
+        <v>83</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>82</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G12" s="13">
-        <v>0.8</v>
+        <v>0.81</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="2" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" s="2" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="9">
         <v>45370</v>
       </c>
       <c r="C13" s="12">
-        <v>0.53055555555555556</v>
+        <v>0.67708333333333337</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G13" s="13">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="2" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="9">
         <v>45370</v>
       </c>
       <c r="C14" s="12">
-        <v>0.10138888888888889</v>
+        <v>0.53055555555555556</v>
       </c>
       <c r="D14" s="21" t="s">
         <v>73</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G14" s="13">
-        <v>0.75</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="9">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="C15" s="12">
-        <v>0.79652777777777772</v>
+        <v>0.10138888888888889</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G15" s="13">
-        <v>0.74</v>
+        <v>0.75</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" s="2" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="9">
         <v>45369</v>
       </c>
       <c r="C16" s="12">
-        <v>0.72430555555555554</v>
+        <v>0.79652777777777772</v>
       </c>
       <c r="D16" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G16" s="13">
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" s="2" customFormat="1" ht="182" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="9">
         <v>45369</v>
       </c>
       <c r="C17" s="12">
-        <v>0.55277777777777781</v>
+        <v>0.72430555555555554</v>
       </c>
       <c r="D17" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G17" s="13">
-        <v>0.71</v>
+        <v>0.73</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" s="2" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
       <c r="B18" s="9">
         <v>45369</v>
       </c>
       <c r="C18" s="12">
-        <v>0.22291666666666668</v>
+        <v>0.55277777777777781</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E18" s="20" t="s">
         <v>66</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G18" s="13">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" s="2" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
       <c r="B19" s="9">
         <v>45369</v>
       </c>
       <c r="C19" s="12">
-        <v>5.8333333333333334E-2</v>
+        <v>0.22291666666666668</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G19" s="13">
-        <v>0.69</v>
+        <v>0.7</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
       <c r="B20" s="9">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="C20" s="12">
-        <v>0.96458333333333335</v>
+        <v>5.8333333333333334E-2</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="G20" s="18">
-        <v>0.68500000000000005</v>
+        <v>61</v>
+      </c>
+      <c r="G20" s="13">
+        <v>0.69</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" s="2" customFormat="1" ht="266" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
       <c r="B21" s="9">
         <v>45368</v>
       </c>
       <c r="C21" s="12">
-        <v>0.79374999999999996</v>
+        <v>0.96458333333333335</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G21" s="13">
-        <v>0.67</v>
+        <v>58</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="18">
+        <v>0.68500000000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" s="2" customFormat="1" ht="351" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
       <c r="B22" s="9">
         <v>45368</v>
       </c>
       <c r="C22" s="12">
-        <v>0.44027777777777777</v>
+        <v>0.79374999999999996</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="G22" s="13">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" s="2" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
       <c r="B23" s="9">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="C23" s="12">
-        <v>7.0833333333333331E-2</v>
+        <v>0.44027777777777777</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G23" s="13">
-        <v>0.64</v>
-      </c>
-      <c r="I23" s="15"/>
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="24" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" s="2" customFormat="1" ht="298" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
       <c r="B24" s="9">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="C24" s="12">
-        <v>0.98611111111111116</v>
+        <v>7.0833333333333331E-2</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G24" s="13">
-        <v>0.63</v>
-      </c>
+        <v>0.64</v>
+      </c>
+      <c r="I24" s="15"/>
     </row>
     <row r="25" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1"/>
       <c r="B25" s="9">
+        <v>45366</v>
+      </c>
+      <c r="C25" s="12">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25" s="13">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="2" customFormat="1" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="1"/>
+      <c r="B26" s="9">
         <v>45365</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C26" s="12">
         <v>2.1527777777777778E-2</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="D26" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="20" t="s">
+      <c r="E26" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="F26" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G25" s="13">
+      <c r="G26" s="13">
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="9">
-        <v>45364</v>
-      </c>
-      <c r="C26" s="12">
-        <v>0.35138888888888886</v>
-      </c>
-      <c r="D26" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G26" s="13">
-        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4109,59 +4120,59 @@
         <v>45364</v>
       </c>
       <c r="C27" s="12">
-        <v>0.22708333333333333</v>
+        <v>0.35138888888888886</v>
       </c>
       <c r="D27" s="21" t="s">
         <v>37</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G27" s="13">
-        <v>0.56000000000000005</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="9">
-        <v>45363</v>
+        <v>45364</v>
       </c>
       <c r="C28" s="12">
-        <v>0.56666666666666665</v>
+        <v>0.22708333333333333</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G28" s="13">
-        <v>0.54</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="9">
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="C29" s="12">
-        <v>0.95208333333333328</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G29" s="13">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4169,19 +4180,19 @@
         <v>45361</v>
       </c>
       <c r="C30" s="12">
-        <v>0.84236111111111112</v>
+        <v>0.95208333333333328</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G30" s="13">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4189,19 +4200,19 @@
         <v>45361</v>
       </c>
       <c r="C31" s="12">
-        <v>0.58819444444444446</v>
+        <v>0.84236111111111112</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="G31" s="13">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4209,19 +4220,19 @@
         <v>45361</v>
       </c>
       <c r="C32" s="12">
-        <v>0.15625</v>
+        <v>0.58819444444444446</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G32" s="13">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4229,39 +4240,39 @@
         <v>45361</v>
       </c>
       <c r="C33" s="12">
-        <v>9.7222222222222224E-3</v>
+        <v>0.15625</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E33" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="G33" s="13">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="9">
-        <v>45360</v>
+        <v>45361</v>
       </c>
       <c r="C34" s="12">
-        <v>0.27291666666666664</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="G34" s="13">
-        <v>0.37</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
@@ -4269,81 +4280,101 @@
         <v>45360</v>
       </c>
       <c r="C35" s="12">
-        <v>0.21458333333333332</v>
+        <v>0.27291666666666664</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G35" s="13">
-        <v>0.34</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="9">
-        <v>45359</v>
-      </c>
-      <c r="C36" s="10">
-        <v>20.32</v>
+        <v>45360</v>
+      </c>
+      <c r="C36" s="12">
+        <v>0.21458333333333332</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G36" s="13">
-        <v>0.32</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="37" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="9">
+        <v>45359</v>
+      </c>
+      <c r="C37" s="10">
+        <v>20.32</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" s="13">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B38" s="9">
         <v>45357</v>
       </c>
-      <c r="C37" s="10">
+      <c r="C38" s="10">
         <v>13.26</v>
       </c>
-      <c r="D37" s="21" t="s">
+      <c r="D38" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E37" s="21" t="s">
+      <c r="E38" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F37" s="11" t="s">
+      <c r="F38" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G37" s="13">
+      <c r="G38" s="13">
         <v>0.22</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="39" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="40" spans="2:7" ht="286" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B5:E21">
+  <conditionalFormatting sqref="B5:E22">
     <cfRule type="expression" dxfId="2" priority="2">
       <formula>$A5=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B22:F37">
-    <cfRule type="expression" dxfId="1" priority="20">
-      <formula>$A22=1</formula>
+  <conditionalFormatting sqref="B23:F38">
+    <cfRule type="expression" dxfId="1" priority="21">
+      <formula>$A23=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G19">
-    <cfRule type="dataBar" priority="17">
+  <conditionalFormatting sqref="G4:G20">
+    <cfRule type="dataBar" priority="18">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4356,8 +4387,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G20:G37">
-    <cfRule type="dataBar" priority="21">
+  <conditionalFormatting sqref="G21:G38">
+    <cfRule type="dataBar" priority="22">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4398,7 +4429,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G4:G19</xm:sqref>
+          <xm:sqref>G4:G20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{272DF8F1-2D7A-C948-BB97-5E4DFA143735}">
@@ -4413,7 +4444,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G20:G37</xm:sqref>
+          <xm:sqref>G21:G38</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4444,7 +4475,7 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45372</v>
+        <v>45373</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
@@ -4456,15 +4487,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -4482,6 +4504,15 @@
     <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4785,14 +4816,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5F743-71A0-4D81-8907-E9763C3648A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4800,6 +4823,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
     <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34EAA5D-D096-4A21-8AE3-15AA4CD3805A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>